<commit_message>
Add support for paths
</commit_message>
<xml_diff>
--- a/XForms/highways.xlsx
+++ b/XForms/highways.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="303">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -216,6 +216,36 @@
     <t xml:space="preserve">(in meters)</t>
   </si>
   <si>
+    <t xml:space="preserve">sac</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Path conditions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${feature_type} = 'path'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select_one sac_scale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sac_scale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What is the difficulty of this path ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hiking</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select_one trail_visibility</t>
+  </si>
+  <si>
+    <t xml:space="preserve">visibility</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How difficult is it to follow the path ?</t>
+  </si>
+  <si>
     <t xml:space="preserve">bridge</t>
   </si>
   <si>
@@ -300,6 +330,9 @@
     <t xml:space="preserve">GPS Coordinates</t>
   </si>
   <si>
+    <t xml:space="preserve">${feature_type} = 'highway' or ${feature_type} = 'path'</t>
+  </si>
+  <si>
     <t xml:space="preserve">select_one gps_type</t>
   </si>
   <si>
@@ -369,6 +402,12 @@
     <t xml:space="preserve">list_name</t>
   </si>
   <si>
+    <t xml:space="preserve">path</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Path (foot traffic only)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Bridge</t>
   </si>
   <si>
@@ -414,12 +453,6 @@
     <t xml:space="preserve">Service (driveways, access roads)</t>
   </si>
   <si>
-    <t xml:space="preserve">path</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Path (foot traffic only)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Track (jeep trail)</t>
   </si>
   <si>
@@ -832,6 +865,63 @@
   </si>
   <si>
     <t xml:space="preserve">Swing Gate (single or double)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hiking (Can be hiked in ordinary sports shoes/trainers, no risk of falling)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mountain_hiking</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mountain Hking (terrain is steep in places and may have fall hazards)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">demanding_mountain_hiking</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Demanding Mountain Hiking (Portions of the route exposed with danger of falling. Trail may have unmarked portions and cross fields of loose scree or talus)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">alpine_hiking</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alpine Hiking (terrain quite exposed. Trail may include steep grassy pitches, talus slopes, easy snowfields, or snow-free glacier crossings )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">demanding_alpine_hiking</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Demanding Alpine Hiking (exposed and demanding terrain. May include steep rock scrambles, glaciers and snowfields with risk of sliding.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">difficult_alpine_hiking</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Difficult Alpine Hiking (severe exposure, difficult craggy terain, includes climbing pitches up to UIAA grade II.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">trail_visibility</t>
+  </si>
+  <si>
+    <t xml:space="preserve">excellent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Excellent (Unambiguous path or markers everywhere)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Good (Next marker always visible, but sometimes has to be searched for. Basic sense of direction recommended)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Intermediate (track mostly visible, Good sense of direction, map required)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bad (path sometimes invisible, route partly pathless, orienting skills recommended)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Horrible (often pathless, advanced orientational skills recommended)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No (mostly pathless, excellent orientational skills recommended)</t>
   </si>
   <si>
     <t xml:space="preserve">form_id</t>
@@ -852,7 +942,7 @@
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\Thh:mm:ss"/>
     <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="15">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -916,6 +1006,13 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
     </font>
@@ -967,6 +1064,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FFE6FF00"/>
       </patternFill>
@@ -979,20 +1088,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFE6FF00"/>
         <bgColor rgb="FFFFFF00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
   </fills>
@@ -1030,7 +1127,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="65">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1099,10 +1196,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1115,27 +1208,99 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1143,111 +1308,59 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1255,8 +1368,12 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -1267,7 +1384,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1348,10 +1465,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AB54"/>
+  <dimension ref="A1:AB60"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I8" activeCellId="0" sqref="I8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F33" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G47" activeCellId="0" sqref="G47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1847,794 +1964,879 @@
       <c r="H27" s="14"/>
       <c r="I27" s="14"/>
     </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="9"/>
-      <c r="B28" s="9"/>
-      <c r="C28" s="9"/>
-      <c r="D28" s="9"/>
-      <c r="E28" s="10"/>
-      <c r="F28" s="10"/>
-      <c r="G28" s="9"/>
-      <c r="H28" s="9"/>
-      <c r="I28" s="9"/>
-    </row>
-    <row r="29" s="20" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="17" t="s">
+    <row r="28" s="19" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="17"/>
+      <c r="B28" s="17"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="17"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="17"/>
+      <c r="H28" s="17"/>
+      <c r="I28" s="17"/>
+    </row>
+    <row r="29" s="22" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B29" s="18" t="s">
+      <c r="B29" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="C29" s="18" t="s">
+      <c r="C29" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="D29" s="18"/>
-      <c r="E29" s="19"/>
-      <c r="F29" s="19"/>
-      <c r="G29" s="18" t="s">
+      <c r="D29" s="20"/>
+      <c r="E29" s="21"/>
+      <c r="F29" s="21"/>
+      <c r="G29" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="H29" s="18"/>
-      <c r="I29" s="18" t="s">
+      <c r="H29" s="20"/>
+      <c r="I29" s="20"/>
+    </row>
+    <row r="30" s="22" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="B30" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="C30" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="D30" s="20"/>
+      <c r="E30" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="F30" s="21"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31" s="22" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="B31" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="C31" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="D31" s="20"/>
+      <c r="E31" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="F31" s="21"/>
+      <c r="G31" s="20"/>
+      <c r="H31" s="20"/>
+      <c r="I31" s="20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="32" s="22" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="B32" s="20"/>
+      <c r="C32" s="20"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="21"/>
+      <c r="F32" s="21"/>
+      <c r="G32" s="20"/>
+      <c r="H32" s="20"/>
+      <c r="I32" s="20"/>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="9"/>
+      <c r="B33" s="9"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="10"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="9"/>
+      <c r="H33" s="9"/>
+      <c r="I33" s="9"/>
+    </row>
+    <row r="34" s="26" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="B34" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="C34" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="D34" s="24"/>
+      <c r="E34" s="25"/>
+      <c r="F34" s="25"/>
+      <c r="G34" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="H34" s="24"/>
+      <c r="I34" s="24" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="30" s="20" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="B30" s="21" t="s">
-        <v>68</v>
-      </c>
-      <c r="C30" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="D30" s="17"/>
-      <c r="E30" s="22" t="s">
+    <row r="35" s="26" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A35" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="B35" s="27" t="s">
+        <v>78</v>
+      </c>
+      <c r="C35" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="D35" s="23"/>
+      <c r="E35" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="F30" s="22" t="n">
+      <c r="F35" s="28" t="n">
         <v>1</v>
       </c>
-      <c r="G30" s="18"/>
-      <c r="I30" s="17" t="s">
+      <c r="G35" s="24"/>
+      <c r="I35" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="J30" s="23"/>
-      <c r="K30" s="23"/>
-      <c r="L30" s="23"/>
-      <c r="M30" s="23"/>
-      <c r="N30" s="23"/>
-      <c r="O30" s="23"/>
-      <c r="P30" s="23"/>
-      <c r="Q30" s="24"/>
-      <c r="R30" s="24"/>
-      <c r="S30" s="24"/>
-      <c r="T30" s="24"/>
-      <c r="U30" s="24"/>
-      <c r="V30" s="24"/>
-      <c r="W30" s="24"/>
-      <c r="X30" s="24"/>
-      <c r="Y30" s="24"/>
-      <c r="Z30" s="24"/>
-      <c r="AA30" s="24"/>
-      <c r="AB30" s="24"/>
-    </row>
-    <row r="31" s="20" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="17" t="s">
+      <c r="J35" s="29"/>
+      <c r="K35" s="29"/>
+      <c r="L35" s="29"/>
+      <c r="M35" s="29"/>
+      <c r="N35" s="29"/>
+      <c r="O35" s="29"/>
+      <c r="P35" s="29"/>
+      <c r="Q35" s="30"/>
+      <c r="R35" s="30"/>
+      <c r="S35" s="30"/>
+      <c r="T35" s="30"/>
+      <c r="U35" s="30"/>
+      <c r="V35" s="30"/>
+      <c r="W35" s="30"/>
+      <c r="X35" s="30"/>
+      <c r="Y35" s="30"/>
+      <c r="Z35" s="30"/>
+      <c r="AA35" s="30"/>
+      <c r="AB35" s="30"/>
+    </row>
+    <row r="36" s="26" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A36" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="B31" s="21" t="s">
-        <v>70</v>
-      </c>
-      <c r="C31" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="D31" s="17"/>
-      <c r="E31" s="22"/>
-      <c r="F31" s="22"/>
-      <c r="G31" s="18"/>
-      <c r="I31" s="17"/>
-      <c r="J31" s="23"/>
-      <c r="K31" s="23"/>
-      <c r="L31" s="23"/>
-      <c r="M31" s="23"/>
-      <c r="N31" s="23"/>
-      <c r="O31" s="23"/>
-      <c r="P31" s="23"/>
-      <c r="Q31" s="24"/>
-      <c r="R31" s="24"/>
-      <c r="S31" s="24"/>
-      <c r="T31" s="24"/>
-      <c r="U31" s="24"/>
-      <c r="V31" s="24"/>
-      <c r="W31" s="24"/>
-      <c r="X31" s="24"/>
-      <c r="Y31" s="24"/>
-      <c r="Z31" s="24"/>
-      <c r="AA31" s="24"/>
-      <c r="AB31" s="24"/>
-    </row>
-    <row r="32" s="20" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="B32" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="C32" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="D32" s="17"/>
-      <c r="E32" s="22"/>
-      <c r="F32" s="22"/>
-      <c r="I32" s="17" t="s">
-        <v>75</v>
-      </c>
-      <c r="J32" s="23"/>
-      <c r="K32" s="23"/>
-      <c r="L32" s="23"/>
-      <c r="M32" s="23"/>
-      <c r="N32" s="23"/>
-      <c r="O32" s="23"/>
-      <c r="P32" s="23"/>
-      <c r="Q32" s="24"/>
-      <c r="R32" s="24"/>
-      <c r="S32" s="24"/>
-      <c r="T32" s="24"/>
-      <c r="U32" s="24"/>
-      <c r="V32" s="24"/>
-      <c r="W32" s="24"/>
-      <c r="X32" s="24"/>
-      <c r="Y32" s="24"/>
-      <c r="Z32" s="24"/>
-      <c r="AA32" s="24"/>
-      <c r="AB32" s="24"/>
-    </row>
-    <row r="33" s="20" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="24" t="s">
+      <c r="B36" s="27" t="s">
+        <v>80</v>
+      </c>
+      <c r="C36" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="D36" s="23"/>
+      <c r="E36" s="28"/>
+      <c r="F36" s="28"/>
+      <c r="G36" s="24"/>
+      <c r="I36" s="23"/>
+      <c r="J36" s="29"/>
+      <c r="K36" s="29"/>
+      <c r="L36" s="29"/>
+      <c r="M36" s="29"/>
+      <c r="N36" s="29"/>
+      <c r="O36" s="29"/>
+      <c r="P36" s="29"/>
+      <c r="Q36" s="30"/>
+      <c r="R36" s="30"/>
+      <c r="S36" s="30"/>
+      <c r="T36" s="30"/>
+      <c r="U36" s="30"/>
+      <c r="V36" s="30"/>
+      <c r="W36" s="30"/>
+      <c r="X36" s="30"/>
+      <c r="Y36" s="30"/>
+      <c r="Z36" s="30"/>
+      <c r="AA36" s="30"/>
+      <c r="AB36" s="30"/>
+    </row>
+    <row r="37" s="26" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A37" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="B37" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="C37" s="27" t="s">
+        <v>84</v>
+      </c>
+      <c r="D37" s="23"/>
+      <c r="E37" s="28"/>
+      <c r="F37" s="28"/>
+      <c r="I37" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="J37" s="29"/>
+      <c r="K37" s="29"/>
+      <c r="L37" s="29"/>
+      <c r="M37" s="29"/>
+      <c r="N37" s="29"/>
+      <c r="O37" s="29"/>
+      <c r="P37" s="29"/>
+      <c r="Q37" s="30"/>
+      <c r="R37" s="30"/>
+      <c r="S37" s="30"/>
+      <c r="T37" s="30"/>
+      <c r="U37" s="30"/>
+      <c r="V37" s="30"/>
+      <c r="W37" s="30"/>
+      <c r="X37" s="30"/>
+      <c r="Y37" s="30"/>
+      <c r="Z37" s="30"/>
+      <c r="AA37" s="30"/>
+      <c r="AB37" s="30"/>
+    </row>
+    <row r="38" s="26" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A38" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="B33" s="21"/>
-      <c r="C33" s="21"/>
-      <c r="D33" s="17"/>
-      <c r="E33" s="22"/>
-      <c r="F33" s="22"/>
-      <c r="G33" s="18"/>
-      <c r="I33" s="17"/>
-      <c r="J33" s="23"/>
-      <c r="K33" s="23"/>
-      <c r="L33" s="23"/>
-      <c r="M33" s="23"/>
-      <c r="N33" s="23"/>
-      <c r="O33" s="23"/>
-      <c r="P33" s="23"/>
-      <c r="Q33" s="24"/>
-      <c r="R33" s="24"/>
-      <c r="S33" s="24"/>
-      <c r="T33" s="24"/>
-      <c r="U33" s="24"/>
-      <c r="V33" s="24"/>
-      <c r="W33" s="24"/>
-      <c r="X33" s="24"/>
-      <c r="Y33" s="24"/>
-      <c r="Z33" s="24"/>
-      <c r="AA33" s="24"/>
-      <c r="AB33" s="24"/>
-    </row>
-    <row r="35" s="29" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="25" t="s">
+      <c r="B38" s="27"/>
+      <c r="C38" s="27"/>
+      <c r="D38" s="23"/>
+      <c r="E38" s="28"/>
+      <c r="F38" s="28"/>
+      <c r="G38" s="24"/>
+      <c r="I38" s="23"/>
+      <c r="J38" s="29"/>
+      <c r="K38" s="29"/>
+      <c r="L38" s="29"/>
+      <c r="M38" s="29"/>
+      <c r="N38" s="29"/>
+      <c r="O38" s="29"/>
+      <c r="P38" s="29"/>
+      <c r="Q38" s="30"/>
+      <c r="R38" s="30"/>
+      <c r="S38" s="30"/>
+      <c r="T38" s="30"/>
+      <c r="U38" s="30"/>
+      <c r="V38" s="30"/>
+      <c r="W38" s="30"/>
+      <c r="X38" s="30"/>
+      <c r="Y38" s="30"/>
+      <c r="Z38" s="30"/>
+      <c r="AA38" s="30"/>
+      <c r="AB38" s="30"/>
+    </row>
+    <row r="40" s="35" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A40" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="B35" s="26" t="s">
-        <v>76</v>
-      </c>
-      <c r="C35" s="26" t="s">
-        <v>77</v>
-      </c>
-      <c r="D35" s="25"/>
-      <c r="E35" s="27"/>
-      <c r="F35" s="27"/>
-      <c r="G35" s="28" t="s">
-        <v>78</v>
-      </c>
-      <c r="I35" s="28" t="s">
+      <c r="B40" s="32" t="s">
+        <v>86</v>
+      </c>
+      <c r="C40" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="D40" s="31"/>
+      <c r="E40" s="33"/>
+      <c r="F40" s="33"/>
+      <c r="G40" s="34" t="s">
+        <v>88</v>
+      </c>
+      <c r="I40" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="J35" s="30"/>
-      <c r="K35" s="30"/>
-      <c r="L35" s="30"/>
-      <c r="M35" s="30"/>
-      <c r="N35" s="30"/>
-      <c r="O35" s="30"/>
-      <c r="P35" s="30"/>
-      <c r="Q35" s="31"/>
-      <c r="R35" s="31"/>
-      <c r="S35" s="31"/>
-      <c r="T35" s="31"/>
-      <c r="U35" s="31"/>
-      <c r="V35" s="31"/>
-      <c r="W35" s="31"/>
-      <c r="X35" s="31"/>
-      <c r="Y35" s="31"/>
-      <c r="Z35" s="31"/>
-      <c r="AA35" s="31"/>
-      <c r="AB35" s="31"/>
-    </row>
-    <row r="36" s="29" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="25" t="s">
-        <v>79</v>
-      </c>
-      <c r="B36" s="26" t="s">
-        <v>80</v>
-      </c>
-      <c r="C36" s="29" t="s">
-        <v>81</v>
-      </c>
-      <c r="D36" s="25"/>
-      <c r="E36" s="27" t="s">
+      <c r="J40" s="36"/>
+      <c r="K40" s="36"/>
+      <c r="L40" s="36"/>
+      <c r="M40" s="36"/>
+      <c r="N40" s="36"/>
+      <c r="O40" s="36"/>
+      <c r="P40" s="36"/>
+      <c r="Q40" s="37"/>
+      <c r="R40" s="37"/>
+      <c r="S40" s="37"/>
+      <c r="T40" s="37"/>
+      <c r="U40" s="37"/>
+      <c r="V40" s="37"/>
+      <c r="W40" s="37"/>
+      <c r="X40" s="37"/>
+      <c r="Y40" s="37"/>
+      <c r="Z40" s="37"/>
+      <c r="AA40" s="37"/>
+      <c r="AB40" s="37"/>
+    </row>
+    <row r="41" s="35" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A41" s="31" t="s">
+        <v>89</v>
+      </c>
+      <c r="B41" s="32" t="s">
+        <v>90</v>
+      </c>
+      <c r="C41" s="35" t="s">
+        <v>91</v>
+      </c>
+      <c r="D41" s="31"/>
+      <c r="E41" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="F36" s="27" t="n">
+      <c r="F41" s="33" t="n">
         <v>1</v>
       </c>
-      <c r="I36" s="25" t="s">
+      <c r="G41" s="34"/>
+      <c r="I41" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="J36" s="30"/>
-      <c r="K36" s="30"/>
-      <c r="L36" s="30"/>
-      <c r="M36" s="30"/>
-      <c r="N36" s="30"/>
-      <c r="O36" s="30"/>
-      <c r="P36" s="30"/>
-      <c r="Q36" s="31"/>
-      <c r="R36" s="31"/>
-      <c r="S36" s="31"/>
-      <c r="T36" s="31"/>
-      <c r="U36" s="31"/>
-      <c r="V36" s="31"/>
-      <c r="W36" s="31"/>
-      <c r="X36" s="31"/>
-      <c r="Y36" s="31"/>
-      <c r="Z36" s="31"/>
-      <c r="AA36" s="31"/>
-      <c r="AB36" s="31"/>
-    </row>
-    <row r="37" s="29" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="25" t="s">
+      <c r="J41" s="36"/>
+      <c r="K41" s="36"/>
+      <c r="L41" s="36"/>
+      <c r="M41" s="36"/>
+      <c r="N41" s="36"/>
+      <c r="O41" s="36"/>
+      <c r="P41" s="36"/>
+      <c r="Q41" s="37"/>
+      <c r="R41" s="37"/>
+      <c r="S41" s="37"/>
+      <c r="T41" s="37"/>
+      <c r="U41" s="37"/>
+      <c r="V41" s="37"/>
+      <c r="W41" s="37"/>
+      <c r="X41" s="37"/>
+      <c r="Y41" s="37"/>
+      <c r="Z41" s="37"/>
+      <c r="AA41" s="37"/>
+      <c r="AB41" s="37"/>
+    </row>
+    <row r="42" s="35" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A42" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="B37" s="26" t="s">
+      <c r="B42" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="C37" s="29" t="s">
+      <c r="C42" s="35" t="s">
+        <v>92</v>
+      </c>
+      <c r="D42" s="31"/>
+      <c r="E42" s="33"/>
+      <c r="F42" s="33"/>
+      <c r="G42" s="34"/>
+      <c r="I42" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="J42" s="36"/>
+      <c r="K42" s="36"/>
+      <c r="L42" s="36"/>
+      <c r="M42" s="36"/>
+      <c r="N42" s="36"/>
+      <c r="O42" s="36"/>
+      <c r="P42" s="36"/>
+      <c r="Q42" s="37"/>
+      <c r="R42" s="37"/>
+      <c r="S42" s="37"/>
+      <c r="T42" s="37"/>
+      <c r="U42" s="37"/>
+      <c r="V42" s="37"/>
+      <c r="W42" s="37"/>
+      <c r="X42" s="37"/>
+      <c r="Y42" s="37"/>
+      <c r="Z42" s="37"/>
+      <c r="AA42" s="37"/>
+      <c r="AB42" s="37"/>
+    </row>
+    <row r="43" s="35" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A43" s="31" t="s">
         <v>82</v>
       </c>
-      <c r="D37" s="25"/>
-      <c r="E37" s="27"/>
-      <c r="F37" s="27"/>
-      <c r="G37" s="28"/>
-      <c r="I37" s="25" t="s">
+      <c r="B43" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="C43" s="32" t="s">
+        <v>94</v>
+      </c>
+      <c r="D43" s="31"/>
+      <c r="E43" s="33"/>
+      <c r="F43" s="33"/>
+      <c r="I43" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="J43" s="36"/>
+      <c r="K43" s="36"/>
+      <c r="L43" s="36"/>
+      <c r="M43" s="36"/>
+      <c r="N43" s="36"/>
+      <c r="O43" s="36"/>
+      <c r="P43" s="36"/>
+      <c r="Q43" s="37"/>
+      <c r="R43" s="37"/>
+      <c r="S43" s="37"/>
+      <c r="T43" s="37"/>
+      <c r="U43" s="37"/>
+      <c r="V43" s="37"/>
+      <c r="W43" s="37"/>
+      <c r="X43" s="37"/>
+      <c r="Y43" s="37"/>
+      <c r="Z43" s="37"/>
+      <c r="AA43" s="37"/>
+      <c r="AB43" s="37"/>
+    </row>
+    <row r="44" s="35" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A44" s="31" t="s">
+        <v>95</v>
+      </c>
+      <c r="B44" s="32" t="s">
+        <v>96</v>
+      </c>
+      <c r="C44" s="32" t="s">
+        <v>97</v>
+      </c>
+      <c r="D44" s="31"/>
+      <c r="E44" s="33" t="s">
+        <v>98</v>
+      </c>
+      <c r="F44" s="33" t="n">
+        <v>0</v>
+      </c>
+      <c r="G44" s="34" t="s">
+        <v>99</v>
+      </c>
+      <c r="I44" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="J37" s="30"/>
-      <c r="K37" s="30"/>
-      <c r="L37" s="30"/>
-      <c r="M37" s="30"/>
-      <c r="N37" s="30"/>
-      <c r="O37" s="30"/>
-      <c r="P37" s="30"/>
-      <c r="Q37" s="31"/>
-      <c r="R37" s="31"/>
-      <c r="S37" s="31"/>
-      <c r="T37" s="31"/>
-      <c r="U37" s="31"/>
-      <c r="V37" s="31"/>
-      <c r="W37" s="31"/>
-      <c r="X37" s="31"/>
-      <c r="Y37" s="31"/>
-      <c r="Z37" s="31"/>
-      <c r="AA37" s="31"/>
-      <c r="AB37" s="31"/>
-    </row>
-    <row r="38" s="29" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="25" t="s">
-        <v>72</v>
-      </c>
-      <c r="B38" s="26" t="s">
-        <v>83</v>
-      </c>
-      <c r="C38" s="26" t="s">
-        <v>84</v>
-      </c>
-      <c r="D38" s="25"/>
-      <c r="E38" s="27"/>
-      <c r="F38" s="27"/>
-      <c r="I38" s="25" t="s">
-        <v>75</v>
-      </c>
-      <c r="J38" s="30"/>
-      <c r="K38" s="30"/>
-      <c r="L38" s="30"/>
-      <c r="M38" s="30"/>
-      <c r="N38" s="30"/>
-      <c r="O38" s="30"/>
-      <c r="P38" s="30"/>
-      <c r="Q38" s="31"/>
-      <c r="R38" s="31"/>
-      <c r="S38" s="31"/>
-      <c r="T38" s="31"/>
-      <c r="U38" s="31"/>
-      <c r="V38" s="31"/>
-      <c r="W38" s="31"/>
-      <c r="X38" s="31"/>
-      <c r="Y38" s="31"/>
-      <c r="Z38" s="31"/>
-      <c r="AA38" s="31"/>
-      <c r="AB38" s="31"/>
-    </row>
-    <row r="39" s="29" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="25" t="s">
+      <c r="J44" s="36"/>
+      <c r="K44" s="36"/>
+      <c r="L44" s="36"/>
+      <c r="M44" s="36"/>
+      <c r="N44" s="36"/>
+      <c r="O44" s="36"/>
+      <c r="P44" s="36"/>
+      <c r="Q44" s="37"/>
+      <c r="R44" s="37"/>
+      <c r="S44" s="37"/>
+      <c r="T44" s="37"/>
+      <c r="U44" s="37"/>
+      <c r="V44" s="37"/>
+      <c r="W44" s="37"/>
+      <c r="X44" s="37"/>
+      <c r="Y44" s="37"/>
+      <c r="Z44" s="37"/>
+      <c r="AA44" s="37"/>
+      <c r="AB44" s="37"/>
+    </row>
+    <row r="45" s="35" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A45" s="37" t="s">
+        <v>34</v>
+      </c>
+      <c r="B45" s="32"/>
+      <c r="C45" s="32"/>
+      <c r="D45" s="31"/>
+      <c r="E45" s="31"/>
+      <c r="F45" s="31"/>
+      <c r="G45" s="31"/>
+      <c r="I45" s="31"/>
+      <c r="J45" s="36"/>
+      <c r="K45" s="36"/>
+      <c r="L45" s="36"/>
+      <c r="M45" s="36"/>
+      <c r="N45" s="36"/>
+      <c r="O45" s="36"/>
+      <c r="P45" s="36"/>
+      <c r="Q45" s="37"/>
+      <c r="R45" s="37"/>
+      <c r="S45" s="37"/>
+      <c r="T45" s="37"/>
+      <c r="U45" s="37"/>
+      <c r="V45" s="37"/>
+      <c r="W45" s="37"/>
+      <c r="X45" s="37"/>
+      <c r="Y45" s="37"/>
+      <c r="Z45" s="37"/>
+      <c r="AA45" s="37"/>
+      <c r="AB45" s="37"/>
+    </row>
+    <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B46" s="38"/>
+      <c r="C46" s="38"/>
+      <c r="G46" s="9"/>
+      <c r="J46" s="39"/>
+      <c r="K46" s="39"/>
+      <c r="L46" s="39"/>
+      <c r="M46" s="39"/>
+      <c r="N46" s="39"/>
+      <c r="O46" s="39"/>
+      <c r="P46" s="39"/>
+      <c r="Q46" s="40"/>
+      <c r="R46" s="40"/>
+      <c r="S46" s="40"/>
+      <c r="T46" s="40"/>
+      <c r="U46" s="40"/>
+      <c r="V46" s="40"/>
+      <c r="W46" s="40"/>
+      <c r="X46" s="40"/>
+      <c r="Y46" s="40"/>
+      <c r="Z46" s="40"/>
+      <c r="AA46" s="40"/>
+      <c r="AB46" s="40"/>
+    </row>
+    <row r="47" s="41" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B47" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="C47" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="D47" s="20"/>
+      <c r="E47" s="21"/>
+      <c r="F47" s="21"/>
+      <c r="G47" s="20" t="s">
+        <v>102</v>
+      </c>
+      <c r="H47" s="20"/>
+      <c r="I47" s="20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="48" s="41" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="B48" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="C48" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="D48" s="20"/>
+      <c r="E48" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="F48" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="G48" s="20"/>
+      <c r="H48" s="20"/>
+      <c r="I48" s="20"/>
+    </row>
+    <row r="49" s="41" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A49" s="42" t="s">
+        <v>82</v>
+      </c>
+      <c r="B49" s="43" t="s">
+        <v>107</v>
+      </c>
+      <c r="C49" s="43" t="s">
+        <v>108</v>
+      </c>
+      <c r="D49" s="42" t="s">
+        <v>109</v>
+      </c>
+      <c r="E49" s="44"/>
+      <c r="F49" s="44"/>
+      <c r="G49" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="I49" s="42" t="s">
         <v>85</v>
       </c>
-      <c r="B39" s="26" t="s">
-        <v>86</v>
-      </c>
-      <c r="C39" s="26" t="s">
-        <v>87</v>
-      </c>
-      <c r="D39" s="25"/>
-      <c r="E39" s="27" t="s">
-        <v>88</v>
-      </c>
-      <c r="F39" s="27" t="n">
-        <v>0</v>
-      </c>
-      <c r="G39" s="28" t="s">
-        <v>89</v>
-      </c>
-      <c r="I39" s="25" t="s">
+      <c r="J49" s="45"/>
+      <c r="K49" s="45"/>
+      <c r="L49" s="45"/>
+      <c r="M49" s="45"/>
+      <c r="N49" s="45"/>
+      <c r="O49" s="45"/>
+      <c r="P49" s="45"/>
+      <c r="Q49" s="46"/>
+      <c r="R49" s="46"/>
+      <c r="S49" s="46"/>
+      <c r="T49" s="46"/>
+      <c r="U49" s="46"/>
+      <c r="V49" s="46"/>
+      <c r="W49" s="46"/>
+      <c r="X49" s="46"/>
+      <c r="Y49" s="46"/>
+      <c r="Z49" s="46"/>
+      <c r="AA49" s="46"/>
+      <c r="AB49" s="46"/>
+    </row>
+    <row r="50" s="41" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A50" s="42" t="s">
+        <v>111</v>
+      </c>
+      <c r="B50" s="43" t="s">
+        <v>112</v>
+      </c>
+      <c r="C50" s="43" t="s">
+        <v>113</v>
+      </c>
+      <c r="D50" s="42"/>
+      <c r="E50" s="44"/>
+      <c r="F50" s="44"/>
+      <c r="G50" s="20" t="s">
+        <v>114</v>
+      </c>
+      <c r="I50" s="42"/>
+      <c r="J50" s="45"/>
+      <c r="K50" s="45"/>
+      <c r="L50" s="45"/>
+      <c r="M50" s="45"/>
+      <c r="N50" s="45"/>
+      <c r="O50" s="45"/>
+      <c r="P50" s="45"/>
+      <c r="Q50" s="46"/>
+      <c r="R50" s="46"/>
+      <c r="S50" s="46"/>
+      <c r="T50" s="46"/>
+      <c r="U50" s="46"/>
+      <c r="V50" s="46"/>
+      <c r="W50" s="46"/>
+      <c r="X50" s="46"/>
+      <c r="Y50" s="46"/>
+      <c r="Z50" s="46"/>
+      <c r="AA50" s="46"/>
+      <c r="AB50" s="46"/>
+    </row>
+    <row r="51" s="41" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A51" s="46" t="s">
+        <v>34</v>
+      </c>
+      <c r="B51" s="43"/>
+      <c r="C51" s="43"/>
+      <c r="D51" s="42"/>
+      <c r="E51" s="44"/>
+      <c r="F51" s="44"/>
+      <c r="I51" s="42"/>
+      <c r="J51" s="45"/>
+      <c r="K51" s="45"/>
+      <c r="L51" s="45"/>
+      <c r="M51" s="45"/>
+      <c r="N51" s="45"/>
+      <c r="O51" s="45"/>
+      <c r="P51" s="45"/>
+      <c r="Q51" s="46"/>
+      <c r="R51" s="46"/>
+      <c r="S51" s="46"/>
+      <c r="T51" s="46"/>
+      <c r="U51" s="46"/>
+      <c r="V51" s="46"/>
+      <c r="W51" s="46"/>
+      <c r="X51" s="46"/>
+      <c r="Y51" s="46"/>
+      <c r="Z51" s="46"/>
+      <c r="AA51" s="46"/>
+      <c r="AB51" s="46"/>
+    </row>
+    <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B52" s="38"/>
+      <c r="C52" s="38"/>
+      <c r="J52" s="39"/>
+      <c r="K52" s="39"/>
+      <c r="L52" s="39"/>
+      <c r="M52" s="39"/>
+      <c r="N52" s="39"/>
+      <c r="O52" s="39"/>
+      <c r="P52" s="39"/>
+      <c r="Q52" s="40"/>
+      <c r="R52" s="40"/>
+      <c r="S52" s="40"/>
+      <c r="T52" s="40"/>
+      <c r="U52" s="40"/>
+      <c r="V52" s="40"/>
+      <c r="W52" s="40"/>
+      <c r="X52" s="40"/>
+      <c r="Y52" s="40"/>
+      <c r="Z52" s="40"/>
+      <c r="AA52" s="40"/>
+      <c r="AB52" s="40"/>
+    </row>
+    <row r="53" s="51" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A53" s="47" t="s">
+        <v>16</v>
+      </c>
+      <c r="B53" s="47" t="s">
+        <v>115</v>
+      </c>
+      <c r="C53" s="48" t="s">
+        <v>116</v>
+      </c>
+      <c r="D53" s="48"/>
+      <c r="E53" s="49"/>
+      <c r="F53" s="50"/>
+      <c r="G53" s="47"/>
+      <c r="H53" s="47"/>
+      <c r="I53" s="47" t="s">
+        <v>19</v>
+      </c>
+      <c r="J53" s="47"/>
+      <c r="K53" s="47"/>
+      <c r="L53" s="47"/>
+      <c r="M53" s="47"/>
+      <c r="N53" s="47"/>
+      <c r="O53" s="47"/>
+      <c r="P53" s="47"/>
+      <c r="Q53" s="47"/>
+      <c r="R53" s="47"/>
+      <c r="S53" s="47"/>
+      <c r="T53" s="47"/>
+      <c r="U53" s="47"/>
+      <c r="V53" s="47"/>
+      <c r="W53" s="47"/>
+      <c r="X53" s="47"/>
+      <c r="Y53" s="47"/>
+      <c r="Z53" s="47"/>
+      <c r="AA53" s="47"/>
+      <c r="AB53" s="47"/>
+    </row>
+    <row r="54" s="51" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A54" s="47" t="s">
+        <v>31</v>
+      </c>
+      <c r="B54" s="52" t="s">
+        <v>117</v>
+      </c>
+      <c r="C54" s="52" t="s">
+        <v>118</v>
+      </c>
+      <c r="D54" s="47"/>
+      <c r="E54" s="50"/>
+      <c r="F54" s="50"/>
+      <c r="G54" s="47"/>
+      <c r="H54" s="47"/>
+      <c r="I54" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="J39" s="30"/>
-      <c r="K39" s="30"/>
-      <c r="L39" s="30"/>
-      <c r="M39" s="30"/>
-      <c r="N39" s="30"/>
-      <c r="O39" s="30"/>
-      <c r="P39" s="30"/>
-      <c r="Q39" s="31"/>
-      <c r="R39" s="31"/>
-      <c r="S39" s="31"/>
-      <c r="T39" s="31"/>
-      <c r="U39" s="31"/>
-      <c r="V39" s="31"/>
-      <c r="W39" s="31"/>
-      <c r="X39" s="31"/>
-      <c r="Y39" s="31"/>
-      <c r="Z39" s="31"/>
-      <c r="AA39" s="31"/>
-      <c r="AB39" s="31"/>
-    </row>
-    <row r="40" s="29" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="31" t="s">
+      <c r="J54" s="47"/>
+      <c r="K54" s="47"/>
+      <c r="L54" s="47"/>
+      <c r="M54" s="47"/>
+      <c r="N54" s="47"/>
+      <c r="O54" s="47"/>
+      <c r="P54" s="47"/>
+      <c r="Q54" s="47"/>
+      <c r="R54" s="47"/>
+      <c r="S54" s="47"/>
+      <c r="T54" s="47"/>
+      <c r="U54" s="47"/>
+      <c r="V54" s="47"/>
+      <c r="W54" s="47"/>
+      <c r="X54" s="47"/>
+      <c r="Y54" s="47"/>
+      <c r="Z54" s="47"/>
+      <c r="AA54" s="47"/>
+      <c r="AB54" s="47"/>
+    </row>
+    <row r="55" s="51" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A55" s="53" t="s">
+        <v>119</v>
+      </c>
+      <c r="B55" s="53" t="s">
+        <v>119</v>
+      </c>
+      <c r="C55" s="54" t="s">
+        <v>120</v>
+      </c>
+      <c r="D55" s="53"/>
+      <c r="E55" s="55"/>
+      <c r="F55" s="55"/>
+      <c r="G55" s="56"/>
+      <c r="H55" s="56"/>
+      <c r="I55" s="47" t="s">
+        <v>25</v>
+      </c>
+      <c r="J55" s="57" t="s">
+        <v>121</v>
+      </c>
+      <c r="K55" s="58"/>
+      <c r="L55" s="58"/>
+      <c r="M55" s="58"/>
+      <c r="N55" s="58"/>
+      <c r="O55" s="58"/>
+      <c r="P55" s="58"/>
+      <c r="Q55" s="58"/>
+      <c r="R55" s="58"/>
+      <c r="S55" s="58"/>
+      <c r="T55" s="58"/>
+      <c r="U55" s="58"/>
+      <c r="V55" s="58"/>
+      <c r="W55" s="58"/>
+      <c r="X55" s="58"/>
+      <c r="Y55" s="58"/>
+      <c r="Z55" s="58"/>
+      <c r="AA55" s="58"/>
+      <c r="AB55" s="58"/>
+    </row>
+    <row r="56" s="51" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A56" s="53" t="s">
+        <v>122</v>
+      </c>
+      <c r="B56" s="53" t="s">
+        <v>122</v>
+      </c>
+      <c r="C56" s="54" t="s">
+        <v>123</v>
+      </c>
+      <c r="D56" s="53"/>
+      <c r="E56" s="55"/>
+      <c r="F56" s="55"/>
+      <c r="G56" s="56"/>
+      <c r="H56" s="56"/>
+      <c r="I56" s="47" t="s">
+        <v>25</v>
+      </c>
+      <c r="J56" s="57" t="s">
+        <v>124</v>
+      </c>
+      <c r="K56" s="58"/>
+      <c r="L56" s="58"/>
+      <c r="M56" s="58"/>
+      <c r="N56" s="58"/>
+      <c r="O56" s="58"/>
+      <c r="P56" s="58"/>
+      <c r="Q56" s="58"/>
+      <c r="R56" s="58"/>
+      <c r="S56" s="58"/>
+      <c r="T56" s="58"/>
+      <c r="U56" s="58"/>
+      <c r="V56" s="58"/>
+      <c r="W56" s="58"/>
+      <c r="X56" s="58"/>
+      <c r="Y56" s="58"/>
+      <c r="Z56" s="58"/>
+      <c r="AA56" s="58"/>
+      <c r="AB56" s="58"/>
+    </row>
+    <row r="57" s="51" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A57" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="B40" s="26"/>
-      <c r="C40" s="26"/>
-      <c r="D40" s="25"/>
-      <c r="E40" s="25"/>
-      <c r="F40" s="25"/>
-      <c r="G40" s="25"/>
-      <c r="I40" s="25"/>
-      <c r="J40" s="30"/>
-      <c r="K40" s="30"/>
-      <c r="L40" s="30"/>
-      <c r="M40" s="30"/>
-      <c r="N40" s="30"/>
-      <c r="O40" s="30"/>
-      <c r="P40" s="30"/>
-      <c r="Q40" s="31"/>
-      <c r="R40" s="31"/>
-      <c r="S40" s="31"/>
-      <c r="T40" s="31"/>
-      <c r="U40" s="31"/>
-      <c r="V40" s="31"/>
-      <c r="W40" s="31"/>
-      <c r="X40" s="31"/>
-      <c r="Y40" s="31"/>
-      <c r="Z40" s="31"/>
-      <c r="AA40" s="31"/>
-      <c r="AB40" s="31"/>
-    </row>
-    <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B41" s="32"/>
-      <c r="C41" s="32"/>
-      <c r="G41" s="9"/>
-      <c r="J41" s="33"/>
-      <c r="K41" s="33"/>
-      <c r="L41" s="33"/>
-      <c r="M41" s="33"/>
-      <c r="N41" s="33"/>
-      <c r="O41" s="33"/>
-      <c r="P41" s="33"/>
-      <c r="Q41" s="34"/>
-      <c r="R41" s="34"/>
-      <c r="S41" s="34"/>
-      <c r="T41" s="34"/>
-      <c r="U41" s="34"/>
-      <c r="V41" s="34"/>
-      <c r="W41" s="34"/>
-      <c r="X41" s="34"/>
-      <c r="Y41" s="34"/>
-      <c r="Z41" s="34"/>
-      <c r="AA41" s="34"/>
-      <c r="AB41" s="34"/>
-    </row>
-    <row r="42" s="37" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="35" t="s">
-        <v>16</v>
-      </c>
-      <c r="B42" s="35" t="s">
-        <v>90</v>
-      </c>
-      <c r="C42" s="35" t="s">
-        <v>91</v>
-      </c>
-      <c r="D42" s="35"/>
-      <c r="E42" s="36"/>
-      <c r="F42" s="36"/>
-      <c r="G42" s="35" t="s">
-        <v>30</v>
-      </c>
-      <c r="H42" s="35"/>
-      <c r="I42" s="35" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="43" s="37" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="35" t="s">
-        <v>92</v>
-      </c>
-      <c r="B43" s="35" t="s">
-        <v>93</v>
-      </c>
-      <c r="C43" s="35" t="s">
-        <v>94</v>
-      </c>
-      <c r="D43" s="35"/>
-      <c r="E43" s="36" t="s">
-        <v>95</v>
-      </c>
-      <c r="F43" s="36" t="n">
-        <v>1</v>
-      </c>
-      <c r="G43" s="35"/>
-      <c r="H43" s="35"/>
-      <c r="I43" s="35"/>
-    </row>
-    <row r="44" s="37" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="38" t="s">
-        <v>72</v>
-      </c>
-      <c r="B44" s="39" t="s">
-        <v>96</v>
-      </c>
-      <c r="C44" s="39" t="s">
-        <v>97</v>
-      </c>
-      <c r="D44" s="38" t="s">
-        <v>98</v>
-      </c>
-      <c r="E44" s="40"/>
-      <c r="F44" s="40"/>
-      <c r="G44" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="I44" s="38" t="s">
-        <v>75</v>
-      </c>
-      <c r="J44" s="41"/>
-      <c r="K44" s="41"/>
-      <c r="L44" s="41"/>
-      <c r="M44" s="41"/>
-      <c r="N44" s="41"/>
-      <c r="O44" s="41"/>
-      <c r="P44" s="41"/>
-      <c r="Q44" s="42"/>
-      <c r="R44" s="42"/>
-      <c r="S44" s="42"/>
-      <c r="T44" s="42"/>
-      <c r="U44" s="42"/>
-      <c r="V44" s="42"/>
-      <c r="W44" s="42"/>
-      <c r="X44" s="42"/>
-      <c r="Y44" s="42"/>
-      <c r="Z44" s="42"/>
-      <c r="AA44" s="42"/>
-      <c r="AB44" s="42"/>
-    </row>
-    <row r="45" s="37" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="38" t="s">
-        <v>100</v>
-      </c>
-      <c r="B45" s="39" t="s">
-        <v>101</v>
-      </c>
-      <c r="C45" s="39" t="s">
-        <v>102</v>
-      </c>
-      <c r="D45" s="38"/>
-      <c r="E45" s="40"/>
-      <c r="F45" s="40"/>
-      <c r="G45" s="35" t="s">
-        <v>103</v>
-      </c>
-      <c r="I45" s="38"/>
-      <c r="J45" s="41"/>
-      <c r="K45" s="41"/>
-      <c r="L45" s="41"/>
-      <c r="M45" s="41"/>
-      <c r="N45" s="41"/>
-      <c r="O45" s="41"/>
-      <c r="P45" s="41"/>
-      <c r="Q45" s="42"/>
-      <c r="R45" s="42"/>
-      <c r="S45" s="42"/>
-      <c r="T45" s="42"/>
-      <c r="U45" s="42"/>
-      <c r="V45" s="42"/>
-      <c r="W45" s="42"/>
-      <c r="X45" s="42"/>
-      <c r="Y45" s="42"/>
-      <c r="Z45" s="42"/>
-      <c r="AA45" s="42"/>
-      <c r="AB45" s="42"/>
-    </row>
-    <row r="46" s="37" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A46" s="42" t="s">
-        <v>34</v>
-      </c>
-      <c r="B46" s="39"/>
-      <c r="C46" s="39"/>
-      <c r="D46" s="38"/>
-      <c r="E46" s="40"/>
-      <c r="F46" s="40"/>
-      <c r="I46" s="38"/>
-      <c r="J46" s="41"/>
-      <c r="K46" s="41"/>
-      <c r="L46" s="41"/>
-      <c r="M46" s="41"/>
-      <c r="N46" s="41"/>
-      <c r="O46" s="41"/>
-      <c r="P46" s="41"/>
-      <c r="Q46" s="42"/>
-      <c r="R46" s="42"/>
-      <c r="S46" s="42"/>
-      <c r="T46" s="42"/>
-      <c r="U46" s="42"/>
-      <c r="V46" s="42"/>
-      <c r="W46" s="42"/>
-      <c r="X46" s="42"/>
-      <c r="Y46" s="42"/>
-      <c r="Z46" s="42"/>
-      <c r="AA46" s="42"/>
-      <c r="AB46" s="42"/>
-    </row>
-    <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B47" s="32"/>
-      <c r="C47" s="32"/>
-      <c r="J47" s="33"/>
-      <c r="K47" s="33"/>
-      <c r="L47" s="33"/>
-      <c r="M47" s="33"/>
-      <c r="N47" s="33"/>
-      <c r="O47" s="33"/>
-      <c r="P47" s="33"/>
-      <c r="Q47" s="34"/>
-      <c r="R47" s="34"/>
-      <c r="S47" s="34"/>
-      <c r="T47" s="34"/>
-      <c r="U47" s="34"/>
-      <c r="V47" s="34"/>
-      <c r="W47" s="34"/>
-      <c r="X47" s="34"/>
-      <c r="Y47" s="34"/>
-      <c r="Z47" s="34"/>
-      <c r="AA47" s="34"/>
-      <c r="AB47" s="34"/>
-    </row>
-    <row r="48" s="47" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A48" s="43" t="s">
-        <v>16</v>
-      </c>
-      <c r="B48" s="43" t="s">
-        <v>104</v>
-      </c>
-      <c r="C48" s="44" t="s">
-        <v>105</v>
-      </c>
-      <c r="D48" s="44"/>
-      <c r="E48" s="45"/>
-      <c r="F48" s="46"/>
-      <c r="G48" s="43"/>
-      <c r="H48" s="43"/>
-      <c r="I48" s="43" t="s">
-        <v>19</v>
-      </c>
-      <c r="J48" s="43"/>
-      <c r="K48" s="43"/>
-      <c r="L48" s="43"/>
-      <c r="M48" s="43"/>
-      <c r="N48" s="43"/>
-      <c r="O48" s="43"/>
-      <c r="P48" s="43"/>
-      <c r="Q48" s="43"/>
-      <c r="R48" s="43"/>
-      <c r="S48" s="43"/>
-      <c r="T48" s="43"/>
-      <c r="U48" s="43"/>
-      <c r="V48" s="43"/>
-      <c r="W48" s="43"/>
-      <c r="X48" s="43"/>
-      <c r="Y48" s="43"/>
-      <c r="Z48" s="43"/>
-      <c r="AA48" s="43"/>
-      <c r="AB48" s="43"/>
-    </row>
-    <row r="49" s="47" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A49" s="43" t="s">
-        <v>31</v>
-      </c>
-      <c r="B49" s="48" t="s">
-        <v>106</v>
-      </c>
-      <c r="C49" s="48" t="s">
-        <v>107</v>
-      </c>
-      <c r="D49" s="43"/>
-      <c r="E49" s="46"/>
-      <c r="F49" s="46"/>
-      <c r="G49" s="43"/>
-      <c r="H49" s="43"/>
-      <c r="I49" s="43" t="s">
-        <v>25</v>
-      </c>
-      <c r="J49" s="43"/>
-      <c r="K49" s="43"/>
-      <c r="L49" s="43"/>
-      <c r="M49" s="43"/>
-      <c r="N49" s="43"/>
-      <c r="O49" s="43"/>
-      <c r="P49" s="43"/>
-      <c r="Q49" s="43"/>
-      <c r="R49" s="43"/>
-      <c r="S49" s="43"/>
-      <c r="T49" s="43"/>
-      <c r="U49" s="43"/>
-      <c r="V49" s="43"/>
-      <c r="W49" s="43"/>
-      <c r="X49" s="43"/>
-      <c r="Y49" s="43"/>
-      <c r="Z49" s="43"/>
-      <c r="AA49" s="43"/>
-      <c r="AB49" s="43"/>
-    </row>
-    <row r="50" s="47" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A50" s="49" t="s">
-        <v>108</v>
-      </c>
-      <c r="B50" s="49" t="s">
-        <v>108</v>
-      </c>
-      <c r="C50" s="50" t="s">
-        <v>109</v>
-      </c>
-      <c r="D50" s="49"/>
-      <c r="E50" s="51"/>
-      <c r="F50" s="51"/>
-      <c r="G50" s="52"/>
-      <c r="H50" s="52"/>
-      <c r="I50" s="43" t="s">
-        <v>25</v>
-      </c>
-      <c r="J50" s="53" t="s">
-        <v>110</v>
-      </c>
-      <c r="K50" s="54"/>
-      <c r="L50" s="54"/>
-      <c r="M50" s="54"/>
-      <c r="N50" s="54"/>
-      <c r="O50" s="54"/>
-      <c r="P50" s="54"/>
-      <c r="Q50" s="54"/>
-      <c r="R50" s="54"/>
-      <c r="S50" s="54"/>
-      <c r="T50" s="54"/>
-      <c r="U50" s="54"/>
-      <c r="V50" s="54"/>
-      <c r="W50" s="54"/>
-      <c r="X50" s="54"/>
-      <c r="Y50" s="54"/>
-      <c r="Z50" s="54"/>
-      <c r="AA50" s="54"/>
-      <c r="AB50" s="54"/>
-    </row>
-    <row r="51" s="47" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A51" s="49" t="s">
-        <v>111</v>
-      </c>
-      <c r="B51" s="49" t="s">
-        <v>111</v>
-      </c>
-      <c r="C51" s="50" t="s">
-        <v>112</v>
-      </c>
-      <c r="D51" s="49"/>
-      <c r="E51" s="51"/>
-      <c r="F51" s="51"/>
-      <c r="G51" s="52"/>
-      <c r="H51" s="52"/>
-      <c r="I51" s="43" t="s">
-        <v>25</v>
-      </c>
-      <c r="J51" s="53" t="s">
-        <v>113</v>
-      </c>
-      <c r="K51" s="54"/>
-      <c r="L51" s="54"/>
-      <c r="M51" s="54"/>
-      <c r="N51" s="54"/>
-      <c r="O51" s="54"/>
-      <c r="P51" s="54"/>
-      <c r="Q51" s="54"/>
-      <c r="R51" s="54"/>
-      <c r="S51" s="54"/>
-      <c r="T51" s="54"/>
-      <c r="U51" s="54"/>
-      <c r="V51" s="54"/>
-      <c r="W51" s="54"/>
-      <c r="X51" s="54"/>
-      <c r="Y51" s="54"/>
-      <c r="Z51" s="54"/>
-      <c r="AA51" s="54"/>
-      <c r="AB51" s="54"/>
-    </row>
-    <row r="52" s="47" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A52" s="43" t="s">
-        <v>34</v>
-      </c>
-      <c r="B52" s="43"/>
-      <c r="C52" s="43"/>
-      <c r="D52" s="43"/>
-      <c r="E52" s="46"/>
-      <c r="F52" s="46"/>
-      <c r="G52" s="43"/>
-      <c r="H52" s="43"/>
-      <c r="I52" s="43"/>
-      <c r="J52" s="43"/>
-      <c r="K52" s="43"/>
-      <c r="L52" s="43"/>
-      <c r="M52" s="43"/>
-      <c r="N52" s="43"/>
-      <c r="O52" s="43"/>
-      <c r="P52" s="43"/>
-      <c r="Q52" s="43"/>
-      <c r="R52" s="43"/>
-      <c r="S52" s="43"/>
-      <c r="T52" s="43"/>
-      <c r="U52" s="43"/>
-      <c r="V52" s="43"/>
-      <c r="W52" s="43"/>
-      <c r="X52" s="43"/>
-      <c r="Y52" s="43"/>
-      <c r="Z52" s="43"/>
-      <c r="AA52" s="43"/>
-      <c r="AB52" s="43"/>
-    </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="0" t="s">
+      <c r="B57" s="47"/>
+      <c r="C57" s="47"/>
+      <c r="D57" s="47"/>
+      <c r="E57" s="50"/>
+      <c r="F57" s="50"/>
+      <c r="G57" s="47"/>
+      <c r="H57" s="47"/>
+      <c r="I57" s="47"/>
+      <c r="J57" s="47"/>
+      <c r="K57" s="47"/>
+      <c r="L57" s="47"/>
+      <c r="M57" s="47"/>
+      <c r="N57" s="47"/>
+      <c r="O57" s="47"/>
+      <c r="P57" s="47"/>
+      <c r="Q57" s="47"/>
+      <c r="R57" s="47"/>
+      <c r="S57" s="47"/>
+      <c r="T57" s="47"/>
+      <c r="U57" s="47"/>
+      <c r="V57" s="47"/>
+      <c r="W57" s="47"/>
+      <c r="X57" s="47"/>
+      <c r="Y57" s="47"/>
+      <c r="Z57" s="47"/>
+      <c r="AA57" s="47"/>
+      <c r="AB57" s="47"/>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2654,20 +2856,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z104"/>
+  <dimension ref="A1:Z119"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A55" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C68" activeCellId="1" sqref="I8 C68"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A97" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C120" activeCellId="0" sqref="C120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.72"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>114</v>
+        <v>125</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -2675,7 +2878,7 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="55"/>
+      <c r="D1" s="59"/>
       <c r="E1" s="8"/>
       <c r="F1" s="8"/>
       <c r="G1" s="8"/>
@@ -2709,556 +2912,557 @@
       <c r="C2" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="D2" s="56"/>
+      <c r="D2" s="60"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="s">
         <v>23</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>64</v>
+        <v>126</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="D3" s="56"/>
+        <v>127</v>
+      </c>
+      <c r="D3" s="60"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
         <v>23</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>116</v>
-      </c>
-      <c r="D4" s="56"/>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="D6" s="56"/>
+        <v>128</v>
+      </c>
+      <c r="D4" s="60"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="D5" s="60"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
         <v>27</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>119</v>
+        <v>130</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="D7" s="56"/>
+        <v>131</v>
+      </c>
+      <c r="D7" s="60"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="9" t="s">
         <v>27</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>121</v>
+        <v>132</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="D8" s="56"/>
+        <v>133</v>
+      </c>
+      <c r="D8" s="60"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="9" t="s">
         <v>27</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>123</v>
+        <v>134</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="D9" s="56"/>
+        <v>135</v>
+      </c>
+      <c r="D9" s="60"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="9" t="s">
         <v>27</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>126</v>
-      </c>
-      <c r="D10" s="56"/>
+        <v>137</v>
+      </c>
+      <c r="D10" s="60"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="9" t="s">
         <v>27</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>29</v>
+        <v>138</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="D11" s="56"/>
+        <v>139</v>
+      </c>
+      <c r="D11" s="60"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="9" t="s">
         <v>27</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>128</v>
+        <v>29</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="D12" s="56"/>
+        <v>140</v>
+      </c>
+      <c r="D12" s="60"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="9" t="s">
         <v>27</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>130</v>
+        <v>141</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="D13" s="56"/>
+        <v>142</v>
+      </c>
+      <c r="D13" s="60"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="9" t="s">
         <v>27</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>101</v>
+        <v>126</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="D14" s="56"/>
+        <v>127</v>
+      </c>
+      <c r="D14" s="60"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="9"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="56"/>
+      <c r="A15" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="D15" s="60"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="9" t="s">
-        <v>133</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>134</v>
-      </c>
-      <c r="D16" s="56"/>
+      <c r="A16" s="9"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="60"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="9" t="s">
-        <v>133</v>
+        <v>144</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>135</v>
+        <v>52</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>136</v>
-      </c>
-      <c r="D17" s="56"/>
+        <v>145</v>
+      </c>
+      <c r="D17" s="60"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="9"/>
-      <c r="B18" s="9"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="56"/>
+      <c r="A18" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="D18" s="60"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>137</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>138</v>
-      </c>
-      <c r="D19" s="56"/>
+      <c r="A19" s="9"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="60"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="9" t="s">
         <v>38</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>139</v>
+        <v>148</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="D20" s="56"/>
+        <v>149</v>
+      </c>
+      <c r="D20" s="60"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="9" t="s">
         <v>38</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>141</v>
+        <v>150</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="D21" s="56"/>
+        <v>151</v>
+      </c>
+      <c r="D21" s="60"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="9" t="s">
         <v>38</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>40</v>
+        <v>152</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="D22" s="56"/>
+        <v>153</v>
+      </c>
+      <c r="D22" s="60"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="9" t="s">
         <v>38</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>144</v>
+        <v>40</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>145</v>
-      </c>
-      <c r="D23" s="56"/>
+        <v>154</v>
+      </c>
+      <c r="D23" s="60"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="9" t="s">
         <v>38</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>146</v>
+        <v>155</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="D24" s="56"/>
+        <v>156</v>
+      </c>
+      <c r="D24" s="60"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="9" t="s">
         <v>38</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>148</v>
+        <v>157</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="D25" s="56"/>
+        <v>158</v>
+      </c>
+      <c r="D25" s="60"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="9" t="s">
         <v>38</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>150</v>
+        <v>159</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="D26" s="56"/>
+        <v>160</v>
+      </c>
+      <c r="D26" s="60"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="9" t="s">
         <v>38</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>152</v>
+        <v>161</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>153</v>
-      </c>
-      <c r="D27" s="56"/>
+        <v>162</v>
+      </c>
+      <c r="D27" s="60"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="9" t="s">
         <v>38</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>155</v>
-      </c>
-      <c r="D28" s="56"/>
+        <v>164</v>
+      </c>
+      <c r="D28" s="60"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="9" t="s">
         <v>38</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>156</v>
+        <v>165</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>157</v>
-      </c>
-      <c r="D29" s="56"/>
+        <v>166</v>
+      </c>
+      <c r="D29" s="60"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="9" t="s">
         <v>38</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>158</v>
+        <v>167</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="D30" s="56"/>
+        <v>168</v>
+      </c>
+      <c r="D30" s="60"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="9"/>
-      <c r="B31" s="9"/>
-      <c r="C31" s="9"/>
-      <c r="D31" s="56"/>
+      <c r="A31" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="D31" s="60"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="B32" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="C32" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="D32" s="56"/>
+      <c r="A32" s="9"/>
+      <c r="B32" s="9"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="60"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="9" t="s">
         <v>42</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>161</v>
+        <v>44</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="D33" s="56"/>
+        <v>171</v>
+      </c>
+      <c r="D33" s="60"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="9" t="s">
         <v>42</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>163</v>
+        <v>172</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="D34" s="56"/>
+        <v>173</v>
+      </c>
+      <c r="D34" s="60"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="9" t="s">
         <v>42</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>165</v>
+        <v>174</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>166</v>
-      </c>
-      <c r="D35" s="56"/>
+        <v>175</v>
+      </c>
+      <c r="D35" s="60"/>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="9" t="s">
         <v>42</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>167</v>
+        <v>176</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>168</v>
-      </c>
-      <c r="D36" s="56"/>
+        <v>177</v>
+      </c>
+      <c r="D36" s="60"/>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B37" s="0" t="s">
-        <v>169</v>
-      </c>
-      <c r="C37" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="D37" s="56"/>
+      <c r="B37" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="D37" s="60"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="9"/>
-      <c r="B38" s="9"/>
-      <c r="C38" s="9"/>
-      <c r="D38" s="56"/>
+      <c r="A38" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="D38" s="60"/>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="B39" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="C39" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="D39" s="56"/>
+      <c r="A39" s="9"/>
+      <c r="B39" s="9"/>
+      <c r="C39" s="9"/>
+      <c r="D39" s="60"/>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="9" t="s">
         <v>46</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>135</v>
+        <v>52</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>135</v>
-      </c>
-      <c r="D40" s="56"/>
+        <v>52</v>
+      </c>
+      <c r="D40" s="60"/>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="9"/>
-      <c r="B41" s="9"/>
-      <c r="C41" s="9"/>
-      <c r="D41" s="56"/>
+      <c r="A41" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="D41" s="60"/>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="B42" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="C42" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="D42" s="56"/>
+      <c r="A42" s="9"/>
+      <c r="B42" s="9"/>
+      <c r="C42" s="9"/>
+      <c r="D42" s="60"/>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="9" t="s">
         <v>50</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>135</v>
+        <v>52</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>135</v>
-      </c>
-      <c r="D43" s="56"/>
+        <v>52</v>
+      </c>
+      <c r="D43" s="60"/>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="9" t="s">
         <v>50</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>171</v>
+        <v>146</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>172</v>
-      </c>
-      <c r="D44" s="56"/>
+        <v>146</v>
+      </c>
+      <c r="D44" s="60"/>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="9"/>
-      <c r="B45" s="9"/>
-      <c r="C45" s="9"/>
-      <c r="D45" s="56"/>
+      <c r="A45" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="D45" s="60"/>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="B46" s="9" t="s">
-        <v>173</v>
-      </c>
-      <c r="C46" s="9" t="s">
-        <v>174</v>
-      </c>
-      <c r="D46" s="56"/>
+      <c r="A46" s="9"/>
+      <c r="B46" s="9"/>
+      <c r="C46" s="9"/>
+      <c r="D46" s="60"/>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="9" t="s">
         <v>54</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>56</v>
+        <v>184</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>175</v>
-      </c>
-      <c r="D47" s="56"/>
+        <v>185</v>
+      </c>
+      <c r="D47" s="60"/>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="9" t="s">
         <v>54</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>176</v>
+        <v>56</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>177</v>
-      </c>
-      <c r="D48" s="56"/>
+        <v>186</v>
+      </c>
+      <c r="D48" s="60"/>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="9" t="s">
         <v>54</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>178</v>
+        <v>187</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="D49" s="56"/>
+        <v>188</v>
+      </c>
+      <c r="D49" s="60"/>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="9" t="s">
         <v>54</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>180</v>
+        <v>189</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="D50" s="56"/>
-    </row>
-    <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="B52" s="0" t="s">
-        <v>182</v>
-      </c>
-      <c r="C52" s="0" t="s">
-        <v>183</v>
-      </c>
+        <v>190</v>
+      </c>
+      <c r="D50" s="60"/>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B51" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="C51" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="D51" s="60"/>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
         <v>58</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>184</v>
+        <v>193</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>185</v>
+        <v>194</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3266,10 +3470,10 @@
         <v>58</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>186</v>
+        <v>195</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>187</v>
+        <v>196</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3277,10 +3481,10 @@
         <v>58</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>188</v>
+        <v>197</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>189</v>
+        <v>198</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3288,483 +3492,626 @@
         <v>58</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A58" s="0" t="s">
-        <v>192</v>
-      </c>
-      <c r="B58" s="0" t="s">
-        <v>193</v>
-      </c>
-      <c r="C58" s="0" t="s">
-        <v>194</v>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="B57" s="0" t="s">
+        <v>201</v>
+      </c>
+      <c r="C57" s="0" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>192</v>
+        <v>203</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>195</v>
+        <v>204</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>196</v>
+        <v>205</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>192</v>
+        <v>203</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>197</v>
+        <v>206</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>198</v>
+        <v>207</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>192</v>
+        <v>203</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>199</v>
+        <v>208</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>200</v>
+        <v>209</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>192</v>
+        <v>203</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>135</v>
+        <v>210</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>201</v>
+        <v>211</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>192</v>
+        <v>203</v>
       </c>
       <c r="B63" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="C63" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A64" s="0" t="s">
+        <v>203</v>
+      </c>
+      <c r="B64" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="C63" s="0" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="B65" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="C65" s="0" t="s">
-        <v>202</v>
+      <c r="C64" s="0" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>95</v>
+        <v>112</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="B68" s="0" t="s">
-        <v>204</v>
-      </c>
-      <c r="C68" s="0" t="s">
-        <v>205</v>
+        <v>213</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="B67" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="C67" s="0" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>88</v>
+        <v>215</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="B71" s="0" t="s">
-        <v>207</v>
-      </c>
-      <c r="C71" s="0" t="s">
-        <v>208</v>
+        <v>216</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="B70" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="C70" s="0" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>209</v>
+        <v>218</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>210</v>
+        <v>219</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>211</v>
+        <v>220</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>212</v>
+        <v>221</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>213</v>
+        <v>222</v>
       </c>
       <c r="C74" s="0" t="s">
-        <v>214</v>
+        <v>223</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>215</v>
+        <v>224</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>217</v>
+        <v>226</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>219</v>
+        <v>228</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>220</v>
+        <v>229</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>221</v>
+        <v>230</v>
       </c>
       <c r="C78" s="0" t="s">
-        <v>222</v>
+        <v>231</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>223</v>
+        <v>232</v>
       </c>
       <c r="C79" s="0" t="s">
-        <v>224</v>
+        <v>233</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="B80" s="0" t="s">
+        <v>234</v>
+      </c>
+      <c r="C80" s="0" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="B81" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="C80" s="0" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="B82" s="0" t="s">
-        <v>226</v>
-      </c>
-      <c r="C82" s="0" t="s">
-        <v>227</v>
+      <c r="C81" s="0" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>228</v>
+        <v>237</v>
       </c>
       <c r="C83" s="0" t="s">
-        <v>229</v>
+        <v>238</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>230</v>
+        <v>239</v>
       </c>
       <c r="C84" s="0" t="s">
-        <v>231</v>
+        <v>240</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>232</v>
+        <v>241</v>
       </c>
       <c r="C85" s="0" t="s">
-        <v>233</v>
+        <v>242</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>234</v>
+        <v>243</v>
       </c>
       <c r="C86" s="0" t="s">
-        <v>235</v>
+        <v>244</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>236</v>
+        <v>245</v>
       </c>
       <c r="C87" s="0" t="s">
-        <v>237</v>
+        <v>246</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>238</v>
+        <v>247</v>
       </c>
       <c r="C88" s="0" t="s">
-        <v>239</v>
+        <v>248</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>240</v>
+        <v>249</v>
       </c>
       <c r="C89" s="0" t="s">
-        <v>241</v>
+        <v>250</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>242</v>
+        <v>251</v>
       </c>
       <c r="C90" s="0" t="s">
-        <v>243</v>
+        <v>252</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="B91" s="0" t="s">
-        <v>244</v>
+        <v>253</v>
       </c>
       <c r="C91" s="0" t="s">
-        <v>245</v>
+        <v>254</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="B92" s="0" t="s">
-        <v>246</v>
+        <v>255</v>
       </c>
       <c r="C92" s="0" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="B93" s="0" t="s">
-        <v>248</v>
+        <v>257</v>
       </c>
       <c r="C93" s="0" t="s">
-        <v>249</v>
+        <v>258</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="B94" s="0" t="s">
-        <v>250</v>
+        <v>259</v>
       </c>
       <c r="C94" s="0" t="s">
-        <v>251</v>
+        <v>260</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="B95" s="0" t="s">
-        <v>252</v>
+        <v>261</v>
       </c>
       <c r="C95" s="0" t="s">
-        <v>253</v>
+        <v>262</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="B96" s="0" t="s">
-        <v>254</v>
+        <v>263</v>
       </c>
       <c r="C96" s="0" t="s">
-        <v>255</v>
+        <v>264</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="B97" s="0" t="s">
-        <v>256</v>
+        <v>265</v>
       </c>
       <c r="C97" s="0" t="s">
-        <v>257</v>
+        <v>266</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="B98" s="0" t="s">
-        <v>258</v>
+        <v>267</v>
       </c>
       <c r="C98" s="0" t="s">
-        <v>259</v>
+        <v>268</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="B99" s="0" t="s">
-        <v>260</v>
+        <v>269</v>
       </c>
       <c r="C99" s="0" t="s">
-        <v>261</v>
+        <v>270</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="B100" s="0" t="s">
-        <v>262</v>
+        <v>271</v>
       </c>
       <c r="C100" s="0" t="s">
-        <v>263</v>
+        <v>272</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="B101" s="0" t="s">
-        <v>264</v>
+        <v>273</v>
       </c>
       <c r="C101" s="0" t="s">
-        <v>265</v>
+        <v>274</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="B102" s="0" t="s">
-        <v>266</v>
+        <v>275</v>
       </c>
       <c r="C102" s="0" t="s">
-        <v>267</v>
+        <v>276</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="B103" s="0" t="s">
-        <v>52</v>
+        <v>277</v>
       </c>
       <c r="C103" s="0" t="s">
-        <v>268</v>
+        <v>278</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="B104" s="0" t="s">
-        <v>86</v>
+        <v>52</v>
       </c>
       <c r="C104" s="0" t="s">
-        <v>269</v>
+        <v>279</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="B105" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="C105" s="0" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="B107" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="C107" s="0" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="B108" s="0" t="s">
+        <v>282</v>
+      </c>
+      <c r="C108" s="0" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="B109" s="0" t="s">
+        <v>284</v>
+      </c>
+      <c r="C109" s="0" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="B110" s="0" t="s">
+        <v>286</v>
+      </c>
+      <c r="C110" s="0" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="B111" s="0" t="s">
+        <v>288</v>
+      </c>
+      <c r="C111" s="0" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="B112" s="0" t="s">
+        <v>290</v>
+      </c>
+      <c r="C112" s="0" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="61" t="s">
+        <v>292</v>
+      </c>
+      <c r="B114" s="0" t="s">
+        <v>293</v>
+      </c>
+      <c r="C114" s="0" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="61" t="s">
+        <v>292</v>
+      </c>
+      <c r="B115" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="C115" s="0" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="61" t="s">
+        <v>292</v>
+      </c>
+      <c r="B116" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C116" s="0" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="61" t="s">
+        <v>292</v>
+      </c>
+      <c r="B117" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="C117" s="0" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="61" t="s">
+        <v>292</v>
+      </c>
+      <c r="B118" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="C118" s="0" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="61" t="s">
+        <v>292</v>
+      </c>
+      <c r="B119" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="C119" s="0" t="s">
+        <v>299</v>
       </c>
     </row>
   </sheetData>
@@ -3786,7 +4133,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="I8 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3795,20 +4142,20 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="57" t="s">
-        <v>270</v>
-      </c>
-      <c r="B1" s="57" t="s">
-        <v>271</v>
+      <c r="A1" s="62" t="s">
+        <v>300</v>
+      </c>
+      <c r="B1" s="62" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="58" t="n">
+      <c r="A2" s="63" t="n">
         <f aca="true">NOW()</f>
-        <v>44248.7959142919</v>
-      </c>
-      <c r="B2" s="59" t="s">
-        <v>272</v>
+        <v>44248.8522761246</v>
+      </c>
+      <c r="B2" s="64" t="s">
+        <v>302</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add a few more features
</commit_message>
<xml_diff>
--- a/XForms/highways.xlsx
+++ b/XForms/highways.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="310">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -45,7 +45,7 @@
     <t xml:space="preserve">relevant</t>
   </si>
   <si>
-    <t xml:space="preserve">calculation</t>
+    <t xml:space="preserve">parameters</t>
   </si>
   <si>
     <t xml:space="preserve">appearance</t>
@@ -126,6 +126,18 @@
     <t xml:space="preserve">Does this road have a name?</t>
   </si>
   <si>
+    <t xml:space="preserve">highway_ref</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What is the reference number of this highway ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">usfs_ref</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USFS reference (if there is one)</t>
+  </si>
+  <si>
     <t xml:space="preserve">end_group</t>
   </si>
   <si>
@@ -144,411 +156,423 @@
     <t xml:space="preserve">What is the surface of this road?</t>
   </si>
   <si>
+    <t xml:space="preserve">dirt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select_one smoothness</t>
+  </si>
+  <si>
+    <t xml:space="preserve">smoothness</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How smooth is this road?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select_one oneway</t>
+  </si>
+  <si>
+    <t xml:space="preserve">oneway</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is it oneway?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(direction of traffic, NOT the number of lane)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select_one accessibility</t>
+  </si>
+  <si>
+    <t xml:space="preserve">accessibility</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is the road is accessible throughout the year?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select_multiple vehicle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vehicle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What type of vehicle can be used to access your area?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">car</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select_one tracktype</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tracktype</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What is the quality of this highway ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">grade2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">range</t>
+  </si>
+  <si>
+    <t xml:space="preserve">width</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What is the width?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(in meters)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Step=1, end=3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sac</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Path conditions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${feature_type} = 'path'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select_one sac_scale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sac_scale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What is the difficulty of this path ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hiking</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Step=1,end=2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select_one trail_visibility</t>
+  </si>
+  <si>
+    <t xml:space="preserve">visibility</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How difficult is it to follow the path ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">intermediate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bridge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bridges</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${feature_type} = 'bridge'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select_one bridge_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bridge_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What type of bridge is it ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bridge_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name of this bridge if it has one</t>
+  </si>
+  <si>
+    <t xml:space="preserve">geopoint</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bridge_point</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Please take a GPS location on this bridge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">placement-map</t>
+  </si>
+  <si>
+    <t xml:space="preserve">barriers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is there a barrier blocking this highway ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${feature_type} = 'barrier'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select_one barrier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">barrier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What type of barrier is it ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name or reference on the barrier if there is one</t>
+  </si>
+  <si>
+    <t xml:space="preserve">barrier_point</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Please take a GPS location of this barrier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select_one swing_gate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">swing_gate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Type of swing gate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">single</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${barrier} = 'swing_gate'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gps</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPS Coordinates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${feature_type} = 'highway' or ${feature_type} = 'path'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select_one gps_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gps_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Type of GPS recording</t>
+  </si>
+  <si>
+    <t xml:space="preserve">point</t>
+  </si>
+  <si>
+    <t xml:space="preserve">highway_point</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Please take a GPS point at the feature location.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Where are we ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${gps_type} = 'point'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">geotrace</t>
+  </si>
+  <si>
+    <t xml:space="preserve">track</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Please record a GPS tracks while you are walking for driving</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${gps_type} = 'track'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">comments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">comment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Any other comments about this feature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">audio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Audio Note</t>
+  </si>
+  <si>
+    <t xml:space="preserve">odktest.wav</t>
+  </si>
+  <si>
+    <t xml:space="preserve">image</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Take A Picture</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Max-pixels=1000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">odktest.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">list_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">path</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Path (foot traffic only)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bridge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Barrier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">trunk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trunk (The most important roads in a country's system that aren't motorways)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">primary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Primary (The next most important roads in a country's system, ften linking larger towns)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">secondary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Secondary (major road within city)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tertiary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tertiary (The next most important roads in a country's system, ften linking smaller towns and villages)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unclassified</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unclassified (The least important through roads in a country's system – i.e. minor roads of a lower classification than tertiary, but which serve a purpose other than access to properties)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Residential (Roads which serve as an access to housing, without function of connecting settlements. Often lined with housing)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">service</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Service (driveways, access roads)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Track (jeep trail)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes_no</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">paved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paved (predominantly paved; i.e., it is covered with paving stones, concrete or bitumen)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">asphalt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Asphalt (short for asphalt concrete - mineral aggregate bound by asphalt)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">concrete</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Concrete (cement based concrete, forming a large surface, typically cast in place and may have predetermined breaking joints)</t>
+  </si>
+  <si>
     <t xml:space="preserve">unpaved</t>
   </si>
   <si>
-    <t xml:space="preserve">select_one smoothness</t>
-  </si>
-  <si>
-    <t xml:space="preserve">smoothness</t>
-  </si>
-  <si>
-    <t xml:space="preserve">How smooth is this road?</t>
+    <t xml:space="preserve">Unpaved (A feature that is predominantly unsealed (unpaved); i.e., it has a loose covering ranging from compacted stone chippings to earth)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cobblestone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cobblestone (raw cobblestone of natural, uncut, rounded stones. Unlike pebblestone firmly connected to the ground)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sand (small to very small fractions (less than 2mm) of rock.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gravel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gravel (broken/crushed rock with sharp edges, known as ballast on railways. Usually loosely arranged)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">compacted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compacted (mixture of larger (e.g., gravel) and smaller (e.g., sand) parts, compacted (e.g., with a roller), so the surface is more stable than loose gravel)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dirt (gravel is sometimes mistakenly called dirt. Some compacted surfaces are sometimes called "dirt" too, please consider using  compacted)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">metal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Metal (used for metal surfaced bridges, or for temporary tracks over fields for normal road vehicles or site traffic)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">grass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grass (Grass covered ground. Mostly nice to walk. May turn into surface=dirt or become overgrown and disappear)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mud</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mud (most of the year wet which gives a soft ground with low carrying capacity. Mostly found on wetland like swamps or in tidal areas)</t>
   </si>
   <si>
     <t xml:space="preserve">good</t>
   </si>
   <si>
-    <t xml:space="preserve">select_one oneway</t>
-  </si>
-  <si>
-    <t xml:space="preserve">oneway</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Is it oneway?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(direction of traffic, NOT the number of lane)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">select_one accessibility</t>
-  </si>
-  <si>
-    <t xml:space="preserve">accessibility</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Is the road is accessible throughout the year?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">yes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">select_multiple vehicle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vehicle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">What type of vehicle can be used to access your area?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">car</t>
-  </si>
-  <si>
-    <t xml:space="preserve">select_one tracktype</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tracktype</t>
-  </si>
-  <si>
-    <t xml:space="preserve">What is the quality of this highway ?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">integer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">width</t>
-  </si>
-  <si>
-    <t xml:space="preserve">What is the width?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(in meters)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sac</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Path conditions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">${feature_type} = 'path'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">select_one sac_scale</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sac_scale</t>
-  </si>
-  <si>
-    <t xml:space="preserve">What is the difficulty of this path ?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hiking</t>
-  </si>
-  <si>
-    <t xml:space="preserve">select_one trail_visibility</t>
-  </si>
-  <si>
-    <t xml:space="preserve">visibility</t>
-  </si>
-  <si>
-    <t xml:space="preserve">How difficult is it to follow the path ?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bridge</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bridges</t>
-  </si>
-  <si>
-    <t xml:space="preserve">${feature_type} = 'bridge'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">select_one bridge_type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bridge_type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">What type of bridge is it ?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bridge_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Name of this bridge if it has one</t>
-  </si>
-  <si>
-    <t xml:space="preserve">geopoint</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bridge_point</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Please take a GPS location on this bridge</t>
-  </si>
-  <si>
-    <t xml:space="preserve">placement-map</t>
-  </si>
-  <si>
-    <t xml:space="preserve">barriers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Is there a barrier blocking this highway ?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">${feature_type} = 'barrier'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">select_one barrier</t>
-  </si>
-  <si>
-    <t xml:space="preserve">barrier</t>
-  </si>
-  <si>
-    <t xml:space="preserve">What type of barrier is it ?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Name or reference on the barrier if there is one</t>
-  </si>
-  <si>
-    <t xml:space="preserve">barrier_point</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Please take a GPS location of this barrier</t>
-  </si>
-  <si>
-    <t xml:space="preserve">select_one swing_gate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">swing_gate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Type of swing gate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">single</t>
-  </si>
-  <si>
-    <t xml:space="preserve">${barrier} = 'swing_gate'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gps</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GPS Coordinates</t>
-  </si>
-  <si>
-    <t xml:space="preserve">${feature_type} = 'highway' or ${feature_type} = 'path'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">select_one gps_type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gps_type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Type of GPS recording</t>
-  </si>
-  <si>
-    <t xml:space="preserve">point</t>
-  </si>
-  <si>
-    <t xml:space="preserve">highway_point</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Please take a GPS point at the feature location.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Where are we ?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">${gps_type} = 'point'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">geotrace</t>
-  </si>
-  <si>
-    <t xml:space="preserve">track</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Please record a GPS tracks while you are walking for driving</t>
-  </si>
-  <si>
-    <t xml:space="preserve">${gps_type} = 'track'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">comments</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Comments</t>
-  </si>
-  <si>
-    <t xml:space="preserve">comment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Any other comments about this feature</t>
-  </si>
-  <si>
-    <t xml:space="preserve">audio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Audio Note</t>
-  </si>
-  <si>
-    <t xml:space="preserve">odktest.wav</t>
-  </si>
-  <si>
-    <t xml:space="preserve">image</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Take A Picture</t>
-  </si>
-  <si>
-    <t xml:space="preserve">odktest.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">list_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">path</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Path (foot traffic only)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bridge</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Barrier</t>
-  </si>
-  <si>
-    <t xml:space="preserve">trunk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Trunk (The most important roads in a country's system that aren't motorways)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">primary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Primary (The next most important roads in a country's system, ften linking larger towns)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">secondary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Secondary (major road within city)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tertiary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tertiary (The next most important roads in a country's system, ften linking smaller towns and villages)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">unclassified</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unclassified (The least important through roads in a country's system – i.e. minor roads of a lower classification than tertiary, but which serve a purpose other than access to properties)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Residential (Roads which serve as an access to housing, without function of connecting settlements. Often lined with housing)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">service</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Service (driveways, access roads)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Track (jeep trail)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">yes_no</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">no</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No</t>
-  </si>
-  <si>
-    <t xml:space="preserve">paved</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Paved (predominantly paved; i.e., it is covered with paving stones, concrete or bitumen)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">asphalt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Asphalt (short for asphalt concrete - mineral aggregate bound by asphalt)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">concrete</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Concrete (cement based concrete, forming a large surface, typically cast in place and may have predetermined breaking joints)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unpaved (A feature that is predominantly unsealed (unpaved); i.e., it has a loose covering ranging from compacted stone chippings to earth)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cobblestone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cobblestone (raw cobblestone of natural, uncut, rounded stones. Unlike pebblestone firmly connected to the ground)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sand</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sand (small to very small fractions (less than 2mm) of rock.)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gravel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gravel (broken/crushed rock with sharp edges, known as ballast on railways. Usually loosely arranged)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">compacted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Compacted (mixture of larger (e.g., gravel) and smaller (e.g., sand) parts, compacted (e.g., with a roller), so the surface is more stable than loose gravel)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dirt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dirt (gravel is sometimes mistakenly called dirt. Some compacted surfaces are sometimes called "dirt" too, please consider using  compacted)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">metal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Metal (used for metal surfaced bridges, or for temporary tracks over fields for normal road vehicles or site traffic)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">grass</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grass (Grass covered ground. Mostly nice to walk. May turn into surface=dirt or become overgrown and disappear)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mud</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mud (most of the year wet which gives a soft ground with low carrying capacity. Mostly found on wetland like swamps or in tidal areas)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Good (Possible to drive consistently at the speed limit without worrying about imperfections)</t>
   </si>
   <si>
-    <t xml:space="preserve">intermediate</t>
-  </si>
-  <si>
     <t xml:space="preserve">Intermediate (Occasional imperfections requiring caution or slow passage)</t>
   </si>
   <si>
-    <t xml:space="preserve">bad</t>
-  </si>
-  <si>
     <t xml:space="preserve">Bad (Many imperfections, not possible to drive consistently at the speed limit)</t>
   </si>
   <si>
@@ -607,9 +631,6 @@
   </si>
   <si>
     <t xml:space="preserve">Grade 1 (usually a paved or sealed surface)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">grade2</t>
   </si>
   <si>
     <t xml:space="preserve">Grade 2 (solid but unpaved. Usually an unpaved track with surface of gravel)</t>
@@ -1465,18 +1486,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AB60"/>
+  <dimension ref="A1:AB63"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F33" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G47" activeCellId="0" sqref="G47"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H34" activeCellId="0" sqref="H34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="37.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="36.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="14.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="10"/>
   </cols>
@@ -1734,132 +1755,129 @@
     </row>
     <row r="15" s="13" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="11"/>
-      <c r="C15" s="11"/>
+      <c r="C15" s="11" t="s">
+        <v>35</v>
+      </c>
       <c r="D15" s="11"/>
       <c r="E15" s="12"/>
       <c r="F15" s="12"/>
-      <c r="G15" s="11"/>
+      <c r="G15" s="11" t="s">
+        <v>30</v>
+      </c>
       <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
+      <c r="I15" s="11" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="16" s="13" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="11"/>
-      <c r="B16" s="11"/>
-      <c r="C16" s="11"/>
+      <c r="A16" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>37</v>
+      </c>
       <c r="D16" s="11"/>
       <c r="E16" s="12"/>
       <c r="F16" s="12"/>
-      <c r="G16" s="11"/>
+      <c r="G16" s="11" t="s">
+        <v>30</v>
+      </c>
       <c r="H16" s="11"/>
-      <c r="I16" s="11"/>
+      <c r="I16" s="11" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="17" s="13" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0"/>
-      <c r="B17" s="0"/>
-      <c r="C17" s="0"/>
-      <c r="D17" s="0"/>
+      <c r="A17" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
       <c r="E17" s="12"/>
       <c r="F17" s="12"/>
       <c r="G17" s="11"/>
       <c r="H17" s="11"/>
       <c r="I17" s="11"/>
     </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="9"/>
-      <c r="B18" s="9"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9"/>
-    </row>
-    <row r="19" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="B19" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="C19" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="D19" s="14"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="B20" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="C20" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="D20" s="14"/>
-      <c r="E20" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="F20" s="15" t="n">
-        <v>1</v>
-      </c>
-      <c r="H20" s="14"/>
-      <c r="I20" s="14" t="s">
-        <v>25</v>
-      </c>
+    <row r="18" s="13" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="11"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+    </row>
+    <row r="19" s="13" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0"/>
+      <c r="B19" s="0"/>
+      <c r="C19" s="0"/>
+      <c r="D19" s="0"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="9"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
     </row>
     <row r="21" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="14" t="s">
-        <v>41</v>
+        <v>16</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D21" s="14"/>
-      <c r="E21" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="F21" s="15" t="n">
-        <v>1</v>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="14" t="s">
+        <v>30</v>
       </c>
       <c r="H21" s="14"/>
       <c r="I21" s="14" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="14" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="D22" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="E22" s="15"/>
+        <v>43</v>
+      </c>
+      <c r="D22" s="14"/>
+      <c r="E22" s="15" t="s">
+        <v>44</v>
+      </c>
       <c r="F22" s="15" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H22" s="14"/>
       <c r="I22" s="14" t="s">
@@ -1868,21 +1886,20 @@
     </row>
     <row r="23" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="14" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D23" s="14"/>
       <c r="E23" s="15" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="F23" s="15" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H23" s="14"/>
       <c r="I23" s="14" t="s">
@@ -1891,20 +1908,23 @@
     </row>
     <row r="24" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="E24" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="B24" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="C24" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="D24" s="14"/>
-      <c r="E24" s="15" t="s">
-        <v>56</v>
-      </c>
       <c r="F24" s="15" t="n">
-        <v>1</v>
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
       <c r="H24" s="14"/>
       <c r="I24" s="14" t="s">
@@ -1913,17 +1933,22 @@
     </row>
     <row r="25" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="14" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D25" s="14"/>
-      <c r="E25" s="15"/>
-      <c r="F25" s="15"/>
+      <c r="E25" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="F25" s="15" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
       <c r="H25" s="14"/>
       <c r="I25" s="14" t="s">
         <v>25</v>
@@ -1931,278 +1956,246 @@
     </row>
     <row r="26" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="D26" s="14"/>
+      <c r="E26" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="B26" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="C26" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="D26" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="E26" s="15"/>
       <c r="F26" s="15" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="G26" s="14"/>
+        <v>1</v>
+      </c>
       <c r="H26" s="14"/>
-      <c r="I26" s="14"/>
+      <c r="I26" s="14" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="27" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="B27" s="14"/>
-      <c r="C27" s="14"/>
+        <v>61</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>63</v>
+      </c>
       <c r="D27" s="14"/>
-      <c r="E27" s="15"/>
+      <c r="E27" s="15" t="s">
+        <v>64</v>
+      </c>
       <c r="F27" s="15"/>
-      <c r="G27" s="14"/>
       <c r="H27" s="14"/>
-      <c r="I27" s="14"/>
-    </row>
-    <row r="28" s="19" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="17"/>
-      <c r="B28" s="17"/>
-      <c r="C28" s="17"/>
-      <c r="D28" s="17"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="17"/>
-      <c r="H28" s="17"/>
-      <c r="I28" s="17"/>
-    </row>
-    <row r="29" s="22" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="B29" s="20" t="s">
-        <v>64</v>
-      </c>
-      <c r="C29" s="20" t="s">
+      <c r="I27" s="14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="D29" s="20"/>
-      <c r="E29" s="21"/>
-      <c r="F29" s="21"/>
-      <c r="G29" s="20" t="s">
+      <c r="B28" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="H29" s="20"/>
-      <c r="I29" s="20"/>
-    </row>
-    <row r="30" s="22" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="20" t="s">
+      <c r="C28" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="B30" s="20" t="s">
+      <c r="D28" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="C30" s="20" t="s">
+      <c r="E28" s="15"/>
+      <c r="F28" s="15" t="n">
+        <v>2</v>
+      </c>
+      <c r="G28" s="14"/>
+      <c r="H28" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="D30" s="20"/>
-      <c r="E30" s="21" t="s">
-        <v>70</v>
-      </c>
-      <c r="F30" s="21"/>
-      <c r="H30" s="20"/>
-      <c r="I30" s="20" t="s">
+      <c r="I28" s="14" t="s">
         <v>25</v>
       </c>
+    </row>
+    <row r="29" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B29" s="14"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="15"/>
+      <c r="G29" s="14"/>
+      <c r="H29" s="14"/>
+      <c r="I29" s="14"/>
+    </row>
+    <row r="30" s="19" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="17"/>
+      <c r="B30" s="17"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="17"/>
+      <c r="H30" s="17"/>
+      <c r="I30" s="17"/>
     </row>
     <row r="31" s="22" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B31" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="C31" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="B31" s="20" t="s">
+      <c r="D31" s="20"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="21"/>
+      <c r="G31" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="C31" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="D31" s="20"/>
-      <c r="E31" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="F31" s="21"/>
-      <c r="G31" s="20"/>
       <c r="H31" s="20"/>
-      <c r="I31" s="20" t="s">
-        <v>25</v>
-      </c>
+      <c r="I31" s="20"/>
     </row>
     <row r="32" s="22" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="B32" s="20"/>
-      <c r="C32" s="20"/>
+        <v>73</v>
+      </c>
+      <c r="B32" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="C32" s="20" t="s">
+        <v>75</v>
+      </c>
       <c r="D32" s="20"/>
-      <c r="E32" s="21"/>
+      <c r="E32" s="21" t="s">
+        <v>76</v>
+      </c>
       <c r="F32" s="21"/>
-      <c r="G32" s="20"/>
       <c r="H32" s="20"/>
-      <c r="I32" s="20"/>
-    </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="9"/>
-      <c r="B33" s="9"/>
-      <c r="C33" s="9"/>
-      <c r="D33" s="9"/>
-      <c r="E33" s="10"/>
-      <c r="F33" s="10"/>
-      <c r="G33" s="9"/>
-      <c r="H33" s="9"/>
-      <c r="I33" s="9"/>
-    </row>
-    <row r="34" s="26" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="23" t="s">
+      <c r="I32" s="20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="33" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="B33" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C33" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="D33" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="E33" s="15"/>
+      <c r="F33" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="G33" s="14"/>
+      <c r="H33" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="I33" s="20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="34" s="22" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="B34" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="C34" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="D34" s="20"/>
+      <c r="E34" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="F34" s="21"/>
+      <c r="G34" s="20"/>
+      <c r="H34" s="20"/>
+      <c r="I34" s="20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="35" s="22" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B35" s="20"/>
+      <c r="C35" s="20"/>
+      <c r="D35" s="20"/>
+      <c r="E35" s="21"/>
+      <c r="F35" s="21"/>
+      <c r="G35" s="20"/>
+      <c r="H35" s="20"/>
+      <c r="I35" s="20"/>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="9"/>
+      <c r="B36" s="9"/>
+      <c r="C36" s="9"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="10"/>
+      <c r="F36" s="10"/>
+      <c r="G36" s="9"/>
+      <c r="H36" s="9"/>
+      <c r="I36" s="9"/>
+    </row>
+    <row r="37" s="26" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="B34" s="24" t="s">
-        <v>74</v>
-      </c>
-      <c r="C34" s="24" t="s">
-        <v>75</v>
-      </c>
-      <c r="D34" s="24"/>
-      <c r="E34" s="25"/>
-      <c r="F34" s="25"/>
-      <c r="G34" s="24" t="s">
-        <v>76</v>
-      </c>
-      <c r="H34" s="24"/>
-      <c r="I34" s="24" t="s">
+      <c r="B37" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="C37" s="24" t="s">
+        <v>83</v>
+      </c>
+      <c r="D37" s="24"/>
+      <c r="E37" s="25"/>
+      <c r="F37" s="25"/>
+      <c r="G37" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="H37" s="24"/>
+      <c r="I37" s="24" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="35" s="26" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="23" t="s">
-        <v>77</v>
-      </c>
-      <c r="B35" s="27" t="s">
-        <v>78</v>
-      </c>
-      <c r="C35" s="27" t="s">
-        <v>79</v>
-      </c>
-      <c r="D35" s="23"/>
-      <c r="E35" s="28" t="s">
-        <v>52</v>
-      </c>
-      <c r="F35" s="28" t="n">
+    <row r="38" s="26" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A38" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="B38" s="27" t="s">
+        <v>86</v>
+      </c>
+      <c r="C38" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="D38" s="23"/>
+      <c r="E38" s="28" t="s">
+        <v>88</v>
+      </c>
+      <c r="F38" s="28" t="n">
         <v>1</v>
       </c>
-      <c r="G35" s="24"/>
-      <c r="I35" s="23" t="s">
+      <c r="G38" s="24"/>
+      <c r="I38" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="J35" s="29"/>
-      <c r="K35" s="29"/>
-      <c r="L35" s="29"/>
-      <c r="M35" s="29"/>
-      <c r="N35" s="29"/>
-      <c r="O35" s="29"/>
-      <c r="P35" s="29"/>
-      <c r="Q35" s="30"/>
-      <c r="R35" s="30"/>
-      <c r="S35" s="30"/>
-      <c r="T35" s="30"/>
-      <c r="U35" s="30"/>
-      <c r="V35" s="30"/>
-      <c r="W35" s="30"/>
-      <c r="X35" s="30"/>
-      <c r="Y35" s="30"/>
-      <c r="Z35" s="30"/>
-      <c r="AA35" s="30"/>
-      <c r="AB35" s="30"/>
-    </row>
-    <row r="36" s="26" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="B36" s="27" t="s">
-        <v>80</v>
-      </c>
-      <c r="C36" s="27" t="s">
-        <v>81</v>
-      </c>
-      <c r="D36" s="23"/>
-      <c r="E36" s="28"/>
-      <c r="F36" s="28"/>
-      <c r="G36" s="24"/>
-      <c r="I36" s="23"/>
-      <c r="J36" s="29"/>
-      <c r="K36" s="29"/>
-      <c r="L36" s="29"/>
-      <c r="M36" s="29"/>
-      <c r="N36" s="29"/>
-      <c r="O36" s="29"/>
-      <c r="P36" s="29"/>
-      <c r="Q36" s="30"/>
-      <c r="R36" s="30"/>
-      <c r="S36" s="30"/>
-      <c r="T36" s="30"/>
-      <c r="U36" s="30"/>
-      <c r="V36" s="30"/>
-      <c r="W36" s="30"/>
-      <c r="X36" s="30"/>
-      <c r="Y36" s="30"/>
-      <c r="Z36" s="30"/>
-      <c r="AA36" s="30"/>
-      <c r="AB36" s="30"/>
-    </row>
-    <row r="37" s="26" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="23" t="s">
-        <v>82</v>
-      </c>
-      <c r="B37" s="27" t="s">
-        <v>83</v>
-      </c>
-      <c r="C37" s="27" t="s">
-        <v>84</v>
-      </c>
-      <c r="D37" s="23"/>
-      <c r="E37" s="28"/>
-      <c r="F37" s="28"/>
-      <c r="I37" s="23" t="s">
-        <v>85</v>
-      </c>
-      <c r="J37" s="29"/>
-      <c r="K37" s="29"/>
-      <c r="L37" s="29"/>
-      <c r="M37" s="29"/>
-      <c r="N37" s="29"/>
-      <c r="O37" s="29"/>
-      <c r="P37" s="29"/>
-      <c r="Q37" s="30"/>
-      <c r="R37" s="30"/>
-      <c r="S37" s="30"/>
-      <c r="T37" s="30"/>
-      <c r="U37" s="30"/>
-      <c r="V37" s="30"/>
-      <c r="W37" s="30"/>
-      <c r="X37" s="30"/>
-      <c r="Y37" s="30"/>
-      <c r="Z37" s="30"/>
-      <c r="AA37" s="30"/>
-      <c r="AB37" s="30"/>
-    </row>
-    <row r="38" s="26" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="B38" s="27"/>
-      <c r="C38" s="27"/>
-      <c r="D38" s="23"/>
-      <c r="E38" s="28"/>
-      <c r="F38" s="28"/>
-      <c r="G38" s="24"/>
-      <c r="I38" s="23"/>
       <c r="J38" s="29"/>
       <c r="K38" s="29"/>
       <c r="L38" s="29"/>
@@ -2223,138 +2216,126 @@
       <c r="AA38" s="30"/>
       <c r="AB38" s="30"/>
     </row>
-    <row r="40" s="35" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="31" t="s">
-        <v>16</v>
-      </c>
-      <c r="B40" s="32" t="s">
-        <v>86</v>
-      </c>
-      <c r="C40" s="32" t="s">
-        <v>87</v>
-      </c>
-      <c r="D40" s="31"/>
-      <c r="E40" s="33"/>
-      <c r="F40" s="33"/>
-      <c r="G40" s="34" t="s">
-        <v>88</v>
-      </c>
-      <c r="I40" s="34" t="s">
-        <v>19</v>
-      </c>
-      <c r="J40" s="36"/>
-      <c r="K40" s="36"/>
-      <c r="L40" s="36"/>
-      <c r="M40" s="36"/>
-      <c r="N40" s="36"/>
-      <c r="O40" s="36"/>
-      <c r="P40" s="36"/>
-      <c r="Q40" s="37"/>
-      <c r="R40" s="37"/>
-      <c r="S40" s="37"/>
-      <c r="T40" s="37"/>
-      <c r="U40" s="37"/>
-      <c r="V40" s="37"/>
-      <c r="W40" s="37"/>
-      <c r="X40" s="37"/>
-      <c r="Y40" s="37"/>
-      <c r="Z40" s="37"/>
-      <c r="AA40" s="37"/>
-      <c r="AB40" s="37"/>
-    </row>
-    <row r="41" s="35" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="31" t="s">
+    <row r="39" s="26" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A39" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="B39" s="27" t="s">
         <v>89</v>
       </c>
-      <c r="B41" s="32" t="s">
+      <c r="C39" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="C41" s="35" t="s">
+      <c r="D39" s="23"/>
+      <c r="E39" s="28"/>
+      <c r="F39" s="28"/>
+      <c r="G39" s="24"/>
+      <c r="I39" s="23"/>
+      <c r="J39" s="29"/>
+      <c r="K39" s="29"/>
+      <c r="L39" s="29"/>
+      <c r="M39" s="29"/>
+      <c r="N39" s="29"/>
+      <c r="O39" s="29"/>
+      <c r="P39" s="29"/>
+      <c r="Q39" s="30"/>
+      <c r="R39" s="30"/>
+      <c r="S39" s="30"/>
+      <c r="T39" s="30"/>
+      <c r="U39" s="30"/>
+      <c r="V39" s="30"/>
+      <c r="W39" s="30"/>
+      <c r="X39" s="30"/>
+      <c r="Y39" s="30"/>
+      <c r="Z39" s="30"/>
+      <c r="AA39" s="30"/>
+      <c r="AB39" s="30"/>
+    </row>
+    <row r="40" s="26" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A40" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="D41" s="31"/>
-      <c r="E41" s="33" t="s">
-        <v>52</v>
-      </c>
-      <c r="F41" s="33" t="n">
-        <v>1</v>
-      </c>
-      <c r="G41" s="34"/>
-      <c r="I41" s="31" t="s">
-        <v>25</v>
-      </c>
-      <c r="J41" s="36"/>
-      <c r="K41" s="36"/>
-      <c r="L41" s="36"/>
-      <c r="M41" s="36"/>
-      <c r="N41" s="36"/>
-      <c r="O41" s="36"/>
-      <c r="P41" s="36"/>
-      <c r="Q41" s="37"/>
-      <c r="R41" s="37"/>
-      <c r="S41" s="37"/>
-      <c r="T41" s="37"/>
-      <c r="U41" s="37"/>
-      <c r="V41" s="37"/>
-      <c r="W41" s="37"/>
-      <c r="X41" s="37"/>
-      <c r="Y41" s="37"/>
-      <c r="Z41" s="37"/>
-      <c r="AA41" s="37"/>
-      <c r="AB41" s="37"/>
-    </row>
-    <row r="42" s="35" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="31" t="s">
-        <v>31</v>
-      </c>
-      <c r="B42" s="32" t="s">
-        <v>1</v>
-      </c>
-      <c r="C42" s="35" t="s">
+      <c r="B40" s="27" t="s">
         <v>92</v>
       </c>
-      <c r="D42" s="31"/>
-      <c r="E42" s="33"/>
-      <c r="F42" s="33"/>
-      <c r="G42" s="34"/>
-      <c r="I42" s="31" t="s">
-        <v>25</v>
-      </c>
-      <c r="J42" s="36"/>
-      <c r="K42" s="36"/>
-      <c r="L42" s="36"/>
-      <c r="M42" s="36"/>
-      <c r="N42" s="36"/>
-      <c r="O42" s="36"/>
-      <c r="P42" s="36"/>
-      <c r="Q42" s="37"/>
-      <c r="R42" s="37"/>
-      <c r="S42" s="37"/>
-      <c r="T42" s="37"/>
-      <c r="U42" s="37"/>
-      <c r="V42" s="37"/>
-      <c r="W42" s="37"/>
-      <c r="X42" s="37"/>
-      <c r="Y42" s="37"/>
-      <c r="Z42" s="37"/>
-      <c r="AA42" s="37"/>
-      <c r="AB42" s="37"/>
+      <c r="C40" s="27" t="s">
+        <v>93</v>
+      </c>
+      <c r="D40" s="23"/>
+      <c r="E40" s="28"/>
+      <c r="F40" s="28"/>
+      <c r="I40" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="J40" s="29"/>
+      <c r="K40" s="29"/>
+      <c r="L40" s="29"/>
+      <c r="M40" s="29"/>
+      <c r="N40" s="29"/>
+      <c r="O40" s="29"/>
+      <c r="P40" s="29"/>
+      <c r="Q40" s="30"/>
+      <c r="R40" s="30"/>
+      <c r="S40" s="30"/>
+      <c r="T40" s="30"/>
+      <c r="U40" s="30"/>
+      <c r="V40" s="30"/>
+      <c r="W40" s="30"/>
+      <c r="X40" s="30"/>
+      <c r="Y40" s="30"/>
+      <c r="Z40" s="30"/>
+      <c r="AA40" s="30"/>
+      <c r="AB40" s="30"/>
+    </row>
+    <row r="41" s="26" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A41" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="B41" s="27"/>
+      <c r="C41" s="27"/>
+      <c r="D41" s="23"/>
+      <c r="E41" s="28"/>
+      <c r="F41" s="28"/>
+      <c r="G41" s="24"/>
+      <c r="I41" s="23"/>
+      <c r="J41" s="29"/>
+      <c r="K41" s="29"/>
+      <c r="L41" s="29"/>
+      <c r="M41" s="29"/>
+      <c r="N41" s="29"/>
+      <c r="O41" s="29"/>
+      <c r="P41" s="29"/>
+      <c r="Q41" s="30"/>
+      <c r="R41" s="30"/>
+      <c r="S41" s="30"/>
+      <c r="T41" s="30"/>
+      <c r="U41" s="30"/>
+      <c r="V41" s="30"/>
+      <c r="W41" s="30"/>
+      <c r="X41" s="30"/>
+      <c r="Y41" s="30"/>
+      <c r="Z41" s="30"/>
+      <c r="AA41" s="30"/>
+      <c r="AB41" s="30"/>
     </row>
     <row r="43" s="35" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="31" t="s">
-        <v>82</v>
+        <v>16</v>
       </c>
       <c r="B43" s="32" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C43" s="32" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D43" s="31"/>
       <c r="E43" s="33"/>
       <c r="F43" s="33"/>
-      <c r="I43" s="31" t="s">
-        <v>85</v>
+      <c r="G43" s="34" t="s">
+        <v>97</v>
+      </c>
+      <c r="I43" s="34" t="s">
+        <v>19</v>
       </c>
       <c r="J43" s="36"/>
       <c r="K43" s="36"/>
@@ -2378,24 +2359,22 @@
     </row>
     <row r="44" s="35" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="31" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B44" s="32" t="s">
-        <v>96</v>
-      </c>
-      <c r="C44" s="32" t="s">
-        <v>97</v>
+        <v>99</v>
+      </c>
+      <c r="C44" s="35" t="s">
+        <v>100</v>
       </c>
       <c r="D44" s="31"/>
       <c r="E44" s="33" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="F44" s="33" t="n">
-        <v>0</v>
-      </c>
-      <c r="G44" s="34" t="s">
-        <v>99</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="G44" s="34"/>
       <c r="I44" s="31" t="s">
         <v>25</v>
       </c>
@@ -2420,16 +2399,22 @@
       <c r="AB44" s="37"/>
     </row>
     <row r="45" s="35" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="37" t="s">
-        <v>34</v>
-      </c>
-      <c r="B45" s="32"/>
-      <c r="C45" s="32"/>
+      <c r="A45" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="B45" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="C45" s="35" t="s">
+        <v>101</v>
+      </c>
       <c r="D45" s="31"/>
-      <c r="E45" s="31"/>
-      <c r="F45" s="31"/>
-      <c r="G45" s="31"/>
-      <c r="I45" s="31"/>
+      <c r="E45" s="33"/>
+      <c r="F45" s="33"/>
+      <c r="G45" s="34"/>
+      <c r="I45" s="31" t="s">
+        <v>25</v>
+      </c>
       <c r="J45" s="36"/>
       <c r="K45" s="36"/>
       <c r="L45" s="36"/>
@@ -2450,371 +2435,369 @@
       <c r="AA45" s="37"/>
       <c r="AB45" s="37"/>
     </row>
-    <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B46" s="38"/>
-      <c r="C46" s="38"/>
-      <c r="G46" s="9"/>
-      <c r="J46" s="39"/>
-      <c r="K46" s="39"/>
-      <c r="L46" s="39"/>
-      <c r="M46" s="39"/>
-      <c r="N46" s="39"/>
-      <c r="O46" s="39"/>
-      <c r="P46" s="39"/>
-      <c r="Q46" s="40"/>
-      <c r="R46" s="40"/>
-      <c r="S46" s="40"/>
-      <c r="T46" s="40"/>
-      <c r="U46" s="40"/>
-      <c r="V46" s="40"/>
-      <c r="W46" s="40"/>
-      <c r="X46" s="40"/>
-      <c r="Y46" s="40"/>
-      <c r="Z46" s="40"/>
-      <c r="AA46" s="40"/>
-      <c r="AB46" s="40"/>
-    </row>
-    <row r="47" s="41" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="20" t="s">
+    <row r="46" s="35" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A46" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="B46" s="32" t="s">
+        <v>102</v>
+      </c>
+      <c r="C46" s="32" t="s">
+        <v>103</v>
+      </c>
+      <c r="D46" s="31"/>
+      <c r="E46" s="33"/>
+      <c r="F46" s="33"/>
+      <c r="I46" s="31" t="s">
+        <v>94</v>
+      </c>
+      <c r="J46" s="36"/>
+      <c r="K46" s="36"/>
+      <c r="L46" s="36"/>
+      <c r="M46" s="36"/>
+      <c r="N46" s="36"/>
+      <c r="O46" s="36"/>
+      <c r="P46" s="36"/>
+      <c r="Q46" s="37"/>
+      <c r="R46" s="37"/>
+      <c r="S46" s="37"/>
+      <c r="T46" s="37"/>
+      <c r="U46" s="37"/>
+      <c r="V46" s="37"/>
+      <c r="W46" s="37"/>
+      <c r="X46" s="37"/>
+      <c r="Y46" s="37"/>
+      <c r="Z46" s="37"/>
+      <c r="AA46" s="37"/>
+      <c r="AB46" s="37"/>
+    </row>
+    <row r="47" s="35" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A47" s="31" t="s">
+        <v>104</v>
+      </c>
+      <c r="B47" s="32" t="s">
+        <v>105</v>
+      </c>
+      <c r="C47" s="32" t="s">
+        <v>106</v>
+      </c>
+      <c r="D47" s="31"/>
+      <c r="E47" s="33" t="s">
+        <v>107</v>
+      </c>
+      <c r="F47" s="33" t="n">
+        <v>0</v>
+      </c>
+      <c r="G47" s="34" t="s">
+        <v>108</v>
+      </c>
+      <c r="I47" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="J47" s="36"/>
+      <c r="K47" s="36"/>
+      <c r="L47" s="36"/>
+      <c r="M47" s="36"/>
+      <c r="N47" s="36"/>
+      <c r="O47" s="36"/>
+      <c r="P47" s="36"/>
+      <c r="Q47" s="37"/>
+      <c r="R47" s="37"/>
+      <c r="S47" s="37"/>
+      <c r="T47" s="37"/>
+      <c r="U47" s="37"/>
+      <c r="V47" s="37"/>
+      <c r="W47" s="37"/>
+      <c r="X47" s="37"/>
+      <c r="Y47" s="37"/>
+      <c r="Z47" s="37"/>
+      <c r="AA47" s="37"/>
+      <c r="AB47" s="37"/>
+    </row>
+    <row r="48" s="35" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A48" s="37" t="s">
+        <v>38</v>
+      </c>
+      <c r="B48" s="32"/>
+      <c r="C48" s="32"/>
+      <c r="D48" s="31"/>
+      <c r="E48" s="31"/>
+      <c r="F48" s="31"/>
+      <c r="G48" s="31"/>
+      <c r="I48" s="31"/>
+      <c r="J48" s="36"/>
+      <c r="K48" s="36"/>
+      <c r="L48" s="36"/>
+      <c r="M48" s="36"/>
+      <c r="N48" s="36"/>
+      <c r="O48" s="36"/>
+      <c r="P48" s="36"/>
+      <c r="Q48" s="37"/>
+      <c r="R48" s="37"/>
+      <c r="S48" s="37"/>
+      <c r="T48" s="37"/>
+      <c r="U48" s="37"/>
+      <c r="V48" s="37"/>
+      <c r="W48" s="37"/>
+      <c r="X48" s="37"/>
+      <c r="Y48" s="37"/>
+      <c r="Z48" s="37"/>
+      <c r="AA48" s="37"/>
+      <c r="AB48" s="37"/>
+    </row>
+    <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B49" s="38"/>
+      <c r="C49" s="38"/>
+      <c r="G49" s="9"/>
+      <c r="J49" s="39"/>
+      <c r="K49" s="39"/>
+      <c r="L49" s="39"/>
+      <c r="M49" s="39"/>
+      <c r="N49" s="39"/>
+      <c r="O49" s="39"/>
+      <c r="P49" s="39"/>
+      <c r="Q49" s="40"/>
+      <c r="R49" s="40"/>
+      <c r="S49" s="40"/>
+      <c r="T49" s="40"/>
+      <c r="U49" s="40"/>
+      <c r="V49" s="40"/>
+      <c r="W49" s="40"/>
+      <c r="X49" s="40"/>
+      <c r="Y49" s="40"/>
+      <c r="Z49" s="40"/>
+      <c r="AA49" s="40"/>
+      <c r="AB49" s="40"/>
+    </row>
+    <row r="50" s="41" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B47" s="20" t="s">
-        <v>100</v>
-      </c>
-      <c r="C47" s="20" t="s">
-        <v>101</v>
-      </c>
-      <c r="D47" s="20"/>
-      <c r="E47" s="21"/>
-      <c r="F47" s="21"/>
-      <c r="G47" s="20" t="s">
-        <v>102</v>
-      </c>
-      <c r="H47" s="20"/>
-      <c r="I47" s="20" t="s">
+      <c r="B50" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="C50" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="D50" s="20"/>
+      <c r="E50" s="21"/>
+      <c r="F50" s="21"/>
+      <c r="G50" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="H50" s="20"/>
+      <c r="I50" s="20" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="48" s="41" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="20" t="s">
-        <v>103</v>
-      </c>
-      <c r="B48" s="20" t="s">
-        <v>104</v>
-      </c>
-      <c r="C48" s="20" t="s">
-        <v>105</v>
-      </c>
-      <c r="D48" s="20"/>
-      <c r="E48" s="21" t="s">
-        <v>106</v>
-      </c>
-      <c r="F48" s="21" t="n">
+    <row r="51" s="41" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="B51" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="C51" s="20" t="s">
+        <v>114</v>
+      </c>
+      <c r="D51" s="20"/>
+      <c r="E51" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="F51" s="21" t="n">
         <v>1</v>
       </c>
-      <c r="G48" s="20"/>
-      <c r="H48" s="20"/>
-      <c r="I48" s="20"/>
-    </row>
-    <row r="49" s="41" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A49" s="42" t="s">
-        <v>82</v>
-      </c>
-      <c r="B49" s="43" t="s">
-        <v>107</v>
-      </c>
-      <c r="C49" s="43" t="s">
-        <v>108</v>
-      </c>
-      <c r="D49" s="42" t="s">
-        <v>109</v>
-      </c>
-      <c r="E49" s="44"/>
-      <c r="F49" s="44"/>
-      <c r="G49" s="20" t="s">
-        <v>110</v>
-      </c>
-      <c r="I49" s="42" t="s">
-        <v>85</v>
-      </c>
-      <c r="J49" s="45"/>
-      <c r="K49" s="45"/>
-      <c r="L49" s="45"/>
-      <c r="M49" s="45"/>
-      <c r="N49" s="45"/>
-      <c r="O49" s="45"/>
-      <c r="P49" s="45"/>
-      <c r="Q49" s="46"/>
-      <c r="R49" s="46"/>
-      <c r="S49" s="46"/>
-      <c r="T49" s="46"/>
-      <c r="U49" s="46"/>
-      <c r="V49" s="46"/>
-      <c r="W49" s="46"/>
-      <c r="X49" s="46"/>
-      <c r="Y49" s="46"/>
-      <c r="Z49" s="46"/>
-      <c r="AA49" s="46"/>
-      <c r="AB49" s="46"/>
-    </row>
-    <row r="50" s="41" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A50" s="42" t="s">
-        <v>111</v>
-      </c>
-      <c r="B50" s="43" t="s">
-        <v>112</v>
-      </c>
-      <c r="C50" s="43" t="s">
-        <v>113</v>
-      </c>
-      <c r="D50" s="42"/>
-      <c r="E50" s="44"/>
-      <c r="F50" s="44"/>
-      <c r="G50" s="20" t="s">
-        <v>114</v>
-      </c>
-      <c r="I50" s="42"/>
-      <c r="J50" s="45"/>
-      <c r="K50" s="45"/>
-      <c r="L50" s="45"/>
-      <c r="M50" s="45"/>
-      <c r="N50" s="45"/>
-      <c r="O50" s="45"/>
-      <c r="P50" s="45"/>
-      <c r="Q50" s="46"/>
-      <c r="R50" s="46"/>
-      <c r="S50" s="46"/>
-      <c r="T50" s="46"/>
-      <c r="U50" s="46"/>
-      <c r="V50" s="46"/>
-      <c r="W50" s="46"/>
-      <c r="X50" s="46"/>
-      <c r="Y50" s="46"/>
-      <c r="Z50" s="46"/>
-      <c r="AA50" s="46"/>
-      <c r="AB50" s="46"/>
-    </row>
-    <row r="51" s="41" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A51" s="46" t="s">
-        <v>34</v>
-      </c>
-      <c r="B51" s="43"/>
-      <c r="C51" s="43"/>
-      <c r="D51" s="42"/>
-      <c r="E51" s="44"/>
-      <c r="F51" s="44"/>
-      <c r="I51" s="42"/>
-      <c r="J51" s="45"/>
-      <c r="K51" s="45"/>
-      <c r="L51" s="45"/>
-      <c r="M51" s="45"/>
-      <c r="N51" s="45"/>
-      <c r="O51" s="45"/>
-      <c r="P51" s="45"/>
-      <c r="Q51" s="46"/>
-      <c r="R51" s="46"/>
-      <c r="S51" s="46"/>
-      <c r="T51" s="46"/>
-      <c r="U51" s="46"/>
-      <c r="V51" s="46"/>
-      <c r="W51" s="46"/>
-      <c r="X51" s="46"/>
-      <c r="Y51" s="46"/>
-      <c r="Z51" s="46"/>
-      <c r="AA51" s="46"/>
-      <c r="AB51" s="46"/>
-    </row>
-    <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B52" s="38"/>
-      <c r="C52" s="38"/>
-      <c r="J52" s="39"/>
-      <c r="K52" s="39"/>
-      <c r="L52" s="39"/>
-      <c r="M52" s="39"/>
-      <c r="N52" s="39"/>
-      <c r="O52" s="39"/>
-      <c r="P52" s="39"/>
-      <c r="Q52" s="40"/>
-      <c r="R52" s="40"/>
-      <c r="S52" s="40"/>
-      <c r="T52" s="40"/>
-      <c r="U52" s="40"/>
-      <c r="V52" s="40"/>
-      <c r="W52" s="40"/>
-      <c r="X52" s="40"/>
-      <c r="Y52" s="40"/>
-      <c r="Z52" s="40"/>
-      <c r="AA52" s="40"/>
-      <c r="AB52" s="40"/>
-    </row>
-    <row r="53" s="51" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A53" s="47" t="s">
+      <c r="G51" s="20"/>
+      <c r="H51" s="20"/>
+      <c r="I51" s="20"/>
+    </row>
+    <row r="52" s="41" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A52" s="42" t="s">
+        <v>91</v>
+      </c>
+      <c r="B52" s="43" t="s">
+        <v>116</v>
+      </c>
+      <c r="C52" s="43" t="s">
+        <v>117</v>
+      </c>
+      <c r="D52" s="42" t="s">
+        <v>118</v>
+      </c>
+      <c r="E52" s="44"/>
+      <c r="F52" s="44"/>
+      <c r="G52" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="I52" s="42" t="s">
+        <v>94</v>
+      </c>
+      <c r="J52" s="45"/>
+      <c r="K52" s="45"/>
+      <c r="L52" s="45"/>
+      <c r="M52" s="45"/>
+      <c r="N52" s="45"/>
+      <c r="O52" s="45"/>
+      <c r="P52" s="45"/>
+      <c r="Q52" s="46"/>
+      <c r="R52" s="46"/>
+      <c r="S52" s="46"/>
+      <c r="T52" s="46"/>
+      <c r="U52" s="46"/>
+      <c r="V52" s="46"/>
+      <c r="W52" s="46"/>
+      <c r="X52" s="46"/>
+      <c r="Y52" s="46"/>
+      <c r="Z52" s="46"/>
+      <c r="AA52" s="46"/>
+      <c r="AB52" s="46"/>
+    </row>
+    <row r="53" s="41" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A53" s="42" t="s">
+        <v>120</v>
+      </c>
+      <c r="B53" s="43" t="s">
+        <v>121</v>
+      </c>
+      <c r="C53" s="43" t="s">
+        <v>122</v>
+      </c>
+      <c r="D53" s="42"/>
+      <c r="E53" s="44"/>
+      <c r="F53" s="44"/>
+      <c r="G53" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="I53" s="42"/>
+      <c r="J53" s="45"/>
+      <c r="K53" s="45"/>
+      <c r="L53" s="45"/>
+      <c r="M53" s="45"/>
+      <c r="N53" s="45"/>
+      <c r="O53" s="45"/>
+      <c r="P53" s="45"/>
+      <c r="Q53" s="46"/>
+      <c r="R53" s="46"/>
+      <c r="S53" s="46"/>
+      <c r="T53" s="46"/>
+      <c r="U53" s="46"/>
+      <c r="V53" s="46"/>
+      <c r="W53" s="46"/>
+      <c r="X53" s="46"/>
+      <c r="Y53" s="46"/>
+      <c r="Z53" s="46"/>
+      <c r="AA53" s="46"/>
+      <c r="AB53" s="46"/>
+    </row>
+    <row r="54" s="41" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A54" s="46" t="s">
+        <v>38</v>
+      </c>
+      <c r="B54" s="43"/>
+      <c r="C54" s="43"/>
+      <c r="D54" s="42"/>
+      <c r="E54" s="44"/>
+      <c r="F54" s="44"/>
+      <c r="I54" s="42"/>
+      <c r="J54" s="45"/>
+      <c r="K54" s="45"/>
+      <c r="L54" s="45"/>
+      <c r="M54" s="45"/>
+      <c r="N54" s="45"/>
+      <c r="O54" s="45"/>
+      <c r="P54" s="45"/>
+      <c r="Q54" s="46"/>
+      <c r="R54" s="46"/>
+      <c r="S54" s="46"/>
+      <c r="T54" s="46"/>
+      <c r="U54" s="46"/>
+      <c r="V54" s="46"/>
+      <c r="W54" s="46"/>
+      <c r="X54" s="46"/>
+      <c r="Y54" s="46"/>
+      <c r="Z54" s="46"/>
+      <c r="AA54" s="46"/>
+      <c r="AB54" s="46"/>
+    </row>
+    <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B55" s="38"/>
+      <c r="C55" s="38"/>
+      <c r="J55" s="39"/>
+      <c r="K55" s="39"/>
+      <c r="L55" s="39"/>
+      <c r="M55" s="39"/>
+      <c r="N55" s="39"/>
+      <c r="O55" s="39"/>
+      <c r="P55" s="39"/>
+      <c r="Q55" s="40"/>
+      <c r="R55" s="40"/>
+      <c r="S55" s="40"/>
+      <c r="T55" s="40"/>
+      <c r="U55" s="40"/>
+      <c r="V55" s="40"/>
+      <c r="W55" s="40"/>
+      <c r="X55" s="40"/>
+      <c r="Y55" s="40"/>
+      <c r="Z55" s="40"/>
+      <c r="AA55" s="40"/>
+      <c r="AB55" s="40"/>
+    </row>
+    <row r="56" s="51" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A56" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="B53" s="47" t="s">
-        <v>115</v>
-      </c>
-      <c r="C53" s="48" t="s">
-        <v>116</v>
-      </c>
-      <c r="D53" s="48"/>
-      <c r="E53" s="49"/>
-      <c r="F53" s="50"/>
-      <c r="G53" s="47"/>
-      <c r="H53" s="47"/>
-      <c r="I53" s="47" t="s">
+      <c r="B56" s="47" t="s">
+        <v>124</v>
+      </c>
+      <c r="C56" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="D56" s="48"/>
+      <c r="E56" s="49"/>
+      <c r="F56" s="50"/>
+      <c r="G56" s="47"/>
+      <c r="H56" s="47"/>
+      <c r="I56" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="J53" s="47"/>
-      <c r="K53" s="47"/>
-      <c r="L53" s="47"/>
-      <c r="M53" s="47"/>
-      <c r="N53" s="47"/>
-      <c r="O53" s="47"/>
-      <c r="P53" s="47"/>
-      <c r="Q53" s="47"/>
-      <c r="R53" s="47"/>
-      <c r="S53" s="47"/>
-      <c r="T53" s="47"/>
-      <c r="U53" s="47"/>
-      <c r="V53" s="47"/>
-      <c r="W53" s="47"/>
-      <c r="X53" s="47"/>
-      <c r="Y53" s="47"/>
-      <c r="Z53" s="47"/>
-      <c r="AA53" s="47"/>
-      <c r="AB53" s="47"/>
-    </row>
-    <row r="54" s="51" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A54" s="47" t="s">
-        <v>31</v>
-      </c>
-      <c r="B54" s="52" t="s">
-        <v>117</v>
-      </c>
-      <c r="C54" s="52" t="s">
-        <v>118</v>
-      </c>
-      <c r="D54" s="47"/>
-      <c r="E54" s="50"/>
-      <c r="F54" s="50"/>
-      <c r="G54" s="47"/>
-      <c r="H54" s="47"/>
-      <c r="I54" s="47" t="s">
-        <v>25</v>
-      </c>
-      <c r="J54" s="47"/>
-      <c r="K54" s="47"/>
-      <c r="L54" s="47"/>
-      <c r="M54" s="47"/>
-      <c r="N54" s="47"/>
-      <c r="O54" s="47"/>
-      <c r="P54" s="47"/>
-      <c r="Q54" s="47"/>
-      <c r="R54" s="47"/>
-      <c r="S54" s="47"/>
-      <c r="T54" s="47"/>
-      <c r="U54" s="47"/>
-      <c r="V54" s="47"/>
-      <c r="W54" s="47"/>
-      <c r="X54" s="47"/>
-      <c r="Y54" s="47"/>
-      <c r="Z54" s="47"/>
-      <c r="AA54" s="47"/>
-      <c r="AB54" s="47"/>
-    </row>
-    <row r="55" s="51" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A55" s="53" t="s">
-        <v>119</v>
-      </c>
-      <c r="B55" s="53" t="s">
-        <v>119</v>
-      </c>
-      <c r="C55" s="54" t="s">
-        <v>120</v>
-      </c>
-      <c r="D55" s="53"/>
-      <c r="E55" s="55"/>
-      <c r="F55" s="55"/>
-      <c r="G55" s="56"/>
-      <c r="H55" s="56"/>
-      <c r="I55" s="47" t="s">
-        <v>25</v>
-      </c>
-      <c r="J55" s="57" t="s">
-        <v>121</v>
-      </c>
-      <c r="K55" s="58"/>
-      <c r="L55" s="58"/>
-      <c r="M55" s="58"/>
-      <c r="N55" s="58"/>
-      <c r="O55" s="58"/>
-      <c r="P55" s="58"/>
-      <c r="Q55" s="58"/>
-      <c r="R55" s="58"/>
-      <c r="S55" s="58"/>
-      <c r="T55" s="58"/>
-      <c r="U55" s="58"/>
-      <c r="V55" s="58"/>
-      <c r="W55" s="58"/>
-      <c r="X55" s="58"/>
-      <c r="Y55" s="58"/>
-      <c r="Z55" s="58"/>
-      <c r="AA55" s="58"/>
-      <c r="AB55" s="58"/>
-    </row>
-    <row r="56" s="51" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A56" s="53" t="s">
-        <v>122</v>
-      </c>
-      <c r="B56" s="53" t="s">
-        <v>122</v>
-      </c>
-      <c r="C56" s="54" t="s">
-        <v>123</v>
-      </c>
-      <c r="D56" s="53"/>
-      <c r="E56" s="55"/>
-      <c r="F56" s="55"/>
-      <c r="G56" s="56"/>
-      <c r="H56" s="56"/>
-      <c r="I56" s="47" t="s">
-        <v>25</v>
-      </c>
-      <c r="J56" s="57" t="s">
-        <v>124</v>
-      </c>
-      <c r="K56" s="58"/>
-      <c r="L56" s="58"/>
-      <c r="M56" s="58"/>
-      <c r="N56" s="58"/>
-      <c r="O56" s="58"/>
-      <c r="P56" s="58"/>
-      <c r="Q56" s="58"/>
-      <c r="R56" s="58"/>
-      <c r="S56" s="58"/>
-      <c r="T56" s="58"/>
-      <c r="U56" s="58"/>
-      <c r="V56" s="58"/>
-      <c r="W56" s="58"/>
-      <c r="X56" s="58"/>
-      <c r="Y56" s="58"/>
-      <c r="Z56" s="58"/>
-      <c r="AA56" s="58"/>
-      <c r="AB56" s="58"/>
+      <c r="J56" s="47"/>
+      <c r="K56" s="47"/>
+      <c r="L56" s="47"/>
+      <c r="M56" s="47"/>
+      <c r="N56" s="47"/>
+      <c r="O56" s="47"/>
+      <c r="P56" s="47"/>
+      <c r="Q56" s="47"/>
+      <c r="R56" s="47"/>
+      <c r="S56" s="47"/>
+      <c r="T56" s="47"/>
+      <c r="U56" s="47"/>
+      <c r="V56" s="47"/>
+      <c r="W56" s="47"/>
+      <c r="X56" s="47"/>
+      <c r="Y56" s="47"/>
+      <c r="Z56" s="47"/>
+      <c r="AA56" s="47"/>
+      <c r="AB56" s="47"/>
     </row>
     <row r="57" s="51" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="47" t="s">
-        <v>34</v>
-      </c>
-      <c r="B57" s="47"/>
-      <c r="C57" s="47"/>
+        <v>31</v>
+      </c>
+      <c r="B57" s="52" t="s">
+        <v>126</v>
+      </c>
+      <c r="C57" s="52" t="s">
+        <v>127</v>
+      </c>
       <c r="D57" s="47"/>
       <c r="E57" s="50"/>
       <c r="F57" s="50"/>
       <c r="G57" s="47"/>
       <c r="H57" s="47"/>
-      <c r="I57" s="47"/>
+      <c r="I57" s="47" t="s">
+        <v>25</v>
+      </c>
       <c r="J57" s="47"/>
       <c r="K57" s="47"/>
       <c r="L57" s="47"/>
@@ -2835,15 +2818,129 @@
       <c r="AA57" s="47"/>
       <c r="AB57" s="47"/>
     </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="0" t="s">
-        <v>34</v>
+    <row r="58" s="51" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A58" s="53" t="s">
+        <v>128</v>
+      </c>
+      <c r="B58" s="53" t="s">
+        <v>128</v>
+      </c>
+      <c r="C58" s="54" t="s">
+        <v>129</v>
+      </c>
+      <c r="D58" s="53"/>
+      <c r="E58" s="55"/>
+      <c r="F58" s="55"/>
+      <c r="G58" s="56"/>
+      <c r="H58" s="56"/>
+      <c r="I58" s="47" t="s">
+        <v>25</v>
+      </c>
+      <c r="J58" s="57" t="s">
+        <v>130</v>
+      </c>
+      <c r="K58" s="58"/>
+      <c r="L58" s="58"/>
+      <c r="M58" s="58"/>
+      <c r="N58" s="58"/>
+      <c r="O58" s="58"/>
+      <c r="P58" s="58"/>
+      <c r="Q58" s="58"/>
+      <c r="R58" s="58"/>
+      <c r="S58" s="58"/>
+      <c r="T58" s="58"/>
+      <c r="U58" s="58"/>
+      <c r="V58" s="58"/>
+      <c r="W58" s="58"/>
+      <c r="X58" s="58"/>
+      <c r="Y58" s="58"/>
+      <c r="Z58" s="58"/>
+      <c r="AA58" s="58"/>
+      <c r="AB58" s="58"/>
+    </row>
+    <row r="59" s="51" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A59" s="53" t="s">
+        <v>131</v>
+      </c>
+      <c r="B59" s="53" t="s">
+        <v>131</v>
+      </c>
+      <c r="C59" s="54" t="s">
+        <v>132</v>
+      </c>
+      <c r="D59" s="53"/>
+      <c r="E59" s="55"/>
+      <c r="F59" s="55"/>
+      <c r="G59" s="56"/>
+      <c r="H59" s="56" t="s">
+        <v>133</v>
+      </c>
+      <c r="I59" s="47" t="s">
+        <v>25</v>
+      </c>
+      <c r="J59" s="57" t="s">
+        <v>134</v>
+      </c>
+      <c r="K59" s="58"/>
+      <c r="L59" s="58"/>
+      <c r="M59" s="58"/>
+      <c r="N59" s="58"/>
+      <c r="O59" s="58"/>
+      <c r="P59" s="58"/>
+      <c r="Q59" s="58"/>
+      <c r="R59" s="58"/>
+      <c r="S59" s="58"/>
+      <c r="T59" s="58"/>
+      <c r="U59" s="58"/>
+      <c r="V59" s="58"/>
+      <c r="W59" s="58"/>
+      <c r="X59" s="58"/>
+      <c r="Y59" s="58"/>
+      <c r="Z59" s="58"/>
+      <c r="AA59" s="58"/>
+      <c r="AB59" s="58"/>
+    </row>
+    <row r="60" s="51" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A60" s="47" t="s">
+        <v>38</v>
+      </c>
+      <c r="B60" s="47"/>
+      <c r="C60" s="47"/>
+      <c r="D60" s="47"/>
+      <c r="E60" s="50"/>
+      <c r="F60" s="50"/>
+      <c r="G60" s="47"/>
+      <c r="H60" s="47"/>
+      <c r="I60" s="47"/>
+      <c r="J60" s="47"/>
+      <c r="K60" s="47"/>
+      <c r="L60" s="47"/>
+      <c r="M60" s="47"/>
+      <c r="N60" s="47"/>
+      <c r="O60" s="47"/>
+      <c r="P60" s="47"/>
+      <c r="Q60" s="47"/>
+      <c r="R60" s="47"/>
+      <c r="S60" s="47"/>
+      <c r="T60" s="47"/>
+      <c r="U60" s="47"/>
+      <c r="V60" s="47"/>
+      <c r="W60" s="47"/>
+      <c r="X60" s="47"/>
+      <c r="Y60" s="47"/>
+      <c r="Z60" s="47"/>
+      <c r="AA60" s="47"/>
+      <c r="AB60" s="47"/>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="0" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2859,18 +2956,18 @@
   <dimension ref="A1:Z119"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A97" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C120" activeCellId="0" sqref="C120"/>
+      <selection pane="topLeft" activeCell="B116" activeCellId="0" sqref="B116"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.72"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>125</v>
+        <v>135</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -2907,10 +3004,10 @@
         <v>23</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D2" s="60"/>
     </row>
@@ -2919,10 +3016,10 @@
         <v>23</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>127</v>
+        <v>137</v>
       </c>
       <c r="D3" s="60"/>
     </row>
@@ -2931,10 +3028,10 @@
         <v>23</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="D4" s="60"/>
     </row>
@@ -2943,10 +3040,10 @@
         <v>23</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>129</v>
+        <v>139</v>
       </c>
       <c r="D5" s="60"/>
     </row>
@@ -2955,10 +3052,10 @@
         <v>27</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
       <c r="D7" s="60"/>
     </row>
@@ -2967,10 +3064,10 @@
         <v>27</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>132</v>
+        <v>142</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>133</v>
+        <v>143</v>
       </c>
       <c r="D8" s="60"/>
     </row>
@@ -2979,10 +3076,10 @@
         <v>27</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>134</v>
+        <v>144</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>135</v>
+        <v>145</v>
       </c>
       <c r="D9" s="60"/>
     </row>
@@ -2991,10 +3088,10 @@
         <v>27</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>136</v>
+        <v>146</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
       <c r="D10" s="60"/>
     </row>
@@ -3003,10 +3100,10 @@
         <v>27</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>138</v>
+        <v>148</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="D11" s="60"/>
     </row>
@@ -3018,7 +3115,7 @@
         <v>29</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>140</v>
+        <v>150</v>
       </c>
       <c r="D12" s="60"/>
     </row>
@@ -3027,10 +3124,10 @@
         <v>27</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>141</v>
+        <v>151</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>142</v>
+        <v>152</v>
       </c>
       <c r="D13" s="60"/>
     </row>
@@ -3039,10 +3136,10 @@
         <v>27</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>127</v>
+        <v>137</v>
       </c>
       <c r="D14" s="60"/>
     </row>
@@ -3051,10 +3148,10 @@
         <v>27</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>143</v>
+        <v>153</v>
       </c>
       <c r="D15" s="60"/>
     </row>
@@ -3066,25 +3163,25 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="9" t="s">
-        <v>144</v>
+        <v>154</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>52</v>
+        <v>88</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>145</v>
+        <v>155</v>
       </c>
       <c r="D17" s="60"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="9" t="s">
-        <v>144</v>
+        <v>154</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>146</v>
+        <v>53</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>147</v>
+        <v>156</v>
       </c>
       <c r="D18" s="60"/>
     </row>
@@ -3096,145 +3193,145 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="9" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>148</v>
+        <v>157</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>149</v>
+        <v>158</v>
       </c>
       <c r="D20" s="60"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="9" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>150</v>
+        <v>159</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>151</v>
+        <v>160</v>
       </c>
       <c r="D21" s="60"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="9" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>152</v>
+        <v>161</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>153</v>
+        <v>162</v>
       </c>
       <c r="D22" s="60"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="9" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>40</v>
+        <v>163</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
       <c r="D23" s="60"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="9" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>155</v>
+        <v>165</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
       <c r="D24" s="60"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="9" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>157</v>
+        <v>167</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>158</v>
+        <v>168</v>
       </c>
       <c r="D25" s="60"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="9" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>159</v>
+        <v>169</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>160</v>
+        <v>170</v>
       </c>
       <c r="D26" s="60"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="9" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>161</v>
+        <v>171</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>162</v>
+        <v>172</v>
       </c>
       <c r="D27" s="60"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="9" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>163</v>
+        <v>44</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="D28" s="60"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="9" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>165</v>
+        <v>174</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>166</v>
+        <v>175</v>
       </c>
       <c r="D29" s="60"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="9" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>167</v>
+        <v>176</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>168</v>
+        <v>177</v>
       </c>
       <c r="D30" s="60"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="9" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>169</v>
+        <v>178</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="D31" s="60"/>
     </row>
@@ -3246,73 +3343,73 @@
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="9" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>44</v>
+        <v>180</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>171</v>
+        <v>181</v>
       </c>
       <c r="D33" s="60"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="9" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>172</v>
+        <v>81</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>173</v>
+        <v>182</v>
       </c>
       <c r="D34" s="60"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="9" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>174</v>
+        <v>48</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>175</v>
+        <v>183</v>
       </c>
       <c r="D35" s="60"/>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="9" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>176</v>
+        <v>184</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
       <c r="D36" s="60"/>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="9" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>178</v>
+        <v>186</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="D37" s="60"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="9" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="D38" s="60"/>
     </row>
@@ -3324,25 +3421,25 @@
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="9" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>52</v>
+        <v>88</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>52</v>
+        <v>88</v>
       </c>
       <c r="D40" s="60"/>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="9" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>146</v>
+        <v>53</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>146</v>
+        <v>53</v>
       </c>
       <c r="D41" s="60"/>
     </row>
@@ -3354,37 +3451,37 @@
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="9" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>52</v>
+        <v>88</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>52</v>
+        <v>88</v>
       </c>
       <c r="D43" s="60"/>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="9" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>146</v>
+        <v>53</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>146</v>
+        <v>53</v>
       </c>
       <c r="D44" s="60"/>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="9" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>183</v>
+        <v>191</v>
       </c>
       <c r="D45" s="60"/>
     </row>
@@ -3396,728 +3493,728 @@
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="9" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>184</v>
+        <v>192</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
       <c r="D47" s="60"/>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="9" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
       <c r="D48" s="60"/>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="9" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="D49" s="60"/>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="9" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>189</v>
+        <v>197</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="D50" s="60"/>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="9" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>192</v>
+        <v>200</v>
       </c>
       <c r="D51" s="60"/>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>193</v>
+        <v>201</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>194</v>
+        <v>202</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>195</v>
+        <v>64</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>196</v>
+        <v>203</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>197</v>
+        <v>204</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>198</v>
+        <v>205</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>199</v>
+        <v>206</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>201</v>
+        <v>208</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>203</v>
+        <v>210</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>204</v>
+        <v>211</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>203</v>
+        <v>210</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>207</v>
+        <v>214</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>203</v>
+        <v>210</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>208</v>
+        <v>215</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>209</v>
+        <v>216</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>203</v>
+        <v>210</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>210</v>
+        <v>217</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>203</v>
+        <v>210</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>146</v>
+        <v>53</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>212</v>
+        <v>219</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>203</v>
+        <v>210</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>52</v>
+        <v>88</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>145</v>
+        <v>155</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>213</v>
+        <v>220</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>106</v>
+        <v>115</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>215</v>
+        <v>222</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>216</v>
+        <v>223</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>217</v>
+        <v>224</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>218</v>
+        <v>225</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>219</v>
+        <v>226</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>220</v>
+        <v>227</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>221</v>
+        <v>228</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>222</v>
+        <v>229</v>
       </c>
       <c r="C74" s="0" t="s">
-        <v>223</v>
+        <v>230</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>224</v>
+        <v>231</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>225</v>
+        <v>232</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>226</v>
+        <v>233</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>227</v>
+        <v>234</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>228</v>
+        <v>235</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>229</v>
+        <v>236</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>230</v>
+        <v>237</v>
       </c>
       <c r="C78" s="0" t="s">
-        <v>231</v>
+        <v>238</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>232</v>
+        <v>239</v>
       </c>
       <c r="C79" s="0" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>234</v>
+        <v>241</v>
       </c>
       <c r="C80" s="0" t="s">
-        <v>235</v>
+        <v>242</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>52</v>
+        <v>88</v>
       </c>
       <c r="C81" s="0" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>237</v>
+        <v>244</v>
       </c>
       <c r="C83" s="0" t="s">
-        <v>238</v>
+        <v>245</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>239</v>
+        <v>246</v>
       </c>
       <c r="C84" s="0" t="s">
-        <v>240</v>
+        <v>247</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>241</v>
+        <v>248</v>
       </c>
       <c r="C85" s="0" t="s">
-        <v>242</v>
+        <v>249</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>243</v>
+        <v>250</v>
       </c>
       <c r="C86" s="0" t="s">
-        <v>244</v>
+        <v>251</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>245</v>
+        <v>252</v>
       </c>
       <c r="C87" s="0" t="s">
-        <v>246</v>
+        <v>253</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>247</v>
+        <v>254</v>
       </c>
       <c r="C88" s="0" t="s">
-        <v>248</v>
+        <v>255</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>249</v>
+        <v>256</v>
       </c>
       <c r="C89" s="0" t="s">
-        <v>250</v>
+        <v>257</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>251</v>
+        <v>258</v>
       </c>
       <c r="C90" s="0" t="s">
-        <v>252</v>
+        <v>259</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="B91" s="0" t="s">
-        <v>253</v>
+        <v>260</v>
       </c>
       <c r="C91" s="0" t="s">
-        <v>254</v>
+        <v>261</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="B92" s="0" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
       <c r="C92" s="0" t="s">
-        <v>256</v>
+        <v>263</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="B93" s="0" t="s">
-        <v>257</v>
+        <v>264</v>
       </c>
       <c r="C93" s="0" t="s">
-        <v>258</v>
+        <v>265</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="B94" s="0" t="s">
-        <v>259</v>
+        <v>266</v>
       </c>
       <c r="C94" s="0" t="s">
-        <v>260</v>
+        <v>267</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="B95" s="0" t="s">
-        <v>261</v>
+        <v>268</v>
       </c>
       <c r="C95" s="0" t="s">
-        <v>262</v>
+        <v>269</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="B96" s="0" t="s">
-        <v>263</v>
+        <v>270</v>
       </c>
       <c r="C96" s="0" t="s">
-        <v>264</v>
+        <v>271</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="B97" s="0" t="s">
-        <v>265</v>
+        <v>272</v>
       </c>
       <c r="C97" s="0" t="s">
-        <v>266</v>
+        <v>273</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="B98" s="0" t="s">
-        <v>267</v>
+        <v>274</v>
       </c>
       <c r="C98" s="0" t="s">
-        <v>268</v>
+        <v>275</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="B99" s="0" t="s">
-        <v>269</v>
+        <v>276</v>
       </c>
       <c r="C99" s="0" t="s">
-        <v>270</v>
+        <v>277</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="B100" s="0" t="s">
-        <v>271</v>
+        <v>278</v>
       </c>
       <c r="C100" s="0" t="s">
-        <v>272</v>
+        <v>279</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="B101" s="0" t="s">
-        <v>273</v>
+        <v>280</v>
       </c>
       <c r="C101" s="0" t="s">
-        <v>274</v>
+        <v>281</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="B102" s="0" t="s">
-        <v>275</v>
+        <v>282</v>
       </c>
       <c r="C102" s="0" t="s">
-        <v>276</v>
+        <v>283</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="B103" s="0" t="s">
-        <v>277</v>
+        <v>284</v>
       </c>
       <c r="C103" s="0" t="s">
-        <v>278</v>
+        <v>285</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="B104" s="0" t="s">
-        <v>52</v>
+        <v>88</v>
       </c>
       <c r="C104" s="0" t="s">
-        <v>279</v>
+        <v>286</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="B105" s="0" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="C105" s="0" t="s">
-        <v>280</v>
+        <v>287</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="B107" s="0" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="C107" s="0" t="s">
-        <v>281</v>
+        <v>288</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="B108" s="0" t="s">
-        <v>282</v>
+        <v>289</v>
       </c>
       <c r="C108" s="0" t="s">
-        <v>283</v>
+        <v>290</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="B109" s="0" t="s">
-        <v>284</v>
+        <v>291</v>
       </c>
       <c r="C109" s="0" t="s">
-        <v>285</v>
+        <v>292</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="B110" s="0" t="s">
-        <v>286</v>
+        <v>293</v>
       </c>
       <c r="C110" s="0" t="s">
-        <v>287</v>
+        <v>294</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="B111" s="0" t="s">
-        <v>288</v>
+        <v>295</v>
       </c>
       <c r="C111" s="0" t="s">
-        <v>289</v>
+        <v>296</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="B112" s="0" t="s">
-        <v>290</v>
+        <v>297</v>
       </c>
       <c r="C112" s="0" t="s">
-        <v>291</v>
+        <v>298</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="61" t="s">
-        <v>292</v>
+        <v>299</v>
       </c>
       <c r="B114" s="0" t="s">
-        <v>293</v>
+        <v>300</v>
       </c>
       <c r="C114" s="0" t="s">
-        <v>294</v>
+        <v>301</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="61" t="s">
-        <v>292</v>
+        <v>299</v>
       </c>
       <c r="B115" s="0" t="s">
-        <v>44</v>
+        <v>180</v>
       </c>
       <c r="C115" s="0" t="s">
-        <v>295</v>
+        <v>302</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="61" t="s">
-        <v>292</v>
+        <v>299</v>
       </c>
       <c r="B116" s="0" t="s">
-        <v>172</v>
+        <v>81</v>
       </c>
       <c r="C116" s="0" t="s">
-        <v>296</v>
+        <v>303</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="61" t="s">
-        <v>292</v>
+        <v>299</v>
       </c>
       <c r="B117" s="0" t="s">
-        <v>174</v>
+        <v>48</v>
       </c>
       <c r="C117" s="0" t="s">
-        <v>297</v>
+        <v>304</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="61" t="s">
-        <v>292</v>
+        <v>299</v>
       </c>
       <c r="B118" s="0" t="s">
-        <v>178</v>
+        <v>186</v>
       </c>
       <c r="C118" s="0" t="s">
-        <v>298</v>
+        <v>305</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="61" t="s">
-        <v>292</v>
+        <v>299</v>
       </c>
       <c r="B119" s="0" t="s">
-        <v>146</v>
+        <v>53</v>
       </c>
       <c r="C119" s="0" t="s">
-        <v>299</v>
+        <v>306</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -4136,32 +4233,32 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.36"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="62" t="s">
-        <v>300</v>
+        <v>307</v>
       </c>
       <c r="B1" s="62" t="s">
-        <v>301</v>
+        <v>308</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="63" t="n">
         <f aca="true">NOW()</f>
-        <v>44248.8522761246</v>
+        <v>44436.7284810393</v>
       </c>
       <c r="B2" s="64" t="s">
-        <v>302</v>
+        <v>309</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
change feature_type to highway_type
</commit_message>
<xml_diff>
--- a/XForms/highways.xlsx
+++ b/XForms/highways.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="306">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -90,10 +90,10 @@
     <t xml:space="preserve">Feature</t>
   </si>
   <si>
-    <t xml:space="preserve">select_one feature_type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">feature_type</t>
+    <t xml:space="preserve">select_one highway_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">highway_type</t>
   </si>
   <si>
     <t xml:space="preserve">What feature is this?</t>
@@ -102,10 +102,10 @@
     <t xml:space="preserve">minimal</t>
   </si>
   <si>
-    <t xml:space="preserve">select_one highway_type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">highway_type</t>
+    <t xml:space="preserve">select_one highway</t>
+  </si>
+  <si>
+    <t xml:space="preserve">highway</t>
   </si>
   <si>
     <t xml:space="preserve">What type of road is this?</t>
@@ -114,7 +114,7 @@
     <t xml:space="preserve">residential</t>
   </si>
   <si>
-    <t xml:space="preserve">${feature_type} = 'highway'</t>
+    <t xml:space="preserve">${highway_type} = 'highway'</t>
   </si>
   <si>
     <t xml:space="preserve">text</t>
@@ -129,9 +129,6 @@
     <t xml:space="preserve">end_group</t>
   </si>
   <si>
-    <t xml:space="preserve">highway</t>
-  </si>
-  <si>
     <t xml:space="preserve">Highway</t>
   </si>
   <si>
@@ -222,7 +219,7 @@
     <t xml:space="preserve">Path conditions</t>
   </si>
   <si>
-    <t xml:space="preserve">${feature_type} = 'path'</t>
+    <t xml:space="preserve">${highway_type} = 'path'</t>
   </si>
   <si>
     <t xml:space="preserve">select_one sac_scale</t>
@@ -252,7 +249,7 @@
     <t xml:space="preserve">Bridges</t>
   </si>
   <si>
-    <t xml:space="preserve">${feature_type} = 'bridge'</t>
+    <t xml:space="preserve">${highway_type} = 'bridge'</t>
   </si>
   <si>
     <t xml:space="preserve">select_one bridge_type</t>
@@ -288,7 +285,7 @@
     <t xml:space="preserve">Is there a barrier blocking this highway ?</t>
   </si>
   <si>
-    <t xml:space="preserve">${feature_type} = 'barrier'</t>
+    <t xml:space="preserve">${highway_type} = 'barrier'</t>
   </si>
   <si>
     <t xml:space="preserve">select_one barrier</t>
@@ -330,7 +327,7 @@
     <t xml:space="preserve">GPS Coordinates</t>
   </si>
   <si>
-    <t xml:space="preserve">${feature_type} = 'highway' or ${feature_type} = 'path'</t>
+    <t xml:space="preserve">${highway_type} = 'highway' or ${highway_type} = 'path'</t>
   </si>
   <si>
     <t xml:space="preserve">select_one gps_type</t>
@@ -1479,11 +1476,11 @@
   </sheetPr>
   <dimension ref="A1:AB60"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G26" activeCellId="0" sqref="G26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A21" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G34" activeCellId="0" sqref="G34 G40 G47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.79"/>
@@ -1795,10 +1792,10 @@
         <v>16</v>
       </c>
       <c r="B19" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="14" t="s">
         <v>35</v>
-      </c>
-      <c r="C19" s="14" t="s">
-        <v>36</v>
       </c>
       <c r="D19" s="14"/>
       <c r="E19" s="15"/>
@@ -1813,17 +1810,17 @@
     </row>
     <row r="20" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="C20" s="14" t="s">
         <v>38</v>
-      </c>
-      <c r="C20" s="14" t="s">
-        <v>39</v>
       </c>
       <c r="D20" s="14"/>
       <c r="E20" s="15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F20" s="15" t="n">
         <v>1</v>
@@ -1835,17 +1832,17 @@
     </row>
     <row r="21" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="B21" s="14" t="s">
+      <c r="C21" s="14" t="s">
         <v>42</v>
-      </c>
-      <c r="C21" s="14" t="s">
-        <v>43</v>
       </c>
       <c r="D21" s="14"/>
       <c r="E21" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F21" s="15" t="n">
         <v>1</v>
@@ -1857,16 +1854,16 @@
     </row>
     <row r="22" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="B22" s="14" t="s">
+      <c r="C22" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="C22" s="14" t="s">
+      <c r="D22" s="14" t="s">
         <v>47</v>
-      </c>
-      <c r="D22" s="14" t="s">
-        <v>48</v>
       </c>
       <c r="E22" s="15"/>
       <c r="F22" s="15" t="n">
@@ -1880,17 +1877,17 @@
     </row>
     <row r="23" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="B23" s="14" t="s">
+      <c r="C23" s="14" t="s">
         <v>50</v>
-      </c>
-      <c r="C23" s="14" t="s">
-        <v>51</v>
       </c>
       <c r="D23" s="14"/>
       <c r="E23" s="15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F23" s="15" t="n">
         <f aca="false">FALSE()</f>
@@ -1903,17 +1900,17 @@
     </row>
     <row r="24" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="B24" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="B24" s="14" t="s">
+      <c r="C24" s="14" t="s">
         <v>54</v>
-      </c>
-      <c r="C24" s="14" t="s">
-        <v>55</v>
       </c>
       <c r="D24" s="14"/>
       <c r="E24" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F24" s="15" t="n">
         <v>1</v>
@@ -1925,13 +1922,13 @@
     </row>
     <row r="25" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="B25" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="B25" s="14" t="s">
+      <c r="C25" s="14" t="s">
         <v>58</v>
-      </c>
-      <c r="C25" s="14" t="s">
-        <v>59</v>
       </c>
       <c r="D25" s="14"/>
       <c r="E25" s="15"/>
@@ -1943,16 +1940,16 @@
     </row>
     <row r="26" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="B26" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="B26" s="14" t="s">
+      <c r="C26" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="C26" s="14" t="s">
+      <c r="D26" s="14" t="s">
         <v>62</v>
-      </c>
-      <c r="D26" s="14" t="s">
-        <v>63</v>
       </c>
       <c r="E26" s="15"/>
       <c r="F26" s="15" t="n">
@@ -1991,33 +1988,33 @@
         <v>16</v>
       </c>
       <c r="B29" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="C29" s="20" t="s">
         <v>64</v>
-      </c>
-      <c r="C29" s="20" t="s">
-        <v>65</v>
       </c>
       <c r="D29" s="20"/>
       <c r="E29" s="21"/>
       <c r="F29" s="21"/>
       <c r="G29" s="20" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H29" s="20"/>
       <c r="I29" s="20"/>
     </row>
     <row r="30" s="22" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="B30" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="B30" s="20" t="s">
+      <c r="C30" s="20" t="s">
         <v>68</v>
-      </c>
-      <c r="C30" s="20" t="s">
-        <v>69</v>
       </c>
       <c r="D30" s="20"/>
       <c r="E30" s="21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F30" s="21"/>
       <c r="H30" s="20"/>
@@ -2027,17 +2024,17 @@
     </row>
     <row r="31" s="22" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="B31" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="B31" s="20" t="s">
+      <c r="C31" s="20" t="s">
         <v>72</v>
-      </c>
-      <c r="C31" s="20" t="s">
-        <v>73</v>
       </c>
       <c r="D31" s="20"/>
       <c r="E31" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F31" s="21"/>
       <c r="G31" s="20"/>
@@ -2075,16 +2072,16 @@
         <v>16</v>
       </c>
       <c r="B34" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="C34" s="24" t="s">
         <v>74</v>
-      </c>
-      <c r="C34" s="24" t="s">
-        <v>75</v>
       </c>
       <c r="D34" s="24"/>
       <c r="E34" s="25"/>
       <c r="F34" s="25"/>
       <c r="G34" s="24" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H34" s="24"/>
       <c r="I34" s="24" t="s">
@@ -2093,17 +2090,17 @@
     </row>
     <row r="35" s="26" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="B35" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="B35" s="27" t="s">
+      <c r="C35" s="27" t="s">
         <v>78</v>
-      </c>
-      <c r="C35" s="27" t="s">
-        <v>79</v>
       </c>
       <c r="D35" s="23"/>
       <c r="E35" s="28" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F35" s="28" t="n">
         <v>1</v>
@@ -2137,10 +2134,10 @@
         <v>31</v>
       </c>
       <c r="B36" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="C36" s="27" t="s">
         <v>80</v>
-      </c>
-      <c r="C36" s="27" t="s">
-        <v>81</v>
       </c>
       <c r="D36" s="23"/>
       <c r="E36" s="28"/>
@@ -2169,19 +2166,19 @@
     </row>
     <row r="37" s="26" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="B37" s="27" t="s">
         <v>82</v>
       </c>
-      <c r="B37" s="27" t="s">
+      <c r="C37" s="27" t="s">
         <v>83</v>
-      </c>
-      <c r="C37" s="27" t="s">
-        <v>84</v>
       </c>
       <c r="D37" s="23"/>
       <c r="E37" s="28"/>
       <c r="F37" s="28"/>
       <c r="I37" s="23" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J37" s="29"/>
       <c r="K37" s="29"/>
@@ -2239,16 +2236,16 @@
         <v>16</v>
       </c>
       <c r="B40" s="32" t="s">
+        <v>85</v>
+      </c>
+      <c r="C40" s="32" t="s">
         <v>86</v>
-      </c>
-      <c r="C40" s="32" t="s">
-        <v>87</v>
       </c>
       <c r="D40" s="31"/>
       <c r="E40" s="33"/>
       <c r="F40" s="33"/>
       <c r="G40" s="34" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I40" s="34" t="s">
         <v>19</v>
@@ -2275,17 +2272,17 @@
     </row>
     <row r="41" s="35" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="31" t="s">
+        <v>88</v>
+      </c>
+      <c r="B41" s="32" t="s">
         <v>89</v>
       </c>
-      <c r="B41" s="32" t="s">
+      <c r="C41" s="35" t="s">
         <v>90</v>
-      </c>
-      <c r="C41" s="35" t="s">
-        <v>91</v>
       </c>
       <c r="D41" s="31"/>
       <c r="E41" s="33" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F41" s="33" t="n">
         <v>1</v>
@@ -2322,7 +2319,7 @@
         <v>1</v>
       </c>
       <c r="C42" s="35" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D42" s="31"/>
       <c r="E42" s="33"/>
@@ -2353,19 +2350,19 @@
     </row>
     <row r="43" s="35" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="31" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B43" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="C43" s="32" t="s">
         <v>93</v>
-      </c>
-      <c r="C43" s="32" t="s">
-        <v>94</v>
       </c>
       <c r="D43" s="31"/>
       <c r="E43" s="33"/>
       <c r="F43" s="33"/>
       <c r="I43" s="31" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J43" s="36"/>
       <c r="K43" s="36"/>
@@ -2389,23 +2386,23 @@
     </row>
     <row r="44" s="35" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="31" t="s">
+        <v>94</v>
+      </c>
+      <c r="B44" s="32" t="s">
         <v>95</v>
       </c>
-      <c r="B44" s="32" t="s">
+      <c r="C44" s="32" t="s">
         <v>96</v>
-      </c>
-      <c r="C44" s="32" t="s">
-        <v>97</v>
       </c>
       <c r="D44" s="31"/>
       <c r="E44" s="33" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F44" s="33" t="n">
         <v>0</v>
       </c>
       <c r="G44" s="34" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I44" s="31" t="s">
         <v>25</v>
@@ -2490,16 +2487,16 @@
         <v>16</v>
       </c>
       <c r="B47" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="C47" s="20" t="s">
         <v>100</v>
-      </c>
-      <c r="C47" s="20" t="s">
-        <v>101</v>
       </c>
       <c r="D47" s="20"/>
       <c r="E47" s="21"/>
       <c r="F47" s="21"/>
       <c r="G47" s="20" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H47" s="20"/>
       <c r="I47" s="20" t="s">
@@ -2508,17 +2505,17 @@
     </row>
     <row r="48" s="41" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="20" t="s">
+        <v>102</v>
+      </c>
+      <c r="B48" s="20" t="s">
         <v>103</v>
       </c>
-      <c r="B48" s="20" t="s">
+      <c r="C48" s="20" t="s">
         <v>104</v>
-      </c>
-      <c r="C48" s="20" t="s">
-        <v>105</v>
       </c>
       <c r="D48" s="20"/>
       <c r="E48" s="21" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F48" s="21" t="n">
         <v>1</v>
@@ -2529,24 +2526,24 @@
     </row>
     <row r="49" s="41" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="42" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B49" s="43" t="s">
+        <v>106</v>
+      </c>
+      <c r="C49" s="43" t="s">
         <v>107</v>
       </c>
-      <c r="C49" s="43" t="s">
+      <c r="D49" s="42" t="s">
         <v>108</v>
-      </c>
-      <c r="D49" s="42" t="s">
-        <v>109</v>
       </c>
       <c r="E49" s="44"/>
       <c r="F49" s="44"/>
       <c r="G49" s="20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I49" s="42" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J49" s="45"/>
       <c r="K49" s="45"/>
@@ -2570,19 +2567,19 @@
     </row>
     <row r="50" s="41" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="42" t="s">
+        <v>110</v>
+      </c>
+      <c r="B50" s="43" t="s">
         <v>111</v>
       </c>
-      <c r="B50" s="43" t="s">
+      <c r="C50" s="43" t="s">
         <v>112</v>
-      </c>
-      <c r="C50" s="43" t="s">
-        <v>113</v>
       </c>
       <c r="D50" s="42"/>
       <c r="E50" s="44"/>
       <c r="F50" s="44"/>
       <c r="G50" s="20" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I50" s="42"/>
       <c r="J50" s="45"/>
@@ -2663,10 +2660,10 @@
         <v>16</v>
       </c>
       <c r="B53" s="47" t="s">
+        <v>114</v>
+      </c>
+      <c r="C53" s="48" t="s">
         <v>115</v>
-      </c>
-      <c r="C53" s="48" t="s">
-        <v>116</v>
       </c>
       <c r="D53" s="48"/>
       <c r="E53" s="49"/>
@@ -2701,10 +2698,10 @@
         <v>31</v>
       </c>
       <c r="B54" s="52" t="s">
+        <v>116</v>
+      </c>
+      <c r="C54" s="52" t="s">
         <v>117</v>
-      </c>
-      <c r="C54" s="52" t="s">
-        <v>118</v>
       </c>
       <c r="D54" s="47"/>
       <c r="E54" s="50"/>
@@ -2736,13 +2733,13 @@
     </row>
     <row r="55" s="51" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="53" t="s">
+        <v>118</v>
+      </c>
+      <c r="B55" s="53" t="s">
+        <v>118</v>
+      </c>
+      <c r="C55" s="54" t="s">
         <v>119</v>
-      </c>
-      <c r="B55" s="53" t="s">
-        <v>119</v>
-      </c>
-      <c r="C55" s="54" t="s">
-        <v>120</v>
       </c>
       <c r="D55" s="53"/>
       <c r="E55" s="55"/>
@@ -2753,7 +2750,7 @@
         <v>25</v>
       </c>
       <c r="J55" s="57" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K55" s="58"/>
       <c r="L55" s="58"/>
@@ -2776,13 +2773,13 @@
     </row>
     <row r="56" s="51" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="53" t="s">
+        <v>121</v>
+      </c>
+      <c r="B56" s="53" t="s">
+        <v>121</v>
+      </c>
+      <c r="C56" s="54" t="s">
         <v>122</v>
-      </c>
-      <c r="B56" s="53" t="s">
-        <v>122</v>
-      </c>
-      <c r="C56" s="54" t="s">
-        <v>123</v>
       </c>
       <c r="D56" s="53"/>
       <c r="E56" s="55"/>
@@ -2793,7 +2790,7 @@
         <v>25</v>
       </c>
       <c r="J56" s="57" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="K56" s="58"/>
       <c r="L56" s="58"/>
@@ -2854,7 +2851,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2869,11 +2866,11 @@
   </sheetPr>
   <dimension ref="A1:Z123"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A100" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A67" activeCellId="0" sqref="A67"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A15" activeCellId="3" sqref="G34 G40 G47 A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.72"/>
@@ -2881,7 +2878,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -2918,10 +2915,10 @@
         <v>23</v>
       </c>
       <c r="B2" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="9" t="s">
         <v>35</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>36</v>
       </c>
       <c r="D2" s="60"/>
     </row>
@@ -2930,10 +2927,10 @@
         <v>23</v>
       </c>
       <c r="B3" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="C3" s="9" t="s">
         <v>126</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>127</v>
       </c>
       <c r="D3" s="60"/>
     </row>
@@ -2942,22 +2939,19 @@
         <v>23</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C4" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="D4" s="60"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="C5" s="9" t="s">
         <v>128</v>
-      </c>
-      <c r="D4" s="60"/>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>129</v>
       </c>
       <c r="D5" s="60"/>
     </row>
@@ -2966,10 +2960,10 @@
         <v>27</v>
       </c>
       <c r="B7" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="C7" s="9" t="s">
         <v>130</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>131</v>
       </c>
       <c r="D7" s="60"/>
     </row>
@@ -2978,10 +2972,10 @@
         <v>27</v>
       </c>
       <c r="B8" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="C8" s="9" t="s">
         <v>132</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>133</v>
       </c>
       <c r="D8" s="60"/>
     </row>
@@ -2990,10 +2984,10 @@
         <v>27</v>
       </c>
       <c r="B9" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="C9" s="9" t="s">
         <v>134</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>135</v>
       </c>
       <c r="D9" s="60"/>
     </row>
@@ -3002,10 +2996,10 @@
         <v>27</v>
       </c>
       <c r="B10" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="C10" s="9" t="s">
         <v>136</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>137</v>
       </c>
       <c r="D10" s="60"/>
     </row>
@@ -3014,10 +3008,10 @@
         <v>27</v>
       </c>
       <c r="B11" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="C11" s="9" t="s">
         <v>138</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>139</v>
       </c>
       <c r="D11" s="60"/>
     </row>
@@ -3029,7 +3023,7 @@
         <v>29</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D12" s="60"/>
     </row>
@@ -3038,10 +3032,10 @@
         <v>27</v>
       </c>
       <c r="B13" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="C13" s="9" t="s">
         <v>141</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>142</v>
       </c>
       <c r="D13" s="60"/>
     </row>
@@ -3050,10 +3044,10 @@
         <v>27</v>
       </c>
       <c r="B14" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="C14" s="9" t="s">
         <v>126</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>127</v>
       </c>
       <c r="D14" s="60"/>
     </row>
@@ -3062,10 +3056,10 @@
         <v>27</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D15" s="60"/>
     </row>
@@ -3077,25 +3071,25 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" s="9" t="s">
         <v>144</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>145</v>
       </c>
       <c r="D17" s="60"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B18" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="C18" s="9" t="s">
         <v>146</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>147</v>
       </c>
       <c r="D18" s="60"/>
     </row>
@@ -3107,145 +3101,145 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B20" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="C20" s="9" t="s">
         <v>148</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>149</v>
       </c>
       <c r="D20" s="60"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B21" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="C21" s="9" t="s">
         <v>150</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>151</v>
       </c>
       <c r="D21" s="60"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B22" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="C22" s="9" t="s">
         <v>152</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>153</v>
       </c>
       <c r="D22" s="60"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D23" s="60"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B24" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="C24" s="9" t="s">
         <v>155</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>156</v>
       </c>
       <c r="D24" s="60"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B25" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="C25" s="9" t="s">
         <v>157</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>158</v>
       </c>
       <c r="D25" s="60"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B26" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="C26" s="9" t="s">
         <v>159</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>160</v>
       </c>
       <c r="D26" s="60"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B27" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="C27" s="9" t="s">
         <v>161</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>162</v>
       </c>
       <c r="D27" s="60"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B28" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="C28" s="9" t="s">
         <v>163</v>
-      </c>
-      <c r="C28" s="9" t="s">
-        <v>164</v>
       </c>
       <c r="D28" s="60"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B29" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="C29" s="9" t="s">
         <v>165</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>166</v>
       </c>
       <c r="D29" s="60"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B30" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="C30" s="9" t="s">
         <v>167</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>168</v>
       </c>
       <c r="D30" s="60"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B31" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="C31" s="9" t="s">
         <v>169</v>
-      </c>
-      <c r="C31" s="9" t="s">
-        <v>170</v>
       </c>
       <c r="D31" s="60"/>
     </row>
@@ -3257,73 +3251,73 @@
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D33" s="60"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B34" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="C34" s="9" t="s">
         <v>172</v>
-      </c>
-      <c r="C34" s="9" t="s">
-        <v>173</v>
       </c>
       <c r="D34" s="60"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B35" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="C35" s="9" t="s">
         <v>174</v>
-      </c>
-      <c r="C35" s="9" t="s">
-        <v>175</v>
       </c>
       <c r="D35" s="60"/>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B36" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="C36" s="9" t="s">
         <v>176</v>
-      </c>
-      <c r="C36" s="9" t="s">
-        <v>177</v>
       </c>
       <c r="D36" s="60"/>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B37" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="C37" s="9" t="s">
         <v>178</v>
-      </c>
-      <c r="C37" s="9" t="s">
-        <v>179</v>
       </c>
       <c r="D37" s="60"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B38" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="C38" s="0" t="s">
         <v>180</v>
-      </c>
-      <c r="C38" s="0" t="s">
-        <v>181</v>
       </c>
       <c r="D38" s="60"/>
     </row>
@@ -3335,25 +3329,25 @@
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D40" s="60"/>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D41" s="60"/>
     </row>
@@ -3365,37 +3359,37 @@
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D43" s="60"/>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D44" s="60"/>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B45" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="C45" s="9" t="s">
         <v>182</v>
-      </c>
-      <c r="C45" s="9" t="s">
-        <v>183</v>
       </c>
       <c r="D45" s="60"/>
     </row>
@@ -3407,750 +3401,750 @@
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B47" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="C47" s="9" t="s">
         <v>184</v>
-      </c>
-      <c r="C47" s="9" t="s">
-        <v>185</v>
       </c>
       <c r="D47" s="60"/>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D48" s="60"/>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B49" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="C49" s="9" t="s">
         <v>187</v>
-      </c>
-      <c r="C49" s="9" t="s">
-        <v>188</v>
       </c>
       <c r="D49" s="60"/>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B50" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="C50" s="9" t="s">
         <v>189</v>
-      </c>
-      <c r="C50" s="9" t="s">
-        <v>190</v>
       </c>
       <c r="D50" s="60"/>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B51" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="C51" s="9" t="s">
         <v>191</v>
-      </c>
-      <c r="C51" s="9" t="s">
-        <v>192</v>
       </c>
       <c r="D51" s="60"/>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B53" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="C53" s="0" t="s">
         <v>193</v>
-      </c>
-      <c r="C53" s="0" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B54" s="0" t="s">
+        <v>194</v>
+      </c>
+      <c r="C54" s="0" t="s">
         <v>195</v>
-      </c>
-      <c r="C54" s="0" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B55" s="0" t="s">
+        <v>196</v>
+      </c>
+      <c r="C55" s="0" t="s">
         <v>197</v>
-      </c>
-      <c r="C55" s="0" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B56" s="0" t="s">
+        <v>198</v>
+      </c>
+      <c r="C56" s="0" t="s">
         <v>199</v>
-      </c>
-      <c r="C56" s="0" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B57" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="C57" s="0" t="s">
         <v>201</v>
-      </c>
-      <c r="C57" s="0" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
+        <v>202</v>
+      </c>
+      <c r="B59" s="0" t="s">
         <v>203</v>
       </c>
-      <c r="B59" s="0" t="s">
+      <c r="C59" s="0" t="s">
         <v>204</v>
-      </c>
-      <c r="C59" s="0" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B60" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="C60" s="0" t="s">
         <v>206</v>
-      </c>
-      <c r="C60" s="0" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B61" s="0" t="s">
+        <v>207</v>
+      </c>
+      <c r="C61" s="0" t="s">
         <v>208</v>
-      </c>
-      <c r="C61" s="0" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B62" s="0" t="s">
+        <v>209</v>
+      </c>
+      <c r="C62" s="0" t="s">
         <v>210</v>
-      </c>
-      <c r="C62" s="0" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B69" s="0" t="s">
+        <v>214</v>
+      </c>
+      <c r="C69" s="0" t="s">
         <v>215</v>
-      </c>
-      <c r="C69" s="0" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B72" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="C72" s="0" t="s">
         <v>218</v>
-      </c>
-      <c r="C72" s="0" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B73" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="C73" s="0" t="s">
         <v>220</v>
-      </c>
-      <c r="C73" s="0" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B74" s="0" t="s">
+        <v>221</v>
+      </c>
+      <c r="C74" s="0" t="s">
         <v>222</v>
-      </c>
-      <c r="C74" s="0" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B75" s="0" t="s">
+        <v>223</v>
+      </c>
+      <c r="C75" s="0" t="s">
         <v>224</v>
-      </c>
-      <c r="C75" s="0" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B76" s="0" t="s">
+        <v>225</v>
+      </c>
+      <c r="C76" s="0" t="s">
         <v>226</v>
-      </c>
-      <c r="C76" s="0" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B77" s="0" t="s">
+        <v>227</v>
+      </c>
+      <c r="C77" s="0" t="s">
         <v>228</v>
-      </c>
-      <c r="C77" s="0" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B78" s="0" t="s">
+        <v>229</v>
+      </c>
+      <c r="C78" s="0" t="s">
         <v>230</v>
-      </c>
-      <c r="C78" s="0" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B79" s="0" t="s">
+        <v>231</v>
+      </c>
+      <c r="C79" s="0" t="s">
         <v>232</v>
-      </c>
-      <c r="C79" s="0" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B80" s="0" t="s">
+        <v>233</v>
+      </c>
+      <c r="C80" s="0" t="s">
         <v>234</v>
-      </c>
-      <c r="C80" s="0" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C81" s="0" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B83" s="0" t="s">
+        <v>236</v>
+      </c>
+      <c r="C83" s="0" t="s">
         <v>237</v>
-      </c>
-      <c r="C83" s="0" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B84" s="0" t="s">
+        <v>238</v>
+      </c>
+      <c r="C84" s="0" t="s">
         <v>239</v>
-      </c>
-      <c r="C84" s="0" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B85" s="0" t="s">
+        <v>240</v>
+      </c>
+      <c r="C85" s="0" t="s">
         <v>241</v>
-      </c>
-      <c r="C85" s="0" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B86" s="0" t="s">
+        <v>242</v>
+      </c>
+      <c r="C86" s="0" t="s">
         <v>243</v>
-      </c>
-      <c r="C86" s="0" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B87" s="0" t="s">
+        <v>244</v>
+      </c>
+      <c r="C87" s="0" t="s">
         <v>245</v>
-      </c>
-      <c r="C87" s="0" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B88" s="0" t="s">
+        <v>246</v>
+      </c>
+      <c r="C88" s="0" t="s">
         <v>247</v>
-      </c>
-      <c r="C88" s="0" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B89" s="0" t="s">
+        <v>248</v>
+      </c>
+      <c r="C89" s="0" t="s">
         <v>249</v>
-      </c>
-      <c r="C89" s="0" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B90" s="0" t="s">
+        <v>250</v>
+      </c>
+      <c r="C90" s="0" t="s">
         <v>251</v>
-      </c>
-      <c r="C90" s="0" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B91" s="0" t="s">
+        <v>252</v>
+      </c>
+      <c r="C91" s="0" t="s">
         <v>253</v>
-      </c>
-      <c r="C91" s="0" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B92" s="0" t="s">
+        <v>254</v>
+      </c>
+      <c r="C92" s="0" t="s">
         <v>255</v>
-      </c>
-      <c r="C92" s="0" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B93" s="0" t="s">
+        <v>256</v>
+      </c>
+      <c r="C93" s="0" t="s">
         <v>257</v>
-      </c>
-      <c r="C93" s="0" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B94" s="0" t="s">
+        <v>258</v>
+      </c>
+      <c r="C94" s="0" t="s">
         <v>259</v>
-      </c>
-      <c r="C94" s="0" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B95" s="0" t="s">
+        <v>260</v>
+      </c>
+      <c r="C95" s="0" t="s">
         <v>261</v>
-      </c>
-      <c r="C95" s="0" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B96" s="0" t="s">
+        <v>262</v>
+      </c>
+      <c r="C96" s="0" t="s">
         <v>263</v>
-      </c>
-      <c r="C96" s="0" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B97" s="0" t="s">
+        <v>264</v>
+      </c>
+      <c r="C97" s="0" t="s">
         <v>265</v>
-      </c>
-      <c r="C97" s="0" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B98" s="0" t="s">
+        <v>266</v>
+      </c>
+      <c r="C98" s="0" t="s">
         <v>267</v>
-      </c>
-      <c r="C98" s="0" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B99" s="0" t="s">
+        <v>268</v>
+      </c>
+      <c r="C99" s="0" t="s">
         <v>269</v>
-      </c>
-      <c r="C99" s="0" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B100" s="0" t="s">
+        <v>270</v>
+      </c>
+      <c r="C100" s="0" t="s">
         <v>271</v>
-      </c>
-      <c r="C100" s="0" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B101" s="0" t="s">
+        <v>272</v>
+      </c>
+      <c r="C101" s="0" t="s">
         <v>273</v>
-      </c>
-      <c r="C101" s="0" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B102" s="0" t="s">
+        <v>274</v>
+      </c>
+      <c r="C102" s="0" t="s">
         <v>275</v>
-      </c>
-      <c r="C102" s="0" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B103" s="0" t="s">
+        <v>276</v>
+      </c>
+      <c r="C103" s="0" t="s">
         <v>277</v>
-      </c>
-      <c r="C103" s="0" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B104" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C104" s="0" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B105" s="0" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C105" s="0" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B107" s="0" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C107" s="0" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B108" s="0" t="s">
+        <v>281</v>
+      </c>
+      <c r="C108" s="0" t="s">
         <v>282</v>
-      </c>
-      <c r="C108" s="0" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B109" s="0" t="s">
+        <v>283</v>
+      </c>
+      <c r="C109" s="0" t="s">
         <v>284</v>
-      </c>
-      <c r="C109" s="0" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B110" s="0" t="s">
+        <v>285</v>
+      </c>
+      <c r="C110" s="0" t="s">
         <v>286</v>
-      </c>
-      <c r="C110" s="0" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B111" s="0" t="s">
+        <v>287</v>
+      </c>
+      <c r="C111" s="0" t="s">
         <v>288</v>
-      </c>
-      <c r="C111" s="0" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B112" s="0" t="s">
+        <v>289</v>
+      </c>
+      <c r="C112" s="0" t="s">
         <v>290</v>
-      </c>
-      <c r="C112" s="0" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="61" t="s">
+        <v>291</v>
+      </c>
+      <c r="B114" s="0" t="s">
         <v>292</v>
       </c>
-      <c r="B114" s="0" t="s">
+      <c r="C114" s="0" t="s">
         <v>293</v>
-      </c>
-      <c r="C114" s="0" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="61" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B115" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C115" s="0" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="61" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B116" s="0" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C116" s="0" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="61" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B117" s="0" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C117" s="0" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="61" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B118" s="0" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C118" s="0" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="61" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B119" s="0" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C119" s="0" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B122" s="0" t="s">
+        <v>299</v>
+      </c>
+      <c r="C122" s="0" t="s">
         <v>300</v>
-      </c>
-      <c r="C122" s="0" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B123" s="0" t="s">
+        <v>301</v>
+      </c>
+      <c r="C123" s="0" t="s">
         <v>302</v>
-      </c>
-      <c r="C123" s="0" t="s">
-        <v>303</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -4166,35 +4160,35 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="3" sqref="G34 G40 G47 B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.36"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="62" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1" s="62" t="s">
         <v>304</v>
-      </c>
-      <c r="B1" s="62" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="63" t="n">
         <f aca="true">NOW()</f>
-        <v>44280.9173664483</v>
+        <v>44481.6482542914</v>
       </c>
       <c r="B2" s="64" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Don't use =now() for the version.
</commit_message>
<xml_diff>
--- a/XForms/highways.xlsx
+++ b/XForms/highways.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="309">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -72,6 +72,12 @@
     <t xml:space="preserve">phonenumber</t>
   </si>
   <si>
+    <t xml:space="preserve">start-geopoint</t>
+  </si>
+  <si>
+    <t xml:space="preserve">warmup</t>
+  </si>
+  <si>
     <t xml:space="preserve">begin_group</t>
   </si>
   <si>
@@ -732,16 +738,130 @@
     <t xml:space="preserve">Unknown bridge type</t>
   </si>
   <si>
+    <t xml:space="preserve">Swing Gate (single or double)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cattle grid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cattle Grid (bars in the road surface that allow wheeled vehicles but not animals to cross)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chain (chain used to prevent motorized vehicles)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">debris</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Debris (road is blocked by debris with or without ground)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ditch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ditch (trench,  ditch or ravine,  usually with a stream at the bottom  that is not easily crossed especially if not on foot)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cable barrier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cable Barrier (road side or median barrier made of steel wire ropes mounted on weak posts)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gate (entrance that can be opened or closed to get through the barrier)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bollard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bollard (usually concrete or metal) pillar or pillars in the middle of the road to prevent passage by some traffic</t>
+  </si>
+  <si>
     <t xml:space="preserve">block</t>
   </si>
   <si>
     <t xml:space="preserve">Block (large  solid  immobile block that can be moved only with heavy machinery or great effort)</t>
   </si>
   <si>
-    <t xml:space="preserve">bollard</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bollard (usually concrete or metal) pillar or pillars in the middle of the road to prevent passage by some traffic</t>
+    <t xml:space="preserve">fence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fence (structure supported by posts driven into the ground and designed to prevent movement across a boundary)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">guard rail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Guard Rail (also called a crash barrier)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hampshire gate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hampshire Gate (section of wire fence which can be removed temporarily)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hedge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hedge (Is a line of closely spaced shrubs and bushes  planted and trained in such a way as to form a barrier or to mark the boundary of an area)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jersey barrier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jersey Barrier (consists of heavy prefabricated blocks to create a barrier)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kerb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kerb or Curb (short solid barrier, usually found at the edge of a road, path or sidewalk,  which prevents entrance by vehicles) wheelchair users </t>
+  </si>
+  <si>
+    <t xml:space="preserve">lift gate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lift Gate (bar,  or pole pivoted in such a way as to allow the boom to block vehicular access through a controlled point)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">log</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Log (passage is closed by lumber, like the trunk of a tree)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rope</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rope (flexible barrier made of fibers twisted or braided together to improve strength)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sliding gate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sliding Gate (Similar to a lift gate but slides sidewards to open)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stile  (allows pedestrians to cross a wall or fence  but never actually "opens" the barrier )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unknown barrier type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">city wall</t>
+  </si>
+  <si>
+    <t xml:space="preserve">City Wall (A fortification used to defend a city or settlement from potential aggressors)</t>
   </si>
   <si>
     <t xml:space="preserve">border control</t>
@@ -750,120 +870,6 @@
     <t xml:space="preserve">Border Control (control point at an international border between two countries)</t>
   </si>
   <si>
-    <t xml:space="preserve">cable barrier</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cable Barrier (road side or median barrier made of steel wire ropes mounted on weak posts)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cattle grid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cattle Grid (bars in the road surface that allow wheeled vehicles but not animals to cross)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">chain</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chain (chain used to prevent motorized vehicles)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">city wall</t>
-  </si>
-  <si>
-    <t xml:space="preserve">City Wall (A fortification used to defend a city or settlement from potential aggressors)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">debris</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Debris (road is blocked by debris with or without ground)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ditch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ditch (trench,  ditch or ravine,  usually with a stream at the bottom  that is not easily crossed especially if not on foot)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fence</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fence (structure supported by posts driven into the ground and designed to prevent movement across a boundary)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gate (entrance that can be opened or closed to get through the barrier)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">guard rail</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Guard Rail (also called a crash barrier)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hampshire gate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hampshire Gate (section of wire fence which can be removed temporarily)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hedge</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hedge (Is a line of closely spaced shrubs and bushes  planted and trained in such a way as to form a barrier or to mark the boundary of an area)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">jersey barrier</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jersey Barrier (consists of heavy prefabricated blocks to create a barrier)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">kerb</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kerb or Curb (short solid barrier, usually found at the edge of a road, path or sidewalk,  which prevents entrance by vehicles) wheelchair users </t>
-  </si>
-  <si>
-    <t xml:space="preserve">lift gate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lift Gate (bar,  or pole pivoted in such a way as to allow the boom to block vehicular access through a controlled point)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">log</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Log (passage is closed by lumber, like the trunk of a tree)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rope</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rope (flexible barrier made of fibers twisted or braided together to improve strength)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sliding gate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sliding Gate (Similar to a lift gate but slides sidewards to open)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">stile</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stile  (allows pedestrians to cross a wall or fence  but never actually "opens" the barrier )</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unknown barrier type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Swing Gate (single or double)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Hiking (Can be hiked in ordinary sports shoes/trainers, no risk of falling)</t>
   </si>
   <si>
@@ -937,6 +943,9 @@
   </si>
   <si>
     <t xml:space="preserve">title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">v3</t>
   </si>
   <si>
     <t xml:space="preserve">Highways</t>
@@ -1389,7 +1398,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1474,13 +1483,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AB60"/>
+  <dimension ref="A1:AB61"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A21" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G34" activeCellId="0" sqref="G34 G40 G47"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G53" activeCellId="0" sqref="G53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.79"/>
@@ -1620,142 +1629,141 @@
       <c r="E7" s="0"/>
       <c r="F7" s="0"/>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="11" t="s">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="11"/>
       <c r="E8" s="0"/>
       <c r="F8" s="0"/>
-      <c r="I8" s="11" t="s">
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="11" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="9"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-    </row>
-    <row r="10" s="13" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="11" t="s">
+      <c r="C9" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="D9" s="11"/>
+      <c r="E9" s="0"/>
+      <c r="F9" s="0"/>
+      <c r="I9" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E11" s="0"/>
-      <c r="F11" s="0"/>
-    </row>
-    <row r="12" s="13" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="11" t="s">
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="9"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+    </row>
+    <row r="11" s="13" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="C11" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12" s="11"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12" t="n">
-        <v>1</v>
-      </c>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="11" t="s">
-        <v>25</v>
-      </c>
+      <c r="D11" s="11"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E12" s="0"/>
+      <c r="F12" s="0"/>
     </row>
     <row r="13" s="13" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>28</v>
-      </c>
       <c r="D13" s="11"/>
-      <c r="E13" s="12" t="s">
-        <v>29</v>
-      </c>
+      <c r="E13" s="12"/>
       <c r="F13" s="12" t="n">
         <v>1</v>
       </c>
-      <c r="G13" s="11" t="s">
-        <v>30</v>
-      </c>
+      <c r="G13" s="11"/>
       <c r="H13" s="11"/>
       <c r="I13" s="11" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" s="13" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="11"/>
+      <c r="E14" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="F14" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="G14" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="H14" s="11"/>
+      <c r="I14" s="11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" s="13" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="11"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12" t="n">
+      <c r="B15" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="11"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G14" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="H14" s="11"/>
-      <c r="I14" s="11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" s="13" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="B15" s="11"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="11"/>
+      <c r="G15" s="11" t="s">
+        <v>32</v>
+      </c>
       <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
+      <c r="I15" s="11" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="16" s="13" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="11"/>
+      <c r="A16" s="11" t="s">
+        <v>36</v>
+      </c>
       <c r="B16" s="11"/>
       <c r="C16" s="11"/>
       <c r="D16" s="11"/>
@@ -1766,372 +1774,342 @@
       <c r="I16" s="11"/>
     </row>
     <row r="17" s="13" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0"/>
-      <c r="B17" s="0"/>
-      <c r="C17" s="0"/>
-      <c r="D17" s="0"/>
+      <c r="A17" s="11"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
       <c r="E17" s="12"/>
       <c r="F17" s="12"/>
       <c r="G17" s="11"/>
       <c r="H17" s="11"/>
       <c r="I17" s="11"/>
     </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="9"/>
-      <c r="B18" s="9"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9"/>
-    </row>
-    <row r="19" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="B19" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="D19" s="14"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14" t="s">
-        <v>19</v>
-      </c>
+    <row r="18" s="13" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0"/>
+      <c r="B18" s="0"/>
+      <c r="C18" s="0"/>
+      <c r="D18" s="0"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="9"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
     </row>
     <row r="20" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="14" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="B20" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="C20" s="14" t="s">
-        <v>38</v>
-      </c>
       <c r="D20" s="14"/>
-      <c r="E20" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="F20" s="15" t="n">
-        <v>1</v>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="14" t="s">
+        <v>32</v>
       </c>
       <c r="H20" s="14"/>
       <c r="I20" s="14" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" s="14" t="s">
         <v>40</v>
-      </c>
-      <c r="B21" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="C21" s="14" t="s">
-        <v>42</v>
       </c>
       <c r="D21" s="14"/>
       <c r="E21" s="15" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F21" s="15" t="n">
         <v>1</v>
       </c>
       <c r="H21" s="14"/>
       <c r="I21" s="14" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="B22" s="14" t="s">
+      <c r="D22" s="14"/>
+      <c r="E22" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="C22" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="D22" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="E22" s="15"/>
       <c r="F22" s="15" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H22" s="14"/>
       <c r="I22" s="14" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="23" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="C23" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="B23" s="14" t="s">
+      <c r="D23" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="C23" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="D23" s="14"/>
-      <c r="E23" s="15" t="s">
-        <v>51</v>
-      </c>
+      <c r="E23" s="15"/>
       <c r="F23" s="15" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="H23" s="14"/>
       <c r="I23" s="14" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" s="14" t="s">
         <v>52</v>
-      </c>
-      <c r="B24" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="C24" s="14" t="s">
-        <v>54</v>
       </c>
       <c r="D24" s="14"/>
       <c r="E24" s="15" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F24" s="15" t="n">
-        <v>1</v>
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
       <c r="H24" s="14"/>
       <c r="I24" s="14" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="25" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="C25" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="B25" s="14" t="s">
+      <c r="D25" s="14"/>
+      <c r="E25" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="C25" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="D25" s="14"/>
-      <c r="E25" s="15"/>
-      <c r="F25" s="15"/>
+      <c r="F25" s="15" t="n">
+        <v>1</v>
+      </c>
       <c r="H25" s="14"/>
       <c r="I25" s="14" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="26" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B26" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="B26" s="14" t="s">
+      <c r="C26" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="C26" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="D26" s="14" t="s">
-        <v>62</v>
-      </c>
+      <c r="D26" s="14"/>
       <c r="E26" s="15"/>
-      <c r="F26" s="15" t="n">
-        <v>1</v>
-      </c>
-      <c r="G26" s="14"/>
+      <c r="F26" s="15"/>
       <c r="H26" s="14"/>
-      <c r="I26" s="14"/>
+      <c r="I26" s="14" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="27" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="B27" s="14"/>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
+        <v>61</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="D27" s="14" t="s">
+        <v>64</v>
+      </c>
       <c r="E27" s="15"/>
-      <c r="F27" s="15"/>
+      <c r="F27" s="15" t="n">
+        <v>1</v>
+      </c>
       <c r="G27" s="14"/>
       <c r="H27" s="14"/>
       <c r="I27" s="14"/>
     </row>
-    <row r="28" s="19" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="17"/>
-      <c r="B28" s="17"/>
-      <c r="C28" s="17"/>
-      <c r="D28" s="17"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="17"/>
-      <c r="H28" s="17"/>
-      <c r="I28" s="17"/>
-    </row>
-    <row r="29" s="22" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="B29" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="C29" s="20" t="s">
-        <v>64</v>
-      </c>
-      <c r="D29" s="20"/>
-      <c r="E29" s="21"/>
-      <c r="F29" s="21"/>
-      <c r="G29" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="H29" s="20"/>
-      <c r="I29" s="20"/>
+    <row r="28" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" s="14"/>
+      <c r="C28" s="14"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="14"/>
+      <c r="H28" s="14"/>
+      <c r="I28" s="14"/>
+    </row>
+    <row r="29" s="19" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="17"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="17"/>
+      <c r="H29" s="17"/>
+      <c r="I29" s="17"/>
     </row>
     <row r="30" s="22" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="B30" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="C30" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="B30" s="20" t="s">
+      <c r="D30" s="20"/>
+      <c r="E30" s="21"/>
+      <c r="F30" s="21"/>
+      <c r="G30" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="C30" s="20" t="s">
-        <v>68</v>
-      </c>
-      <c r="D30" s="20"/>
-      <c r="E30" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="F30" s="21"/>
       <c r="H30" s="20"/>
-      <c r="I30" s="20" t="s">
-        <v>25</v>
-      </c>
+      <c r="I30" s="20"/>
     </row>
     <row r="31" s="22" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="B31" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="C31" s="20" t="s">
         <v>70</v>
-      </c>
-      <c r="B31" s="20" t="s">
-        <v>71</v>
-      </c>
-      <c r="C31" s="20" t="s">
-        <v>72</v>
       </c>
       <c r="D31" s="20"/>
       <c r="E31" s="21" t="s">
-        <v>43</v>
+        <v>71</v>
       </c>
       <c r="F31" s="21"/>
-      <c r="G31" s="20"/>
       <c r="H31" s="20"/>
       <c r="I31" s="20" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="32" s="22" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="B32" s="20"/>
-      <c r="C32" s="20"/>
+        <v>72</v>
+      </c>
+      <c r="B32" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="C32" s="20" t="s">
+        <v>74</v>
+      </c>
       <c r="D32" s="20"/>
-      <c r="E32" s="21"/>
+      <c r="E32" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="F32" s="21"/>
       <c r="G32" s="20"/>
       <c r="H32" s="20"/>
-      <c r="I32" s="20"/>
-    </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="9"/>
-      <c r="B33" s="9"/>
-      <c r="C33" s="9"/>
-      <c r="D33" s="9"/>
-      <c r="E33" s="10"/>
-      <c r="F33" s="10"/>
-      <c r="G33" s="9"/>
-      <c r="H33" s="9"/>
-      <c r="I33" s="9"/>
-    </row>
-    <row r="34" s="26" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="B34" s="24" t="s">
-        <v>73</v>
-      </c>
-      <c r="C34" s="24" t="s">
-        <v>74</v>
-      </c>
-      <c r="D34" s="24"/>
-      <c r="E34" s="25"/>
-      <c r="F34" s="25"/>
-      <c r="G34" s="24" t="s">
+      <c r="I32" s="20" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="33" s="22" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="B33" s="20"/>
+      <c r="C33" s="20"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="21"/>
+      <c r="F33" s="21"/>
+      <c r="G33" s="20"/>
+      <c r="H33" s="20"/>
+      <c r="I33" s="20"/>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="9"/>
+      <c r="B34" s="9"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="10"/>
+      <c r="F34" s="10"/>
+      <c r="G34" s="9"/>
+      <c r="H34" s="9"/>
+      <c r="I34" s="9"/>
+    </row>
+    <row r="35" s="26" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="B35" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="H34" s="24"/>
-      <c r="I34" s="24" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="35" s="26" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="23" t="s">
+      <c r="C35" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="B35" s="27" t="s">
+      <c r="D35" s="24"/>
+      <c r="E35" s="25"/>
+      <c r="F35" s="25"/>
+      <c r="G35" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="C35" s="27" t="s">
-        <v>78</v>
-      </c>
-      <c r="D35" s="23"/>
-      <c r="E35" s="28" t="s">
-        <v>51</v>
-      </c>
-      <c r="F35" s="28" t="n">
-        <v>1</v>
-      </c>
-      <c r="G35" s="24"/>
-      <c r="I35" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="J35" s="29"/>
-      <c r="K35" s="29"/>
-      <c r="L35" s="29"/>
-      <c r="M35" s="29"/>
-      <c r="N35" s="29"/>
-      <c r="O35" s="29"/>
-      <c r="P35" s="29"/>
-      <c r="Q35" s="30"/>
-      <c r="R35" s="30"/>
-      <c r="S35" s="30"/>
-      <c r="T35" s="30"/>
-      <c r="U35" s="30"/>
-      <c r="V35" s="30"/>
-      <c r="W35" s="30"/>
-      <c r="X35" s="30"/>
-      <c r="Y35" s="30"/>
-      <c r="Z35" s="30"/>
-      <c r="AA35" s="30"/>
-      <c r="AB35" s="30"/>
+      <c r="H35" s="24"/>
+      <c r="I35" s="24" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="36" s="26" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="23" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="B36" s="27" t="s">
         <v>79</v>
@@ -2140,10 +2118,16 @@
         <v>80</v>
       </c>
       <c r="D36" s="23"/>
-      <c r="E36" s="28"/>
-      <c r="F36" s="28"/>
+      <c r="E36" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="F36" s="28" t="n">
+        <v>1</v>
+      </c>
       <c r="G36" s="24"/>
-      <c r="I36" s="23"/>
+      <c r="I36" s="23" t="s">
+        <v>27</v>
+      </c>
       <c r="J36" s="29"/>
       <c r="K36" s="29"/>
       <c r="L36" s="29"/>
@@ -2166,20 +2150,19 @@
     </row>
     <row r="37" s="26" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="B37" s="27" t="s">
         <v>81</v>
       </c>
-      <c r="B37" s="27" t="s">
+      <c r="C37" s="27" t="s">
         <v>82</v>
-      </c>
-      <c r="C37" s="27" t="s">
-        <v>83</v>
       </c>
       <c r="D37" s="23"/>
       <c r="E37" s="28"/>
       <c r="F37" s="28"/>
-      <c r="I37" s="23" t="s">
-        <v>84</v>
-      </c>
+      <c r="G37" s="24"/>
+      <c r="I37" s="23"/>
       <c r="J37" s="29"/>
       <c r="K37" s="29"/>
       <c r="L37" s="29"/>
@@ -2201,16 +2184,21 @@
       <c r="AB37" s="30"/>
     </row>
     <row r="38" s="26" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="B38" s="27"/>
-      <c r="C38" s="27"/>
+      <c r="A38" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="B38" s="27" t="s">
+        <v>84</v>
+      </c>
+      <c r="C38" s="27" t="s">
+        <v>85</v>
+      </c>
       <c r="D38" s="23"/>
       <c r="E38" s="28"/>
       <c r="F38" s="28"/>
-      <c r="G38" s="24"/>
-      <c r="I38" s="23"/>
+      <c r="I38" s="23" t="s">
+        <v>86</v>
+      </c>
       <c r="J38" s="29"/>
       <c r="K38" s="29"/>
       <c r="L38" s="29"/>
@@ -2231,65 +2219,55 @@
       <c r="AA38" s="30"/>
       <c r="AB38" s="30"/>
     </row>
-    <row r="40" s="35" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="31" t="s">
-        <v>16</v>
-      </c>
-      <c r="B40" s="32" t="s">
-        <v>85</v>
-      </c>
-      <c r="C40" s="32" t="s">
-        <v>86</v>
-      </c>
-      <c r="D40" s="31"/>
-      <c r="E40" s="33"/>
-      <c r="F40" s="33"/>
-      <c r="G40" s="34" t="s">
-        <v>87</v>
-      </c>
-      <c r="I40" s="34" t="s">
-        <v>19</v>
-      </c>
-      <c r="J40" s="36"/>
-      <c r="K40" s="36"/>
-      <c r="L40" s="36"/>
-      <c r="M40" s="36"/>
-      <c r="N40" s="36"/>
-      <c r="O40" s="36"/>
-      <c r="P40" s="36"/>
-      <c r="Q40" s="37"/>
-      <c r="R40" s="37"/>
-      <c r="S40" s="37"/>
-      <c r="T40" s="37"/>
-      <c r="U40" s="37"/>
-      <c r="V40" s="37"/>
-      <c r="W40" s="37"/>
-      <c r="X40" s="37"/>
-      <c r="Y40" s="37"/>
-      <c r="Z40" s="37"/>
-      <c r="AA40" s="37"/>
-      <c r="AB40" s="37"/>
+    <row r="39" s="26" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A39" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="B39" s="27"/>
+      <c r="C39" s="27"/>
+      <c r="D39" s="23"/>
+      <c r="E39" s="28"/>
+      <c r="F39" s="28"/>
+      <c r="G39" s="24"/>
+      <c r="I39" s="23"/>
+      <c r="J39" s="29"/>
+      <c r="K39" s="29"/>
+      <c r="L39" s="29"/>
+      <c r="M39" s="29"/>
+      <c r="N39" s="29"/>
+      <c r="O39" s="29"/>
+      <c r="P39" s="29"/>
+      <c r="Q39" s="30"/>
+      <c r="R39" s="30"/>
+      <c r="S39" s="30"/>
+      <c r="T39" s="30"/>
+      <c r="U39" s="30"/>
+      <c r="V39" s="30"/>
+      <c r="W39" s="30"/>
+      <c r="X39" s="30"/>
+      <c r="Y39" s="30"/>
+      <c r="Z39" s="30"/>
+      <c r="AA39" s="30"/>
+      <c r="AB39" s="30"/>
     </row>
     <row r="41" s="35" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="B41" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="C41" s="32" t="s">
         <v>88</v>
       </c>
-      <c r="B41" s="32" t="s">
+      <c r="D41" s="31"/>
+      <c r="E41" s="33"/>
+      <c r="F41" s="33"/>
+      <c r="G41" s="34" t="s">
         <v>89</v>
       </c>
-      <c r="C41" s="35" t="s">
-        <v>90</v>
-      </c>
-      <c r="D41" s="31"/>
-      <c r="E41" s="33" t="s">
-        <v>51</v>
-      </c>
-      <c r="F41" s="33" t="n">
-        <v>1</v>
-      </c>
-      <c r="G41" s="34"/>
-      <c r="I41" s="31" t="s">
-        <v>25</v>
+      <c r="I41" s="34" t="s">
+        <v>21</v>
       </c>
       <c r="J41" s="36"/>
       <c r="K41" s="36"/>
@@ -2313,20 +2291,24 @@
     </row>
     <row r="42" s="35" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="31" t="s">
-        <v>31</v>
+        <v>90</v>
       </c>
       <c r="B42" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="C42" s="35" t="s">
+        <v>92</v>
+      </c>
+      <c r="D42" s="31"/>
+      <c r="E42" s="33" t="s">
+        <v>53</v>
+      </c>
+      <c r="F42" s="33" t="n">
         <v>1</v>
       </c>
-      <c r="C42" s="35" t="s">
-        <v>91</v>
-      </c>
-      <c r="D42" s="31"/>
-      <c r="E42" s="33"/>
-      <c r="F42" s="33"/>
       <c r="G42" s="34"/>
       <c r="I42" s="31" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="J42" s="36"/>
       <c r="K42" s="36"/>
@@ -2350,19 +2332,20 @@
     </row>
     <row r="43" s="35" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="31" t="s">
-        <v>81</v>
+        <v>33</v>
       </c>
       <c r="B43" s="32" t="s">
-        <v>92</v>
-      </c>
-      <c r="C43" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="C43" s="35" t="s">
         <v>93</v>
       </c>
       <c r="D43" s="31"/>
       <c r="E43" s="33"/>
       <c r="F43" s="33"/>
+      <c r="G43" s="34"/>
       <c r="I43" s="31" t="s">
-        <v>84</v>
+        <v>27</v>
       </c>
       <c r="J43" s="36"/>
       <c r="K43" s="36"/>
@@ -2386,26 +2369,19 @@
     </row>
     <row r="44" s="35" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="B44" s="32" t="s">
         <v>94</v>
       </c>
-      <c r="B44" s="32" t="s">
+      <c r="C44" s="32" t="s">
         <v>95</v>
       </c>
-      <c r="C44" s="32" t="s">
-        <v>96</v>
-      </c>
       <c r="D44" s="31"/>
-      <c r="E44" s="33" t="s">
-        <v>97</v>
-      </c>
-      <c r="F44" s="33" t="n">
-        <v>0</v>
-      </c>
-      <c r="G44" s="34" t="s">
-        <v>98</v>
-      </c>
+      <c r="E44" s="33"/>
+      <c r="F44" s="33"/>
       <c r="I44" s="31" t="s">
-        <v>25</v>
+        <v>86</v>
       </c>
       <c r="J44" s="36"/>
       <c r="K44" s="36"/>
@@ -2428,16 +2404,28 @@
       <c r="AB44" s="37"/>
     </row>
     <row r="45" s="35" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="37" t="s">
-        <v>34</v>
-      </c>
-      <c r="B45" s="32"/>
-      <c r="C45" s="32"/>
+      <c r="A45" s="31" t="s">
+        <v>96</v>
+      </c>
+      <c r="B45" s="32" t="s">
+        <v>97</v>
+      </c>
+      <c r="C45" s="32" t="s">
+        <v>98</v>
+      </c>
       <c r="D45" s="31"/>
-      <c r="E45" s="31"/>
-      <c r="F45" s="31"/>
-      <c r="G45" s="31"/>
-      <c r="I45" s="31"/>
+      <c r="E45" s="33" t="s">
+        <v>99</v>
+      </c>
+      <c r="F45" s="33" t="n">
+        <v>0</v>
+      </c>
+      <c r="G45" s="34" t="s">
+        <v>100</v>
+      </c>
+      <c r="I45" s="31" t="s">
+        <v>27</v>
+      </c>
       <c r="J45" s="36"/>
       <c r="K45" s="36"/>
       <c r="L45" s="36"/>
@@ -2458,130 +2446,124 @@
       <c r="AA45" s="37"/>
       <c r="AB45" s="37"/>
     </row>
-    <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B46" s="38"/>
-      <c r="C46" s="38"/>
-      <c r="G46" s="9"/>
-      <c r="J46" s="39"/>
-      <c r="K46" s="39"/>
-      <c r="L46" s="39"/>
-      <c r="M46" s="39"/>
-      <c r="N46" s="39"/>
-      <c r="O46" s="39"/>
-      <c r="P46" s="39"/>
-      <c r="Q46" s="40"/>
-      <c r="R46" s="40"/>
-      <c r="S46" s="40"/>
-      <c r="T46" s="40"/>
-      <c r="U46" s="40"/>
-      <c r="V46" s="40"/>
-      <c r="W46" s="40"/>
-      <c r="X46" s="40"/>
-      <c r="Y46" s="40"/>
-      <c r="Z46" s="40"/>
-      <c r="AA46" s="40"/>
-      <c r="AB46" s="40"/>
-    </row>
-    <row r="47" s="41" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="B47" s="20" t="s">
-        <v>99</v>
-      </c>
-      <c r="C47" s="20" t="s">
-        <v>100</v>
-      </c>
-      <c r="D47" s="20"/>
-      <c r="E47" s="21"/>
-      <c r="F47" s="21"/>
-      <c r="G47" s="20" t="s">
-        <v>101</v>
-      </c>
-      <c r="H47" s="20"/>
-      <c r="I47" s="20" t="s">
-        <v>19</v>
-      </c>
+    <row r="46" s="35" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A46" s="37" t="s">
+        <v>36</v>
+      </c>
+      <c r="B46" s="32"/>
+      <c r="C46" s="32"/>
+      <c r="D46" s="31"/>
+      <c r="E46" s="31"/>
+      <c r="F46" s="31"/>
+      <c r="G46" s="31"/>
+      <c r="I46" s="31"/>
+      <c r="J46" s="36"/>
+      <c r="K46" s="36"/>
+      <c r="L46" s="36"/>
+      <c r="M46" s="36"/>
+      <c r="N46" s="36"/>
+      <c r="O46" s="36"/>
+      <c r="P46" s="36"/>
+      <c r="Q46" s="37"/>
+      <c r="R46" s="37"/>
+      <c r="S46" s="37"/>
+      <c r="T46" s="37"/>
+      <c r="U46" s="37"/>
+      <c r="V46" s="37"/>
+      <c r="W46" s="37"/>
+      <c r="X46" s="37"/>
+      <c r="Y46" s="37"/>
+      <c r="Z46" s="37"/>
+      <c r="AA46" s="37"/>
+      <c r="AB46" s="37"/>
+    </row>
+    <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B47" s="38"/>
+      <c r="C47" s="38"/>
+      <c r="G47" s="9"/>
+      <c r="J47" s="39"/>
+      <c r="K47" s="39"/>
+      <c r="L47" s="39"/>
+      <c r="M47" s="39"/>
+      <c r="N47" s="39"/>
+      <c r="O47" s="39"/>
+      <c r="P47" s="39"/>
+      <c r="Q47" s="40"/>
+      <c r="R47" s="40"/>
+      <c r="S47" s="40"/>
+      <c r="T47" s="40"/>
+      <c r="U47" s="40"/>
+      <c r="V47" s="40"/>
+      <c r="W47" s="40"/>
+      <c r="X47" s="40"/>
+      <c r="Y47" s="40"/>
+      <c r="Z47" s="40"/>
+      <c r="AA47" s="40"/>
+      <c r="AB47" s="40"/>
     </row>
     <row r="48" s="41" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="B48" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="C48" s="20" t="s">
         <v>102</v>
       </c>
-      <c r="B48" s="20" t="s">
+      <c r="D48" s="20"/>
+      <c r="E48" s="21"/>
+      <c r="F48" s="21"/>
+      <c r="G48" s="20" t="s">
         <v>103</v>
       </c>
-      <c r="C48" s="20" t="s">
+      <c r="H48" s="20"/>
+      <c r="I48" s="20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="49" s="41" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="20" t="s">
         <v>104</v>
       </c>
-      <c r="D48" s="20"/>
-      <c r="E48" s="21" t="s">
+      <c r="B49" s="20" t="s">
         <v>105</v>
       </c>
-      <c r="F48" s="21" t="n">
+      <c r="C49" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="D49" s="20"/>
+      <c r="E49" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="F49" s="21" t="n">
         <v>1</v>
       </c>
-      <c r="G48" s="20"/>
-      <c r="H48" s="20"/>
-      <c r="I48" s="20"/>
-    </row>
-    <row r="49" s="41" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A49" s="42" t="s">
-        <v>81</v>
-      </c>
-      <c r="B49" s="43" t="s">
-        <v>106</v>
-      </c>
-      <c r="C49" s="43" t="s">
-        <v>107</v>
-      </c>
-      <c r="D49" s="42" t="s">
-        <v>108</v>
-      </c>
-      <c r="E49" s="44"/>
-      <c r="F49" s="44"/>
-      <c r="G49" s="20" t="s">
-        <v>109</v>
-      </c>
-      <c r="I49" s="42" t="s">
-        <v>84</v>
-      </c>
-      <c r="J49" s="45"/>
-      <c r="K49" s="45"/>
-      <c r="L49" s="45"/>
-      <c r="M49" s="45"/>
-      <c r="N49" s="45"/>
-      <c r="O49" s="45"/>
-      <c r="P49" s="45"/>
-      <c r="Q49" s="46"/>
-      <c r="R49" s="46"/>
-      <c r="S49" s="46"/>
-      <c r="T49" s="46"/>
-      <c r="U49" s="46"/>
-      <c r="V49" s="46"/>
-      <c r="W49" s="46"/>
-      <c r="X49" s="46"/>
-      <c r="Y49" s="46"/>
-      <c r="Z49" s="46"/>
-      <c r="AA49" s="46"/>
-      <c r="AB49" s="46"/>
+      <c r="G49" s="20"/>
+      <c r="H49" s="20"/>
+      <c r="I49" s="20"/>
     </row>
     <row r="50" s="41" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="B50" s="43" t="s">
+        <v>108</v>
+      </c>
+      <c r="C50" s="43" t="s">
+        <v>109</v>
+      </c>
+      <c r="D50" s="42" t="s">
         <v>110</v>
       </c>
-      <c r="B50" s="43" t="s">
-        <v>111</v>
-      </c>
-      <c r="C50" s="43" t="s">
-        <v>112</v>
-      </c>
-      <c r="D50" s="42"/>
       <c r="E50" s="44"/>
       <c r="F50" s="44"/>
       <c r="G50" s="20" t="s">
-        <v>113</v>
-      </c>
-      <c r="I50" s="42"/>
+        <v>111</v>
+      </c>
+      <c r="I50" s="42" t="s">
+        <v>86</v>
+      </c>
       <c r="J50" s="45"/>
       <c r="K50" s="45"/>
       <c r="L50" s="45"/>
@@ -2603,14 +2585,21 @@
       <c r="AB50" s="46"/>
     </row>
     <row r="51" s="41" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A51" s="46" t="s">
-        <v>34</v>
-      </c>
-      <c r="B51" s="43"/>
-      <c r="C51" s="43"/>
+      <c r="A51" s="42" t="s">
+        <v>112</v>
+      </c>
+      <c r="B51" s="43" t="s">
+        <v>113</v>
+      </c>
+      <c r="C51" s="43" t="s">
+        <v>114</v>
+      </c>
       <c r="D51" s="42"/>
       <c r="E51" s="44"/>
       <c r="F51" s="44"/>
+      <c r="G51" s="20" t="s">
+        <v>115</v>
+      </c>
       <c r="I51" s="42"/>
       <c r="J51" s="45"/>
       <c r="K51" s="45"/>
@@ -2632,84 +2621,76 @@
       <c r="AA51" s="46"/>
       <c r="AB51" s="46"/>
     </row>
-    <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B52" s="38"/>
-      <c r="C52" s="38"/>
-      <c r="J52" s="39"/>
-      <c r="K52" s="39"/>
-      <c r="L52" s="39"/>
-      <c r="M52" s="39"/>
-      <c r="N52" s="39"/>
-      <c r="O52" s="39"/>
-      <c r="P52" s="39"/>
-      <c r="Q52" s="40"/>
-      <c r="R52" s="40"/>
-      <c r="S52" s="40"/>
-      <c r="T52" s="40"/>
-      <c r="U52" s="40"/>
-      <c r="V52" s="40"/>
-      <c r="W52" s="40"/>
-      <c r="X52" s="40"/>
-      <c r="Y52" s="40"/>
-      <c r="Z52" s="40"/>
-      <c r="AA52" s="40"/>
-      <c r="AB52" s="40"/>
-    </row>
-    <row r="53" s="51" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A53" s="47" t="s">
-        <v>16</v>
-      </c>
-      <c r="B53" s="47" t="s">
-        <v>114</v>
-      </c>
-      <c r="C53" s="48" t="s">
-        <v>115</v>
-      </c>
-      <c r="D53" s="48"/>
-      <c r="E53" s="49"/>
-      <c r="F53" s="50"/>
-      <c r="G53" s="47"/>
-      <c r="H53" s="47"/>
-      <c r="I53" s="47" t="s">
-        <v>19</v>
-      </c>
-      <c r="J53" s="47"/>
-      <c r="K53" s="47"/>
-      <c r="L53" s="47"/>
-      <c r="M53" s="47"/>
-      <c r="N53" s="47"/>
-      <c r="O53" s="47"/>
-      <c r="P53" s="47"/>
-      <c r="Q53" s="47"/>
-      <c r="R53" s="47"/>
-      <c r="S53" s="47"/>
-      <c r="T53" s="47"/>
-      <c r="U53" s="47"/>
-      <c r="V53" s="47"/>
-      <c r="W53" s="47"/>
-      <c r="X53" s="47"/>
-      <c r="Y53" s="47"/>
-      <c r="Z53" s="47"/>
-      <c r="AA53" s="47"/>
-      <c r="AB53" s="47"/>
+    <row r="52" s="41" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A52" s="46" t="s">
+        <v>36</v>
+      </c>
+      <c r="B52" s="43"/>
+      <c r="C52" s="43"/>
+      <c r="D52" s="42"/>
+      <c r="E52" s="44"/>
+      <c r="F52" s="44"/>
+      <c r="I52" s="42"/>
+      <c r="J52" s="45"/>
+      <c r="K52" s="45"/>
+      <c r="L52" s="45"/>
+      <c r="M52" s="45"/>
+      <c r="N52" s="45"/>
+      <c r="O52" s="45"/>
+      <c r="P52" s="45"/>
+      <c r="Q52" s="46"/>
+      <c r="R52" s="46"/>
+      <c r="S52" s="46"/>
+      <c r="T52" s="46"/>
+      <c r="U52" s="46"/>
+      <c r="V52" s="46"/>
+      <c r="W52" s="46"/>
+      <c r="X52" s="46"/>
+      <c r="Y52" s="46"/>
+      <c r="Z52" s="46"/>
+      <c r="AA52" s="46"/>
+      <c r="AB52" s="46"/>
+    </row>
+    <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B53" s="38"/>
+      <c r="C53" s="38"/>
+      <c r="J53" s="39"/>
+      <c r="K53" s="39"/>
+      <c r="L53" s="39"/>
+      <c r="M53" s="39"/>
+      <c r="N53" s="39"/>
+      <c r="O53" s="39"/>
+      <c r="P53" s="39"/>
+      <c r="Q53" s="40"/>
+      <c r="R53" s="40"/>
+      <c r="S53" s="40"/>
+      <c r="T53" s="40"/>
+      <c r="U53" s="40"/>
+      <c r="V53" s="40"/>
+      <c r="W53" s="40"/>
+      <c r="X53" s="40"/>
+      <c r="Y53" s="40"/>
+      <c r="Z53" s="40"/>
+      <c r="AA53" s="40"/>
+      <c r="AB53" s="40"/>
     </row>
     <row r="54" s="51" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="47" t="s">
-        <v>31</v>
-      </c>
-      <c r="B54" s="52" t="s">
+        <v>18</v>
+      </c>
+      <c r="B54" s="47" t="s">
         <v>116</v>
       </c>
-      <c r="C54" s="52" t="s">
+      <c r="C54" s="48" t="s">
         <v>117</v>
       </c>
-      <c r="D54" s="47"/>
-      <c r="E54" s="50"/>
+      <c r="D54" s="48"/>
+      <c r="E54" s="49"/>
       <c r="F54" s="50"/>
       <c r="G54" s="47"/>
       <c r="H54" s="47"/>
       <c r="I54" s="47" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="J54" s="47"/>
       <c r="K54" s="47"/>
@@ -2732,54 +2713,52 @@
       <c r="AB54" s="47"/>
     </row>
     <row r="55" s="51" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A55" s="53" t="s">
+      <c r="A55" s="47" t="s">
+        <v>33</v>
+      </c>
+      <c r="B55" s="52" t="s">
         <v>118</v>
       </c>
-      <c r="B55" s="53" t="s">
-        <v>118</v>
-      </c>
-      <c r="C55" s="54" t="s">
+      <c r="C55" s="52" t="s">
         <v>119</v>
       </c>
-      <c r="D55" s="53"/>
-      <c r="E55" s="55"/>
-      <c r="F55" s="55"/>
-      <c r="G55" s="56"/>
-      <c r="H55" s="56"/>
+      <c r="D55" s="47"/>
+      <c r="E55" s="50"/>
+      <c r="F55" s="50"/>
+      <c r="G55" s="47"/>
+      <c r="H55" s="47"/>
       <c r="I55" s="47" t="s">
-        <v>25</v>
-      </c>
-      <c r="J55" s="57" t="s">
-        <v>120</v>
-      </c>
-      <c r="K55" s="58"/>
-      <c r="L55" s="58"/>
-      <c r="M55" s="58"/>
-      <c r="N55" s="58"/>
-      <c r="O55" s="58"/>
-      <c r="P55" s="58"/>
-      <c r="Q55" s="58"/>
-      <c r="R55" s="58"/>
-      <c r="S55" s="58"/>
-      <c r="T55" s="58"/>
-      <c r="U55" s="58"/>
-      <c r="V55" s="58"/>
-      <c r="W55" s="58"/>
-      <c r="X55" s="58"/>
-      <c r="Y55" s="58"/>
-      <c r="Z55" s="58"/>
-      <c r="AA55" s="58"/>
-      <c r="AB55" s="58"/>
+        <v>27</v>
+      </c>
+      <c r="J55" s="47"/>
+      <c r="K55" s="47"/>
+      <c r="L55" s="47"/>
+      <c r="M55" s="47"/>
+      <c r="N55" s="47"/>
+      <c r="O55" s="47"/>
+      <c r="P55" s="47"/>
+      <c r="Q55" s="47"/>
+      <c r="R55" s="47"/>
+      <c r="S55" s="47"/>
+      <c r="T55" s="47"/>
+      <c r="U55" s="47"/>
+      <c r="V55" s="47"/>
+      <c r="W55" s="47"/>
+      <c r="X55" s="47"/>
+      <c r="Y55" s="47"/>
+      <c r="Z55" s="47"/>
+      <c r="AA55" s="47"/>
+      <c r="AB55" s="47"/>
     </row>
     <row r="56" s="51" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="53" t="s">
+        <v>120</v>
+      </c>
+      <c r="B56" s="53" t="s">
+        <v>120</v>
+      </c>
+      <c r="C56" s="54" t="s">
         <v>121</v>
-      </c>
-      <c r="B56" s="53" t="s">
-        <v>121</v>
-      </c>
-      <c r="C56" s="54" t="s">
-        <v>122</v>
       </c>
       <c r="D56" s="53"/>
       <c r="E56" s="55"/>
@@ -2787,10 +2766,10 @@
       <c r="G56" s="56"/>
       <c r="H56" s="56"/>
       <c r="I56" s="47" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="J56" s="57" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K56" s="58"/>
       <c r="L56" s="58"/>
@@ -2812,40 +2791,80 @@
       <c r="AB56" s="58"/>
     </row>
     <row r="57" s="51" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A57" s="47" t="s">
-        <v>34</v>
-      </c>
-      <c r="B57" s="47"/>
-      <c r="C57" s="47"/>
-      <c r="D57" s="47"/>
-      <c r="E57" s="50"/>
-      <c r="F57" s="50"/>
-      <c r="G57" s="47"/>
-      <c r="H57" s="47"/>
-      <c r="I57" s="47"/>
-      <c r="J57" s="47"/>
-      <c r="K57" s="47"/>
-      <c r="L57" s="47"/>
-      <c r="M57" s="47"/>
-      <c r="N57" s="47"/>
-      <c r="O57" s="47"/>
-      <c r="P57" s="47"/>
-      <c r="Q57" s="47"/>
-      <c r="R57" s="47"/>
-      <c r="S57" s="47"/>
-      <c r="T57" s="47"/>
-      <c r="U57" s="47"/>
-      <c r="V57" s="47"/>
-      <c r="W57" s="47"/>
-      <c r="X57" s="47"/>
-      <c r="Y57" s="47"/>
-      <c r="Z57" s="47"/>
-      <c r="AA57" s="47"/>
-      <c r="AB57" s="47"/>
-    </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="0" t="s">
-        <v>34</v>
+      <c r="A57" s="53" t="s">
+        <v>123</v>
+      </c>
+      <c r="B57" s="53" t="s">
+        <v>123</v>
+      </c>
+      <c r="C57" s="54" t="s">
+        <v>124</v>
+      </c>
+      <c r="D57" s="53"/>
+      <c r="E57" s="55"/>
+      <c r="F57" s="55"/>
+      <c r="G57" s="56"/>
+      <c r="H57" s="56"/>
+      <c r="I57" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="J57" s="57" t="s">
+        <v>125</v>
+      </c>
+      <c r="K57" s="58"/>
+      <c r="L57" s="58"/>
+      <c r="M57" s="58"/>
+      <c r="N57" s="58"/>
+      <c r="O57" s="58"/>
+      <c r="P57" s="58"/>
+      <c r="Q57" s="58"/>
+      <c r="R57" s="58"/>
+      <c r="S57" s="58"/>
+      <c r="T57" s="58"/>
+      <c r="U57" s="58"/>
+      <c r="V57" s="58"/>
+      <c r="W57" s="58"/>
+      <c r="X57" s="58"/>
+      <c r="Y57" s="58"/>
+      <c r="Z57" s="58"/>
+      <c r="AA57" s="58"/>
+      <c r="AB57" s="58"/>
+    </row>
+    <row r="58" s="51" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A58" s="47" t="s">
+        <v>36</v>
+      </c>
+      <c r="B58" s="47"/>
+      <c r="C58" s="47"/>
+      <c r="D58" s="47"/>
+      <c r="E58" s="50"/>
+      <c r="F58" s="50"/>
+      <c r="G58" s="47"/>
+      <c r="H58" s="47"/>
+      <c r="I58" s="47"/>
+      <c r="J58" s="47"/>
+      <c r="K58" s="47"/>
+      <c r="L58" s="47"/>
+      <c r="M58" s="47"/>
+      <c r="N58" s="47"/>
+      <c r="O58" s="47"/>
+      <c r="P58" s="47"/>
+      <c r="Q58" s="47"/>
+      <c r="R58" s="47"/>
+      <c r="S58" s="47"/>
+      <c r="T58" s="47"/>
+      <c r="U58" s="47"/>
+      <c r="V58" s="47"/>
+      <c r="W58" s="47"/>
+      <c r="X58" s="47"/>
+      <c r="Y58" s="47"/>
+      <c r="Z58" s="47"/>
+      <c r="AA58" s="47"/>
+      <c r="AB58" s="47"/>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="0" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -2867,10 +2886,10 @@
   <dimension ref="A1:Z123"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A15" activeCellId="3" sqref="G34 G40 G47 A15"/>
+      <selection pane="topLeft" activeCell="A92" activeCellId="0" sqref="A92"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.72"/>
@@ -2878,7 +2897,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -2912,154 +2931,157 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D2" s="60"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="D3" s="60"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="D4" s="60"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="9" t="s">
+        <v>25</v>
+      </c>
       <c r="B5" s="9" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="D5" s="60"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="D7" s="60"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="9" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D8" s="60"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="9" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="D9" s="60"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="9" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="D10" s="60"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="9" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D11" s="60"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="9" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="D12" s="60"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="9" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D13" s="60"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="9" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="D14" s="60"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="9" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D15" s="60"/>
     </row>
@@ -3071,25 +3093,25 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="9" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="D17" s="60"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="9" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="D18" s="60"/>
     </row>
@@ -3101,145 +3123,145 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="9" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D20" s="60"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="9" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="D21" s="60"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="9" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="D22" s="60"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="9" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="D23" s="60"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="9" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="D24" s="60"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="9" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="D25" s="60"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="9" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="D26" s="60"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="9" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="D27" s="60"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="9" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="D28" s="60"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="9" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="D29" s="60"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="9" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="D30" s="60"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="9" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="D31" s="60"/>
     </row>
@@ -3251,73 +3273,73 @@
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="9" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="D33" s="60"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="9" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="D34" s="60"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="9" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="D35" s="60"/>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="9" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="D36" s="60"/>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="9" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="D37" s="60"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="9" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="D38" s="60"/>
     </row>
@@ -3329,25 +3351,25 @@
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="9" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D40" s="60"/>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="9" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D41" s="60"/>
     </row>
@@ -3359,37 +3381,37 @@
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="9" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D43" s="60"/>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="9" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D44" s="60"/>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="9" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="D45" s="60"/>
     </row>
@@ -3401,565 +3423,565 @@
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="9" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="D47" s="60"/>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="9" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="D48" s="60"/>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="9" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="D49" s="60"/>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="9" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="D50" s="60"/>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="9" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="D51" s="60"/>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="C74" s="0" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="C78" s="0" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="C79" s="0" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="C80" s="0" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C81" s="0" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>236</v>
+        <v>97</v>
       </c>
       <c r="C83" s="0" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C84" s="0" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C85" s="0" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="C86" s="0" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C87" s="0" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="C88" s="0" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C89" s="0" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C90" s="0" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B91" s="0" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C91" s="0" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B92" s="0" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C92" s="0" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B93" s="0" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="C93" s="0" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B94" s="0" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C94" s="0" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B95" s="0" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="C95" s="0" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B96" s="0" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C96" s="0" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B97" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="C97" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B98" s="0" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C98" s="0" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B99" s="0" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="C99" s="0" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B100" s="0" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="C100" s="0" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B101" s="0" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="C101" s="0" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B102" s="0" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C102" s="0" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B103" s="0" t="s">
-        <v>276</v>
+        <v>53</v>
       </c>
       <c r="C103" s="0" t="s">
         <v>277</v>
@@ -3967,178 +3989,178 @@
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B104" s="0" t="s">
-        <v>51</v>
+        <v>278</v>
       </c>
       <c r="C104" s="0" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B105" s="0" t="s">
-        <v>95</v>
+        <v>280</v>
       </c>
       <c r="C105" s="0" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B107" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C107" s="0" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B108" s="0" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="C108" s="0" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B109" s="0" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="C109" s="0" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B110" s="0" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="C110" s="0" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B111" s="0" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="C111" s="0" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B112" s="0" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="C112" s="0" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="61" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="B114" s="0" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="C114" s="0" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="61" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="B115" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C115" s="0" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="61" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="B116" s="0" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="C116" s="0" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="61" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="B117" s="0" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C117" s="0" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="61" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="B118" s="0" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C118" s="0" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="61" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="B119" s="0" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="C119" s="0" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B122" s="0" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="C122" s="0" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B123" s="0" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="C123" s="0" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
   </sheetData>
@@ -4160,29 +4182,28 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="3" sqref="G34 G40 G47 B2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.36"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="62" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="B1" s="62" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="63" t="n">
-        <f aca="true">NOW()</f>
-        <v>44481.6482542914</v>
+      <c r="A2" s="63" t="s">
+        <v>307</v>
       </c>
       <c r="B2" s="64" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
     </row>
   </sheetData>

</xml_diff>